<commit_message>
add more lstm model performances
</commit_message>
<xml_diff>
--- a/ModelPerformances.xlsx
+++ b/ModelPerformances.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8340" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="6460" windowWidth="23220" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Per epoch" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
   <si>
     <t>CNN</t>
   </si>
@@ -99,6 +99,9 @@
   <si>
     <t>No.</t>
   </si>
+  <si>
+    <t>paper</t>
+  </si>
 </sst>
 </file>
 
@@ -107,7 +110,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -155,15 +158,15 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -220,7 +223,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -405,11 +407,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1396913168"/>
-        <c:axId val="-1420531456"/>
+        <c:axId val="-314223520"/>
+        <c:axId val="-314221472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1396913168"/>
+        <c:axId val="-314223520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -451,7 +453,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1420531456"/>
+        <c:crossAx val="-314221472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -459,7 +461,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1420531456"/>
+        <c:axId val="-314221472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -509,7 +511,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1396913168"/>
+        <c:crossAx val="-314223520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -523,7 +525,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1446,10 +1447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R20"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1457,8 +1458,8 @@
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="3"/>
-    <col min="9" max="16" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="16" width="10.83203125" style="1"/>
     <col min="17" max="17" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
@@ -1469,24 +1470,24 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1510,37 +1511,37 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="R4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1563,58 +1564,58 @@
       <c r="G5">
         <v>30</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>0.52200000000000002</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>0.65200000000000002</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>0.50800000000000001</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>0.42499999999999999</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>0.53600000000000003</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>0.66300000000000003</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>0.52200000000000002</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>0.41399999999999998</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <f t="shared" ref="Q5" si="0">HARMEAN(I5:L5)</f>
         <v>0.51474114023626782</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="3">
         <f t="shared" ref="R5" si="1">HARMEAN(M5:P5)</f>
         <v>0.51913431641040286</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -1635,37 +1636,37 @@
       <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="M11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="2" t="s">
+      <c r="N11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="P11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="R11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1682,38 +1683,38 @@
       <c r="G12">
         <v>9</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>0.54700000000000004</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>0.66600000000000004</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="1">
         <v>0.44800000000000001</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <v>0.71799999999999997</v>
       </c>
-      <c r="O12" s="2">
+      <c r="O12" s="1">
         <v>0.58099999999999996</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="1">
         <v>0.433</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="4">
         <f t="shared" ref="Q12:Q13" si="2">HARMEAN(I12:L12)</f>
         <v>0.5341466465864888</v>
       </c>
-      <c r="R12" s="5">
+      <c r="R12" s="4">
         <f t="shared" ref="R12:R13" si="3">HARMEAN(M12:P12)</f>
         <v>0.55869760966365589</v>
       </c>
@@ -1734,38 +1735,38 @@
       <c r="G13">
         <v>10</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>1.06E-3</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>0.66</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>0.503</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="1">
         <v>0.443</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="1">
         <v>0.71499999999999997</v>
       </c>
-      <c r="O13" s="2">
+      <c r="O13" s="1">
         <v>0.57499999999999996</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="1">
         <v>0.434</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <f t="shared" si="2"/>
         <v>0.52616485943031976</v>
       </c>
-      <c r="R13" s="4">
+      <c r="R13" s="3">
         <f t="shared" si="3"/>
         <v>0.55584387920748157</v>
       </c>
@@ -1783,35 +1784,35 @@
       <c r="G14">
         <v>30</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <v>0.65500000000000003</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>0.497</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="1">
         <v>0.45</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O14" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="1">
         <v>0.434</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <f>HARMEAN(I14:L14)</f>
         <v>0.52660163719849273</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R14" s="3">
         <f>HARMEAN(M14:P14)</f>
         <v>0.56445727117426536</v>
       </c>
@@ -1829,38 +1830,38 @@
       <c r="G16">
         <v>7</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>2.63E-3</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>0.67200000000000004</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="1">
         <v>0.53400000000000003</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="1">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="1">
         <v>0.73</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="1">
         <v>0.43</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="Q16" s="4">
         <f t="shared" ref="Q16:Q17" si="4">HARMEAN(I16:L16)</f>
         <v>0.53888105693368749</v>
       </c>
-      <c r="R16" s="5">
+      <c r="R16" s="4">
         <f t="shared" ref="R16:R17" si="5">HARMEAN(M16:P16)</f>
         <v>0.56380716978729306</v>
       </c>
@@ -1881,95 +1882,95 @@
       <c r="G17">
         <v>10</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>1.56E-3</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>0.66500000000000004</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="1">
         <v>0.44800000000000001</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M17" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N17" s="2">
+      <c r="N17" s="1">
         <v>0.72799999999999998</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O17" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="1">
         <v>0.432</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q17" s="5">
         <f t="shared" si="4"/>
         <v>0.53302736458221989</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17" s="5">
         <f t="shared" si="5"/>
         <v>0.56341248542736644</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="D19">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="D18">
         <v>240</v>
       </c>
-      <c r="E19">
+      <c r="E18">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="F19">
-        <v>1E-3</v>
-      </c>
-      <c r="G19">
-        <v>9</v>
-      </c>
-      <c r="H19" s="3">
-        <v>3.5E-4</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.53700000000000003</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.66500000000000004</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.52900000000000003</v>
-      </c>
-      <c r="L19" s="2">
-        <v>0.433</v>
-      </c>
-      <c r="M19" s="2">
-        <v>0.57299999999999995</v>
-      </c>
-      <c r="N19" s="2">
-        <v>0.70199999999999996</v>
-      </c>
-      <c r="O19" s="2">
-        <v>0.54300000000000004</v>
-      </c>
-      <c r="P19" s="2">
-        <v>0.438</v>
-      </c>
-      <c r="Q19" s="5">
-        <f t="shared" ref="Q19:Q20" si="6">HARMEAN(I19:L19)</f>
-        <v>0.52869598003963159</v>
-      </c>
-      <c r="R19" s="5">
-        <f t="shared" ref="R19:R20" si="7">HARMEAN(M19:P19)</f>
-        <v>0.54836378195331514</v>
+      <c r="F18">
+        <v>0.01</v>
+      </c>
+      <c r="G18">
+        <v>50</v>
+      </c>
+      <c r="H18" s="2">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.497</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0.443</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0.441</v>
+      </c>
+      <c r="Q18" s="5">
+        <f t="shared" ref="Q18" si="6">HARMEAN(I18:L18)</f>
+        <v>0.52127713009104992</v>
+      </c>
+      <c r="R18" s="5">
+        <f t="shared" ref="R18" si="7">HARMEAN(M18:P18)</f>
+        <v>0.56879315414671461</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20">
-        <v>3</v>
-      </c>
       <c r="D20">
         <v>240</v>
       </c>
@@ -1980,42 +1981,131 @@
         <v>1E-3</v>
       </c>
       <c r="G20">
+        <v>9</v>
+      </c>
+      <c r="H20" s="2">
+        <v>3.5E-4</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.433</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="P20" s="1">
+        <v>0.438</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" ref="Q20:Q21" si="8">HARMEAN(I20:L20)</f>
+        <v>0.52869598003963159</v>
+      </c>
+      <c r="R20" s="4">
+        <f t="shared" ref="R20:R21" si="9">HARMEAN(M20:P20)</f>
+        <v>0.54836378195331514</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>240</v>
+      </c>
+      <c r="E21">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F21">
+        <v>1E-3</v>
+      </c>
+      <c r="G21">
         <v>10</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H21" s="2">
         <v>3.2000000000000003E-4</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I21" s="1">
         <v>0.53200000000000003</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J21" s="1">
         <v>0.65700000000000003</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K21" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L21" s="1">
         <v>0.434</v>
       </c>
-      <c r="M20" s="2">
+      <c r="M21" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="N20" s="2">
+      <c r="N21" s="1">
         <v>0.71499999999999997</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O21" s="1">
         <v>0.54800000000000004</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P21" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="Q20" s="4">
-        <f t="shared" si="6"/>
+      <c r="Q21" s="3">
+        <f t="shared" si="8"/>
         <v>0.52406101678472494</v>
       </c>
-      <c r="R20" s="4">
-        <f t="shared" si="7"/>
+      <c r="R21" s="3">
+        <f t="shared" si="9"/>
         <v>0.55440506132671519</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.58399999999999996</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.72299999999999998</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="L23" s="1">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0.432</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" ref="Q23" si="10">HARMEAN(I23:L23)</f>
+        <v>0.57826082952638469</v>
+      </c>
+      <c r="R23" s="4">
+        <f t="shared" ref="R23" si="11">HARMEAN(M23:P23)</f>
+        <v>0.54839395595501261</v>
       </c>
     </row>
   </sheetData>
@@ -2042,8 +2132,8 @@
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="3"/>
-    <col min="9" max="16" width="10.83203125" style="2"/>
+    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="9" max="16" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -2052,24 +2142,24 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2093,31 +2183,31 @@
       <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2142,24 +2232,24 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2180,37 +2270,37 @@
       <c r="G24" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="2" t="s">
+      <c r="J24" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="2" t="s">
+      <c r="M24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O24" s="2" t="s">
+      <c r="O24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P24" s="2" t="s">
+      <c r="P24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="Q24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="R24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2227,38 +2317,38 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="2">
         <v>7.9900000000000006E-3</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="1">
         <v>0.53</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="1">
         <v>0.64800000000000002</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="1">
         <v>0.49199999999999999</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="1">
         <v>0.434</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="1">
         <v>0.54700000000000004</v>
       </c>
-      <c r="N25" s="2">
+      <c r="N25" s="1">
         <v>0.69399999999999995</v>
       </c>
-      <c r="O25" s="2">
+      <c r="O25" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="P25" s="2">
+      <c r="P25" s="1">
         <v>0.41799999999999998</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <f t="shared" ref="Q25:Q34" si="0">HARMEAN(I25:L25)</f>
         <v>0.51502123022994617</v>
       </c>
-      <c r="R25" s="4">
+      <c r="R25" s="3">
         <f t="shared" ref="R25:R34" si="1">HARMEAN(M25:P25)</f>
         <v>0.53572808040143882</v>
       </c>
@@ -2276,38 +2366,38 @@
       <c r="G26">
         <v>2</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>5.5300000000000002E-3</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="1">
         <v>0.67</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="1">
         <v>0.52900000000000003</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="1">
         <v>0.42499999999999999</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="1">
         <v>0.55700000000000005</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N26" s="1">
         <v>0.7</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O26" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P26" s="1">
         <v>0.43</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <f t="shared" si="0"/>
         <v>0.52669183929534913</v>
       </c>
-      <c r="R26" s="4">
+      <c r="R26" s="3">
         <f t="shared" si="1"/>
         <v>0.54119102388377971</v>
       </c>
@@ -2325,38 +2415,38 @@
       <c r="G27">
         <v>3</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="2">
         <v>4.4600000000000004E-3</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="1">
         <v>0.65800000000000003</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="1">
         <v>0.50800000000000001</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="1">
         <v>0.437</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="1">
         <v>0.56499999999999995</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="1">
         <v>0.71099999999999997</v>
       </c>
-      <c r="O27" s="2">
+      <c r="O27" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P27" s="2">
+      <c r="P27" s="1">
         <v>0.42799999999999999</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <f t="shared" si="0"/>
         <v>0.52505766002134979</v>
       </c>
-      <c r="R27" s="4">
+      <c r="R27" s="3">
         <f t="shared" si="1"/>
         <v>0.55041711908235125</v>
       </c>
@@ -2374,38 +2464,38 @@
       <c r="G28">
         <v>4</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H28" s="2">
         <v>3.5699999999999998E-3</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="1">
         <v>0.54100000000000004</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="1">
         <v>0.65200000000000002</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="1">
         <v>0.503</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="1">
         <v>0.438</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N28" s="2">
+      <c r="N28" s="1">
         <v>0.71399999999999997</v>
       </c>
-      <c r="O28" s="2">
+      <c r="O28" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P28" s="2">
+      <c r="P28" s="1">
         <v>0.439</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <f t="shared" si="0"/>
         <v>0.52264709841212131</v>
       </c>
-      <c r="R28" s="4">
+      <c r="R28" s="3">
         <f t="shared" si="1"/>
         <v>0.55796086065014805</v>
       </c>
@@ -2423,38 +2513,38 @@
       <c r="G29">
         <v>5</v>
       </c>
-      <c r="H29" s="3">
+      <c r="H29" s="2">
         <v>2.96E-3</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="1">
         <v>0.65600000000000003</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="1">
         <v>0.50800000000000001</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="1">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="1">
         <v>0.55800000000000005</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N29" s="1">
         <v>0.69599999999999995</v>
       </c>
-      <c r="O29" s="2">
+      <c r="O29" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P29" s="1">
         <v>0.437</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <f t="shared" si="0"/>
         <v>0.52898253665827866</v>
       </c>
-      <c r="R29" s="4">
+      <c r="R29" s="3">
         <f t="shared" si="1"/>
         <v>0.54356345482995394</v>
       </c>
@@ -2472,38 +2562,38 @@
       <c r="G30">
         <v>6</v>
       </c>
-      <c r="H30" s="3">
+      <c r="H30" s="2">
         <v>2.5500000000000002E-3</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="1">
         <v>0.55700000000000005</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="1">
         <v>0.66800000000000004</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="1">
         <v>0.503</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="1">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N30" s="2">
+      <c r="N30" s="1">
         <v>0.72</v>
       </c>
-      <c r="O30" s="2">
+      <c r="O30" s="1">
         <v>0.59099999999999997</v>
       </c>
-      <c r="P30" s="2">
+      <c r="P30" s="1">
         <v>0.44</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="Q30" s="4">
         <f t="shared" si="0"/>
         <v>0.53279477107657458</v>
       </c>
-      <c r="R30" s="5">
+      <c r="R30" s="4">
         <f t="shared" si="1"/>
         <v>0.56419282663231396</v>
       </c>
@@ -2521,38 +2611,38 @@
       <c r="G31">
         <v>7</v>
       </c>
-      <c r="H31" s="3">
+      <c r="H31" s="2">
         <v>2.16E-3</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="1">
         <v>0.54200000000000004</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="1">
         <v>0.65300000000000002</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="1">
         <v>0.48099999999999998</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="1">
         <v>0.45100000000000001</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="N31" s="2">
+      <c r="N31" s="1">
         <v>0.72199999999999998</v>
       </c>
-      <c r="O31" s="2">
+      <c r="O31" s="1">
         <v>0.59099999999999997</v>
       </c>
-      <c r="P31" s="2">
+      <c r="P31" s="1">
         <v>0.45300000000000001</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q31" s="3">
         <f t="shared" si="0"/>
         <v>0.52132825593600363</v>
       </c>
-      <c r="R31" s="4">
+      <c r="R31" s="3">
         <f t="shared" si="1"/>
         <v>0.57071661237113447</v>
       </c>
@@ -2570,38 +2660,38 @@
       <c r="G32">
         <v>8</v>
       </c>
-      <c r="H32" s="3">
+      <c r="H32" s="2">
         <v>1.6800000000000001E-3</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="1">
         <v>0.54100000000000004</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="1">
         <v>0.64900000000000002</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="1">
         <v>0.48699999999999999</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="1">
         <v>0.56799999999999995</v>
       </c>
-      <c r="N32" s="2">
+      <c r="N32" s="1">
         <v>0.70899999999999996</v>
       </c>
-      <c r="O32" s="2">
+      <c r="O32" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P32" s="2">
+      <c r="P32" s="1">
         <v>0.43</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="Q32" s="3">
         <f t="shared" si="0"/>
         <v>0.52084788448923691</v>
       </c>
-      <c r="R32" s="4">
+      <c r="R32" s="3">
         <f t="shared" si="1"/>
         <v>0.55165048489970792</v>
       </c>
@@ -2619,38 +2709,38 @@
       <c r="G33">
         <v>9</v>
       </c>
-      <c r="H33" s="3">
+      <c r="H33" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="1">
         <v>0.54700000000000004</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="1">
         <v>0.66600000000000004</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="1">
         <v>0.44800000000000001</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N33" s="2">
+      <c r="N33" s="1">
         <v>0.71799999999999997</v>
       </c>
-      <c r="O33" s="2">
+      <c r="O33" s="1">
         <v>0.58099999999999996</v>
       </c>
-      <c r="P33" s="2">
+      <c r="P33" s="1">
         <v>0.433</v>
       </c>
-      <c r="Q33" s="5">
+      <c r="Q33" s="4">
         <f t="shared" si="0"/>
         <v>0.5341466465864888</v>
       </c>
-      <c r="R33" s="5">
+      <c r="R33" s="4">
         <f t="shared" si="1"/>
         <v>0.55869760966365589</v>
       </c>
@@ -2671,38 +2761,38 @@
       <c r="G34">
         <v>10</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H34" s="2">
         <v>1.06E-3</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="1">
         <v>0.66</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="1">
         <v>0.503</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="1">
         <v>0.443</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N34" s="1">
         <v>0.71499999999999997</v>
       </c>
-      <c r="O34" s="2">
+      <c r="O34" s="1">
         <v>0.57499999999999996</v>
       </c>
-      <c r="P34" s="2">
+      <c r="P34" s="1">
         <v>0.434</v>
       </c>
-      <c r="Q34" s="4">
+      <c r="Q34" s="3">
         <f t="shared" si="0"/>
         <v>0.52616485943031976</v>
       </c>
-      <c r="R34" s="4">
+      <c r="R34" s="3">
         <f t="shared" si="1"/>
         <v>0.55584387920748157</v>
       </c>
@@ -2720,35 +2810,35 @@
       <c r="G35">
         <v>30</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="1">
         <v>0.65500000000000003</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="1">
         <v>0.497</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="1">
         <v>0.45</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M35" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="N35" s="2">
+      <c r="N35" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="O35" s="2">
+      <c r="O35" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="P35" s="2">
+      <c r="P35" s="1">
         <v>0.434</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="Q35" s="3">
         <f>HARMEAN(I35:L35)</f>
         <v>0.52660163719849273</v>
       </c>
-      <c r="R35" s="4">
+      <c r="R35" s="3">
         <f>HARMEAN(M35:P35)</f>
         <v>0.56445727117426536</v>
       </c>
@@ -2766,38 +2856,38 @@
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H37" s="2">
         <v>8.8699999999999994E-3</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="1">
         <v>0.53600000000000003</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="1">
         <v>0.66600000000000004</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="1">
         <v>0.52400000000000002</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="1">
         <v>0.435</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="N37" s="2">
+      <c r="N37" s="1">
         <v>0.68799999999999994</v>
       </c>
-      <c r="O37" s="2">
+      <c r="O37" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="P37" s="2">
+      <c r="P37" s="1">
         <v>0.40799999999999997</v>
       </c>
-      <c r="Q37" s="4">
+      <c r="Q37" s="3">
         <f t="shared" ref="Q37:Q46" si="2">HARMEAN(I37:L37)</f>
         <v>0.5280931938082476</v>
       </c>
-      <c r="R37" s="4">
+      <c r="R37" s="3">
         <f t="shared" ref="R37:R46" si="3">HARMEAN(M37:P37)</f>
         <v>0.52852314026594327</v>
       </c>
@@ -2815,38 +2905,38 @@
       <c r="G38">
         <v>2</v>
       </c>
-      <c r="H38" s="3">
+      <c r="H38" s="2">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="1">
         <v>0.53600000000000003</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="1">
         <v>0.66900000000000004</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="1">
         <v>0.52400000000000002</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="1">
         <v>0.433</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="N38" s="2">
+      <c r="N38" s="1">
         <v>0.69699999999999995</v>
       </c>
-      <c r="O38" s="2">
+      <c r="O38" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="P38" s="2">
+      <c r="P38" s="1">
         <v>0.42399999999999999</v>
       </c>
-      <c r="Q38" s="4">
+      <c r="Q38" s="3">
         <f t="shared" si="2"/>
         <v>0.52782246415372303</v>
       </c>
-      <c r="R38" s="4">
+      <c r="R38" s="3">
         <f t="shared" si="3"/>
         <v>0.53934183397116575</v>
       </c>
@@ -2864,38 +2954,38 @@
       <c r="G39">
         <v>3</v>
       </c>
-      <c r="H39" s="3">
+      <c r="H39" s="2">
         <v>4.9899999999999996E-3</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="1">
         <v>0.53700000000000003</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="1">
         <v>0.66800000000000004</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="1">
         <v>0.52400000000000002</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="1">
         <v>0.442</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="1">
         <v>0.56499999999999995</v>
       </c>
-      <c r="N39" s="2">
+      <c r="N39" s="1">
         <v>0.71599999999999997</v>
       </c>
-      <c r="O39" s="2">
+      <c r="O39" s="1">
         <v>0.58099999999999996</v>
       </c>
-      <c r="P39" s="2">
+      <c r="P39" s="1">
         <v>0.42299999999999999</v>
       </c>
-      <c r="Q39" s="4">
+      <c r="Q39" s="3">
         <f t="shared" si="2"/>
         <v>0.53120541182435321</v>
       </c>
-      <c r="R39" s="4">
+      <c r="R39" s="3">
         <f t="shared" si="3"/>
         <v>0.55158748583351191</v>
       </c>
@@ -2913,38 +3003,38 @@
       <c r="G40">
         <v>4</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H40" s="2">
         <v>4.0899999999999999E-3</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="1">
         <v>0.54</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="1">
         <v>0.66900000000000004</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="1">
         <v>0.53400000000000003</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="1">
         <v>0.56699999999999995</v>
       </c>
-      <c r="N40" s="2">
+      <c r="N40" s="1">
         <v>0.71099999999999997</v>
       </c>
-      <c r="O40" s="2">
+      <c r="O40" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P40" s="2">
+      <c r="P40" s="1">
         <v>0.42699999999999999</v>
       </c>
-      <c r="Q40" s="6">
+      <c r="Q40" s="5">
         <f t="shared" si="2"/>
         <v>0.53645077005910691</v>
       </c>
-      <c r="R40" s="6">
+      <c r="R40" s="5">
         <f t="shared" si="3"/>
         <v>0.55047554316491354</v>
       </c>
@@ -2962,38 +3052,38 @@
       <c r="G41">
         <v>5</v>
       </c>
-      <c r="H41" s="3">
+      <c r="H41" s="2">
         <v>3.5000000000000001E-3</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="1">
         <v>0.65700000000000003</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="1">
         <v>0.50800000000000001</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="1">
         <v>0.437</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41" s="1">
         <v>0.56899999999999995</v>
       </c>
-      <c r="N41" s="2">
+      <c r="N41" s="1">
         <v>0.71599999999999997</v>
       </c>
-      <c r="O41" s="2">
+      <c r="O41" s="1">
         <v>0.57499999999999996</v>
       </c>
-      <c r="P41" s="2">
+      <c r="P41" s="1">
         <v>0.42799999999999999</v>
       </c>
-      <c r="Q41" s="6">
+      <c r="Q41" s="5">
         <f t="shared" si="2"/>
         <v>0.52489828109576153</v>
       </c>
-      <c r="R41" s="6">
+      <c r="R41" s="5">
         <f t="shared" si="3"/>
         <v>0.55327358465754639</v>
       </c>
@@ -3011,38 +3101,38 @@
       <c r="G42">
         <v>6</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="2">
         <v>3.0899999999999999E-3</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="1">
         <v>0.54200000000000004</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="1">
         <v>0.65700000000000003</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="1">
         <v>0.503</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="1">
         <v>0.57199999999999995</v>
       </c>
-      <c r="N42" s="2">
+      <c r="N42" s="1">
         <v>0.73299999999999998</v>
       </c>
-      <c r="O42" s="2">
+      <c r="O42" s="1">
         <v>0.60199999999999998</v>
       </c>
-      <c r="P42" s="2">
+      <c r="P42" s="1">
         <v>0.43099999999999999</v>
       </c>
-      <c r="Q42" s="6">
+      <c r="Q42" s="5">
         <f t="shared" si="2"/>
         <v>0.52684981405979958</v>
       </c>
-      <c r="R42" s="6">
+      <c r="R42" s="5">
         <f t="shared" si="3"/>
         <v>0.56387081662583782</v>
       </c>
@@ -3060,38 +3150,38 @@
       <c r="G43">
         <v>7</v>
       </c>
-      <c r="H43" s="3">
+      <c r="H43" s="2">
         <v>2.63E-3</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="1">
         <v>0.54500000000000004</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="1">
         <v>0.67200000000000004</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="1">
         <v>0.53400000000000003</v>
       </c>
-      <c r="L43" s="2">
+      <c r="L43" s="1">
         <v>0.44900000000000001</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M43" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="N43" s="2">
+      <c r="N43" s="1">
         <v>0.73</v>
       </c>
-      <c r="O43" s="2">
+      <c r="O43" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="P43" s="2">
+      <c r="P43" s="1">
         <v>0.43</v>
       </c>
-      <c r="Q43" s="5">
+      <c r="Q43" s="4">
         <f t="shared" si="2"/>
         <v>0.53888105693368749</v>
       </c>
-      <c r="R43" s="5">
+      <c r="R43" s="4">
         <f t="shared" si="3"/>
         <v>0.56380716978729306</v>
       </c>
@@ -3109,38 +3199,38 @@
       <c r="G44">
         <v>8</v>
       </c>
-      <c r="H44" s="3">
+      <c r="H44" s="2">
         <v>2.2699999999999999E-3</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="1">
         <v>0.53600000000000003</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="1">
         <v>0.65800000000000003</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="1">
         <v>0.50800000000000001</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L44" s="1">
         <v>0.443</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="1">
         <v>0.57799999999999996</v>
       </c>
-      <c r="N44" s="2">
+      <c r="N44" s="1">
         <v>0.73099999999999998</v>
       </c>
-      <c r="O44" s="2">
+      <c r="O44" s="1">
         <v>0.60199999999999998</v>
       </c>
-      <c r="P44" s="2">
+      <c r="P44" s="1">
         <v>0.438</v>
       </c>
-      <c r="Q44" s="6">
+      <c r="Q44" s="5">
         <f t="shared" si="2"/>
         <v>0.52553655976394087</v>
       </c>
-      <c r="R44" s="6">
+      <c r="R44" s="5">
         <f t="shared" si="3"/>
         <v>0.56799403699300466</v>
       </c>
@@ -3158,38 +3248,38 @@
       <c r="G45">
         <v>9</v>
       </c>
-      <c r="H45" s="3">
+      <c r="H45" s="2">
         <v>1.8699999999999999E-3</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="1">
         <v>0.66400000000000003</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45" s="1">
         <v>0.45</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="1">
         <v>0.58299999999999996</v>
       </c>
-      <c r="N45" s="2">
+      <c r="N45" s="1">
         <v>0.73499999999999999</v>
       </c>
-      <c r="O45" s="2">
+      <c r="O45" s="1">
         <v>0.60199999999999998</v>
       </c>
-      <c r="P45" s="2">
+      <c r="P45" s="1">
         <v>0.44</v>
       </c>
-      <c r="Q45" s="6">
+      <c r="Q45" s="5">
         <f t="shared" si="2"/>
         <v>0.53357171764188072</v>
       </c>
-      <c r="R45" s="6">
+      <c r="R45" s="5">
         <f t="shared" si="3"/>
         <v>0.57064052300232759</v>
       </c>
@@ -3210,45 +3300,45 @@
       <c r="G46">
         <v>10</v>
       </c>
-      <c r="H46" s="3">
+      <c r="H46" s="2">
         <v>1.56E-3</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="1">
         <v>0.66500000000000004</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L46" s="1">
         <v>0.44800000000000001</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N46" s="1">
         <v>0.72799999999999998</v>
       </c>
-      <c r="O46" s="2">
+      <c r="O46" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="P46" s="2">
+      <c r="P46" s="1">
         <v>0.432</v>
       </c>
-      <c r="Q46" s="6">
+      <c r="Q46" s="5">
         <f t="shared" si="2"/>
         <v>0.53302736458221989</v>
       </c>
-      <c r="R46" s="6">
+      <c r="R46" s="5">
         <f t="shared" si="3"/>
         <v>0.56341248542736644</v>
       </c>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="Q47" s="7"/>
-      <c r="R47" s="7"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.2">
       <c r="D48">
@@ -3263,38 +3353,38 @@
       <c r="G48">
         <v>1</v>
       </c>
-      <c r="H48" s="3">
+      <c r="H48" s="2">
         <v>7.9900000000000006E-3</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="1">
         <v>0.53</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48" s="1">
         <v>0.64800000000000002</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="1">
         <v>0.49199999999999999</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="1">
         <v>0.434</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48" s="1">
         <v>0.54700000000000004</v>
       </c>
-      <c r="N48" s="2">
+      <c r="N48" s="1">
         <v>0.69399999999999995</v>
       </c>
-      <c r="O48" s="2">
+      <c r="O48" s="1">
         <v>0.55400000000000005</v>
       </c>
-      <c r="P48" s="2">
+      <c r="P48" s="1">
         <v>0.41799999999999998</v>
       </c>
-      <c r="Q48" s="6">
+      <c r="Q48" s="5">
         <f t="shared" ref="Q48:Q57" si="4">HARMEAN(I48:L48)</f>
         <v>0.51502123022994617</v>
       </c>
-      <c r="R48" s="6">
+      <c r="R48" s="5">
         <f t="shared" ref="R48:R57" si="5">HARMEAN(M48:P48)</f>
         <v>0.53572808040143882</v>
       </c>
@@ -3312,38 +3402,38 @@
       <c r="G49">
         <v>2</v>
       </c>
-      <c r="H49" s="3">
+      <c r="H49" s="2">
         <v>5.5300000000000002E-3</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J49" s="1">
         <v>0.67</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="1">
         <v>0.52900000000000003</v>
       </c>
-      <c r="L49" s="2">
+      <c r="L49" s="1">
         <v>0.42499999999999999</v>
       </c>
-      <c r="M49" s="2">
+      <c r="M49" s="1">
         <v>0.55700000000000005</v>
       </c>
-      <c r="N49" s="2">
+      <c r="N49" s="1">
         <v>0.7</v>
       </c>
-      <c r="O49" s="2">
+      <c r="O49" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="P49" s="2">
+      <c r="P49" s="1">
         <v>0.43</v>
       </c>
-      <c r="Q49" s="6">
+      <c r="Q49" s="5">
         <f t="shared" si="4"/>
         <v>0.52669183929534913</v>
       </c>
-      <c r="R49" s="6">
+      <c r="R49" s="5">
         <f t="shared" si="5"/>
         <v>0.54119102388377971</v>
       </c>
@@ -3361,38 +3451,38 @@
       <c r="G50">
         <v>3</v>
       </c>
-      <c r="H50" s="3">
+      <c r="H50" s="2">
         <v>4.4600000000000004E-3</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="1">
         <v>0.65800000000000003</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="1">
         <v>0.50800000000000001</v>
       </c>
-      <c r="L50" s="2">
+      <c r="L50" s="1">
         <v>0.437</v>
       </c>
-      <c r="M50" s="2">
+      <c r="M50" s="1">
         <v>0.56499999999999995</v>
       </c>
-      <c r="N50" s="2">
+      <c r="N50" s="1">
         <v>0.71099999999999997</v>
       </c>
-      <c r="O50" s="2">
+      <c r="O50" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P50" s="2">
+      <c r="P50" s="1">
         <v>0.42799999999999999</v>
       </c>
-      <c r="Q50" s="6">
+      <c r="Q50" s="5">
         <f t="shared" si="4"/>
         <v>0.52505766002134979</v>
       </c>
-      <c r="R50" s="6">
+      <c r="R50" s="5">
         <f t="shared" si="5"/>
         <v>0.55041711908235125</v>
       </c>
@@ -3410,38 +3500,38 @@
       <c r="G51">
         <v>4</v>
       </c>
-      <c r="H51" s="3">
+      <c r="H51" s="2">
         <v>3.5699999999999998E-3</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="1">
         <v>0.54100000000000004</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J51" s="1">
         <v>0.65200000000000002</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="1">
         <v>0.503</v>
       </c>
-      <c r="L51" s="2">
+      <c r="L51" s="1">
         <v>0.438</v>
       </c>
-      <c r="M51" s="2">
+      <c r="M51" s="1">
         <v>0.57599999999999996</v>
       </c>
-      <c r="N51" s="2">
+      <c r="N51" s="1">
         <v>0.71399999999999997</v>
       </c>
-      <c r="O51" s="2">
+      <c r="O51" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="P51" s="2">
+      <c r="P51" s="1">
         <v>0.439</v>
       </c>
-      <c r="Q51" s="6">
+      <c r="Q51" s="5">
         <f t="shared" si="4"/>
         <v>0.52264709841212131</v>
       </c>
-      <c r="R51" s="6">
+      <c r="R51" s="5">
         <f t="shared" si="5"/>
         <v>0.55796086065014805</v>
       </c>
@@ -3459,38 +3549,38 @@
       <c r="G52">
         <v>5</v>
       </c>
-      <c r="H52" s="3">
+      <c r="H52" s="2">
         <v>5.4000000000000001E-4</v>
       </c>
-      <c r="I52" s="2">
+      <c r="I52" s="1">
         <v>0.53300000000000003</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J52" s="1">
         <v>0.66100000000000003</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L52" s="2">
+      <c r="L52" s="1">
         <v>0.437</v>
       </c>
-      <c r="M52" s="2">
+      <c r="M52" s="1">
         <v>0.55500000000000005</v>
       </c>
-      <c r="N52" s="2">
+      <c r="N52" s="1">
         <v>0.68500000000000005</v>
       </c>
-      <c r="O52" s="2">
+      <c r="O52" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="P52" s="2">
+      <c r="P52" s="1">
         <v>0.41899999999999998</v>
       </c>
-      <c r="Q52" s="6">
+      <c r="Q52" s="5">
         <f t="shared" si="4"/>
         <v>0.5260289856647643</v>
       </c>
-      <c r="R52" s="6">
+      <c r="R52" s="5">
         <f t="shared" si="5"/>
         <v>0.53283412312153111</v>
       </c>
@@ -3508,38 +3598,38 @@
       <c r="G53">
         <v>6</v>
       </c>
-      <c r="H53" s="3">
+      <c r="H53" s="2">
         <v>4.8999999999999998E-4</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="1">
         <v>0.53300000000000003</v>
       </c>
-      <c r="J53" s="2">
+      <c r="J53" s="1">
         <v>0.65500000000000003</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="1">
         <v>0.503</v>
       </c>
-      <c r="L53" s="2">
+      <c r="L53" s="1">
         <v>0.436</v>
       </c>
-      <c r="M53" s="2">
+      <c r="M53" s="1">
         <v>0.56499999999999995</v>
       </c>
-      <c r="N53" s="2">
+      <c r="N53" s="1">
         <v>0.70399999999999996</v>
       </c>
-      <c r="O53" s="2">
+      <c r="O53" s="1">
         <v>0.55900000000000005</v>
       </c>
-      <c r="P53" s="2">
+      <c r="P53" s="1">
         <v>0.42799999999999999</v>
       </c>
-      <c r="Q53" s="6">
+      <c r="Q53" s="5">
         <f t="shared" si="4"/>
         <v>0.52052564592304795</v>
       </c>
-      <c r="R53" s="6">
+      <c r="R53" s="5">
         <f t="shared" si="5"/>
         <v>0.54676752712239651</v>
       </c>
@@ -3557,38 +3647,38 @@
       <c r="G54">
         <v>7</v>
       </c>
-      <c r="H54" s="3">
+      <c r="H54" s="2">
         <v>4.4000000000000002E-4</v>
       </c>
-      <c r="I54" s="2">
+      <c r="I54" s="1">
         <v>0.53400000000000003</v>
       </c>
-      <c r="J54" s="2">
+      <c r="J54" s="1">
         <v>0.65100000000000002</v>
       </c>
-      <c r="K54" s="2">
+      <c r="K54" s="1">
         <v>0.497</v>
       </c>
-      <c r="L54" s="2">
+      <c r="L54" s="1">
         <v>0.42899999999999999</v>
       </c>
-      <c r="M54" s="2">
+      <c r="M54" s="1">
         <v>0.56799999999999995</v>
       </c>
-      <c r="N54" s="2">
+      <c r="N54" s="1">
         <v>0.69799999999999995</v>
       </c>
-      <c r="O54" s="2">
+      <c r="O54" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="P54" s="2">
+      <c r="P54" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="Q54" s="6">
+      <c r="Q54" s="5">
         <f t="shared" si="4"/>
         <v>0.51600703807840764</v>
       </c>
-      <c r="R54" s="6">
+      <c r="R54" s="5">
         <f t="shared" si="5"/>
         <v>0.55005612284334315</v>
       </c>
@@ -3606,38 +3696,38 @@
       <c r="G55">
         <v>8</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H55" s="2">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="I55" s="2">
+      <c r="I55" s="1">
         <v>0.53500000000000003</v>
       </c>
-      <c r="J55" s="2">
+      <c r="J55" s="1">
         <v>0.66700000000000004</v>
       </c>
-      <c r="K55" s="2">
+      <c r="K55" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L55" s="2">
+      <c r="L55" s="1">
         <v>0.43099999999999999</v>
       </c>
-      <c r="M55" s="2">
+      <c r="M55" s="1">
         <v>0.56599999999999995</v>
       </c>
-      <c r="N55" s="2">
+      <c r="N55" s="1">
         <v>0.7</v>
       </c>
-      <c r="O55" s="2">
+      <c r="O55" s="1">
         <v>0.53800000000000003</v>
       </c>
-      <c r="P55" s="2">
+      <c r="P55" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="Q55" s="6">
+      <c r="Q55" s="5">
         <f t="shared" si="4"/>
         <v>0.52525304072734935</v>
       </c>
-      <c r="R55" s="6">
+      <c r="R55" s="5">
         <f t="shared" si="5"/>
         <v>0.54860440209062888</v>
       </c>
@@ -3655,38 +3745,38 @@
       <c r="G56">
         <v>9</v>
       </c>
-      <c r="H56" s="3">
+      <c r="H56" s="2">
         <v>3.5E-4</v>
       </c>
-      <c r="I56" s="2">
+      <c r="I56" s="1">
         <v>0.53700000000000003</v>
       </c>
-      <c r="J56" s="2">
+      <c r="J56" s="1">
         <v>0.66500000000000004</v>
       </c>
-      <c r="K56" s="2">
+      <c r="K56" s="1">
         <v>0.52900000000000003</v>
       </c>
-      <c r="L56" s="2">
+      <c r="L56" s="1">
         <v>0.433</v>
       </c>
-      <c r="M56" s="2">
+      <c r="M56" s="1">
         <v>0.57299999999999995</v>
       </c>
-      <c r="N56" s="2">
+      <c r="N56" s="1">
         <v>0.70199999999999996</v>
       </c>
-      <c r="O56" s="2">
+      <c r="O56" s="1">
         <v>0.54300000000000004</v>
       </c>
-      <c r="P56" s="2">
+      <c r="P56" s="1">
         <v>0.438</v>
       </c>
-      <c r="Q56" s="5">
+      <c r="Q56" s="4">
         <f t="shared" si="4"/>
         <v>0.52869598003963159</v>
       </c>
-      <c r="R56" s="5">
+      <c r="R56" s="4">
         <f t="shared" si="5"/>
         <v>0.54836378195331514</v>
       </c>
@@ -3707,38 +3797,38 @@
       <c r="G57">
         <v>10</v>
       </c>
-      <c r="H57" s="3">
+      <c r="H57" s="2">
         <v>3.2000000000000003E-4</v>
       </c>
-      <c r="I57" s="2">
+      <c r="I57" s="1">
         <v>0.53200000000000003</v>
       </c>
-      <c r="J57" s="2">
+      <c r="J57" s="1">
         <v>0.65700000000000003</v>
       </c>
-      <c r="K57" s="2">
+      <c r="K57" s="1">
         <v>0.51900000000000002</v>
       </c>
-      <c r="L57" s="2">
+      <c r="L57" s="1">
         <v>0.434</v>
       </c>
-      <c r="M57" s="2">
+      <c r="M57" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="N57" s="2">
+      <c r="N57" s="1">
         <v>0.71499999999999997</v>
       </c>
-      <c r="O57" s="2">
+      <c r="O57" s="1">
         <v>0.54800000000000004</v>
       </c>
-      <c r="P57" s="2">
+      <c r="P57" s="1">
         <v>0.44700000000000001</v>
       </c>
-      <c r="Q57" s="4">
+      <c r="Q57" s="3">
         <f t="shared" si="4"/>
         <v>0.52406101678472494</v>
       </c>
-      <c r="R57" s="4">
+      <c r="R57" s="3">
         <f t="shared" si="5"/>
         <v>0.55440506132671519</v>
       </c>

</xml_diff>

<commit_message>
A few more trials added
</commit_message>
<xml_diff>
--- a/ModelPerformances.xlsx
+++ b/ModelPerformances.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nslonge/Documents/mit/year4/6806/final_proj_gh/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenhu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="72">
   <si>
     <t>CNN</t>
   </si>
@@ -154,18 +154,6 @@
     <t>test set</t>
   </si>
   <si>
-    <t>Harmean</t>
-  </si>
-  <si>
-    <t>precision</t>
-  </si>
-  <si>
-    <t>recall</t>
-  </si>
-  <si>
-    <t>accuracy</t>
-  </si>
-  <si>
     <t>epoch 1</t>
   </si>
   <si>
@@ -211,9 +199,6 @@
     <t>Accuracy</t>
   </si>
   <si>
-    <t>4 in 10</t>
-  </si>
-  <si>
     <t>max title</t>
   </si>
   <si>
@@ -237,6 +222,30 @@
   <si>
     <t>2,3</t>
   </si>
+  <si>
+    <t>layer</t>
+  </si>
+  <si>
+    <t>devAUC</t>
+  </si>
+  <si>
+    <t>testAUC</t>
+  </si>
+  <si>
+    <t>--model lstm --full-eval False --snapshot ./lstm6.pkl --max-title 38</t>
+  </si>
+  <si>
+    <t>TARGET DOMAIN performances</t>
+  </si>
+  <si>
+    <t>Direct Transfer on target</t>
+  </si>
+  <si>
+    <t>hidden layer</t>
+  </si>
+  <si>
+    <t>LSTM model#</t>
+  </si>
 </sst>
 </file>
 
@@ -247,21 +256,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -307,8 +302,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +329,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -339,35 +353,30 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -404,6 +413,28 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -439,7 +470,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -618,11 +648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2109041056"/>
-        <c:axId val="-2109038736"/>
+        <c:axId val="591704400"/>
+        <c:axId val="591706720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109041056"/>
+        <c:axId val="591704400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -664,7 +694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109038736"/>
+        <c:crossAx val="591706720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -672,7 +702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109038736"/>
+        <c:axId val="591706720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -722,7 +752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109041056"/>
+        <c:crossAx val="591704400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -736,7 +766,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -818,7 +847,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -997,11 +1025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2107826464"/>
-        <c:axId val="-2107823712"/>
+        <c:axId val="591731408"/>
+        <c:axId val="591733728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2107826464"/>
+        <c:axId val="591731408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1043,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107823712"/>
+        <c:crossAx val="591733728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1051,7 +1079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107823712"/>
+        <c:axId val="591733728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1101,7 +1129,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107826464"/>
+        <c:crossAx val="591731408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1115,7 +1143,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2622,10 +2649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V93"/>
+  <dimension ref="A1:AH96"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J85" sqref="J85"/>
+    <sheetView showRuler="0" topLeftCell="W57" workbookViewId="0">
+      <selection activeCell="AG73" sqref="AG73:AH73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2649,27 +2676,27 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="3"/>
-      <c r="I3" s="6"/>
+      <c r="I3" s="5"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -3659,11 +3686,11 @@
       <c r="S28" s="1">
         <v>0.41299999999999998</v>
       </c>
-      <c r="T28" s="10">
+      <c r="T28" s="8">
         <f>HARMEAN(L28:O28)</f>
         <v>0.54619824881451606</v>
       </c>
-      <c r="U28" s="10">
+      <c r="U28" s="8">
         <f>HARMEAN(P28:S28)</f>
         <v>0.51475724622296581</v>
       </c>
@@ -4171,11 +4198,11 @@
       <c r="S41" s="1">
         <v>0.39460000000000001</v>
       </c>
-      <c r="T41" s="11">
+      <c r="T41" s="9">
         <f>HARMEAN(L41:O41)</f>
         <v>0.55825877732488272</v>
       </c>
-      <c r="U41" s="11">
+      <c r="U41" s="9">
         <f>HARMEAN(P41:S41)</f>
         <v>0.49960077603223724</v>
       </c>
@@ -4421,11 +4448,11 @@
       <c r="S47" s="1">
         <v>0.42899999999999999</v>
       </c>
-      <c r="T47" s="11">
+      <c r="T47" s="9">
         <f>HARMEAN(L47:O47)</f>
         <v>0.55986164163140495</v>
       </c>
-      <c r="U47" s="11">
+      <c r="U47" s="9">
         <f>HARMEAN(P47:S47)</f>
         <v>0.52555639369579144</v>
       </c>
@@ -4795,45 +4822,65 @@
       <c r="S61" s="1">
         <v>0.432</v>
       </c>
-      <c r="T61" s="9">
+      <c r="T61" s="7">
         <f t="shared" ref="T61" si="0">HARMEAN(L61:O61)</f>
         <v>0.5727891378247163</v>
       </c>
-      <c r="U61" s="9">
+      <c r="U61" s="7">
         <f t="shared" ref="U61" si="1">HARMEAN(P61:S61)</f>
         <v>0.55651420838971588</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C65" s="20" t="s">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C65" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="6"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="20" t="s">
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
+      <c r="F65" s="22"/>
+      <c r="G65" s="22"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="L65" s="20"/>
-      <c r="M65" s="20"/>
-      <c r="N65" s="20"/>
-      <c r="O65" s="20"/>
-      <c r="P65" s="20"/>
-      <c r="Q65" s="20"/>
-      <c r="R65" s="20"/>
-      <c r="S65" s="20"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="L65" s="22"/>
+      <c r="M65" s="22"/>
+      <c r="N65" s="22"/>
+      <c r="O65" s="22"/>
+      <c r="P65" s="22"/>
+      <c r="Q65" s="22"/>
+      <c r="R65" s="22"/>
+      <c r="S65" s="22"/>
+      <c r="V65" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="W65" s="22"/>
+      <c r="X65" s="22"/>
+      <c r="Y65" s="22"/>
+      <c r="Z65" s="22"/>
+      <c r="AA65" s="22"/>
+      <c r="AB65" s="22"/>
+      <c r="AC65" s="22"/>
+      <c r="AD65" s="22"/>
+      <c r="AE65" s="1"/>
+      <c r="AF65" s="1"/>
+      <c r="AG65" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH65" s="22"/>
+    </row>
+    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1</v>
       </c>
       <c r="B66" t="s">
         <v>22</v>
       </c>
+      <c r="C66" t="s">
+        <v>64</v>
+      </c>
       <c r="D66" t="s">
         <v>15</v>
       </c>
@@ -4888,8 +4935,50 @@
       <c r="U66" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V66" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="W66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="X66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y66" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA66" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB66" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC66" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD66" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF66" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG66" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH66" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C67">
+        <v>1</v>
+      </c>
       <c r="D67">
         <v>240</v>
       </c>
@@ -4914,7 +5003,7 @@
       <c r="K67" s="2">
         <v>1.5E-3</v>
       </c>
-      <c r="L67" s="5">
+      <c r="L67" s="25">
         <v>0.54700000000000004</v>
       </c>
       <c r="M67" s="1">
@@ -4938,17 +5027,20 @@
       <c r="S67" s="1">
         <v>0.433</v>
       </c>
-      <c r="T67" s="9">
+      <c r="T67" s="7">
         <f>HARMEAN(L67:O67)</f>
         <v>0.5341466465864888</v>
       </c>
-      <c r="U67" s="9">
+      <c r="U67" s="7">
         <f t="shared" ref="U67:U68" si="2">HARMEAN(P67:S67)</f>
         <v>0.55869760966365589</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
         <v>1</v>
       </c>
       <c r="D68">
@@ -5008,7 +5100,10 @@
         <v>0.55584387920748157</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C69">
+        <v>1</v>
+      </c>
       <c r="D69">
         <v>240</v>
       </c>
@@ -5063,7 +5158,10 @@
         <v>0.56445727117426536</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C71">
+        <v>1</v>
+      </c>
       <c r="D71">
         <v>240</v>
       </c>
@@ -5109,21 +5207,21 @@
       <c r="R71" s="1">
         <v>0.59699999999999998</v>
       </c>
-      <c r="S71" s="7">
+      <c r="S71" s="25">
         <v>0.43</v>
       </c>
-      <c r="T71" s="11">
-        <f t="shared" ref="T71:T72" si="4">HARMEAN(L71:O71)</f>
+      <c r="T71" s="9">
+        <f t="shared" ref="T71:T73" si="4">HARMEAN(L71:O71)</f>
         <v>0.53888105693368749</v>
       </c>
-      <c r="U71" s="11">
-        <f t="shared" ref="U71:U72" si="5">HARMEAN(P71:S71)</f>
+      <c r="U71" s="9">
+        <f t="shared" ref="U71:U73" si="5">HARMEAN(P71:S71)</f>
         <v>0.56380716978729306</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B72">
-        <v>2</v>
+    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C72">
+        <v>1</v>
       </c>
       <c r="D72">
         <v>240</v>
@@ -5173,16 +5271,22 @@
       <c r="S72" s="1">
         <v>0.432</v>
       </c>
-      <c r="T72" s="10">
+      <c r="T72" s="8">
         <f t="shared" si="4"/>
         <v>0.53302736458221989</v>
       </c>
-      <c r="U72" s="10">
+      <c r="U72" s="8">
         <f t="shared" si="5"/>
         <v>0.56341248542736644</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>2</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
       <c r="D73">
         <v>240</v>
       </c>
@@ -5231,16 +5335,57 @@
       <c r="S73" s="1">
         <v>0.441</v>
       </c>
-      <c r="T73" s="10">
-        <f t="shared" ref="T73" si="6">HARMEAN(L73:O73)</f>
+      <c r="T73" s="8">
+        <f t="shared" si="4"/>
         <v>0.52127713009104992</v>
       </c>
-      <c r="U73" s="10">
-        <f t="shared" ref="U73" si="7">HARMEAN(P73:S73)</f>
+      <c r="U73" s="8">
+        <f t="shared" si="5"/>
         <v>0.56879315414671461</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="W73" s="1">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="X73" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="Y73" s="1">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="Z73" s="1">
+        <v>0.155</v>
+      </c>
+      <c r="AA73" s="1">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="AB73" s="1">
+        <v>0.622</v>
+      </c>
+      <c r="AC73" s="1">
+        <v>0.497</v>
+      </c>
+      <c r="AD73" s="1">
+        <v>0.157</v>
+      </c>
+      <c r="AE73" s="7">
+        <f t="shared" ref="AE73" si="6">HARMEAN(W73:Z73)</f>
+        <v>0.3354152106002744</v>
+      </c>
+      <c r="AF73" s="7">
+        <f t="shared" ref="AF73" si="7">HARMEAN(AA73:AD73)</f>
+        <v>0.3446871822423288</v>
+      </c>
+      <c r="AG73" s="26">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="AH73" s="26">
+        <v>0.29799999999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C75">
+        <v>1</v>
+      </c>
       <c r="D75">
         <v>240</v>
       </c>
@@ -5289,18 +5434,21 @@
       <c r="S75" s="1">
         <v>0.438</v>
       </c>
-      <c r="T75" s="9">
+      <c r="T75" s="7">
         <f t="shared" ref="T75:T76" si="8">HARMEAN(L75:O75)</f>
         <v>0.52869598003963159</v>
       </c>
-      <c r="U75" s="9">
+      <c r="U75" s="7">
         <f t="shared" ref="U75:U76" si="9">HARMEAN(P75:S75)</f>
         <v>0.54836378195331514</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B76">
         <v>3</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
       </c>
       <c r="D76">
         <v>240</v>
@@ -5359,7 +5507,10 @@
         <v>0.55440506132671519</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="C78">
+        <v>1</v>
+      </c>
       <c r="D78">
         <v>240</v>
       </c>
@@ -5381,30 +5532,30 @@
       <c r="J78" t="s">
         <v>27</v>
       </c>
-      <c r="K78" s="2">
-        <v>2.63E-3</v>
-      </c>
-      <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="12"/>
-      <c r="P78" s="12"/>
-      <c r="Q78" s="12"/>
-      <c r="R78" s="12"/>
-      <c r="S78" s="12"/>
-      <c r="T78" s="13" t="e">
-        <f t="shared" ref="T78" si="10">HARMEAN(L78:O78)</f>
+      <c r="L78" s="25"/>
+      <c r="M78" s="25"/>
+      <c r="N78" s="25"/>
+      <c r="O78" s="25"/>
+      <c r="P78" s="25"/>
+      <c r="Q78" s="25"/>
+      <c r="R78" s="25"/>
+      <c r="S78" s="25"/>
+      <c r="T78" s="27" t="e">
+        <f t="shared" ref="T78:T79" si="10">HARMEAN(L78:O78)</f>
         <v>#N/A</v>
       </c>
-      <c r="U78" s="13" t="e">
-        <f t="shared" ref="U78" si="11">HARMEAN(P78:S78)</f>
+      <c r="U78" s="27" t="e">
+        <f t="shared" ref="U78:U79" si="11">HARMEAN(P78:S78)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B79">
         <v>4</v>
       </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
       <c r="D79">
         <v>240</v>
       </c>
@@ -5426,51 +5577,51 @@
       <c r="J79" t="s">
         <v>27</v>
       </c>
-      <c r="K79" s="2">
-        <v>1.56E-3</v>
-      </c>
-      <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
-      <c r="O79" s="12"/>
-      <c r="P79" s="12"/>
-      <c r="Q79" s="12"/>
-      <c r="R79" s="12"/>
-      <c r="S79" s="12"/>
-      <c r="T79" s="14" t="e">
-        <f t="shared" ref="T79" si="12">HARMEAN(L79:O79)</f>
+      <c r="L79" s="25"/>
+      <c r="M79" s="25"/>
+      <c r="N79" s="25"/>
+      <c r="O79" s="25"/>
+      <c r="P79" s="25"/>
+      <c r="Q79" s="25"/>
+      <c r="R79" s="25"/>
+      <c r="S79" s="25"/>
+      <c r="T79" s="27" t="e">
+        <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
-      <c r="U79" s="14" t="e">
-        <f t="shared" ref="U79" si="13">HARMEAN(P79:S79)</f>
+      <c r="U79" s="27" t="e">
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
-      <c r="O80" s="12"/>
-      <c r="P80" s="12"/>
-      <c r="Q80" s="12"/>
-      <c r="R80" s="12"/>
-      <c r="S80" s="12"/>
-      <c r="T80" s="14"/>
-      <c r="U80" s="14"/>
-    </row>
-    <row r="81" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
-      <c r="O81" s="12"/>
-      <c r="P81" s="12"/>
-      <c r="Q81" s="12"/>
-      <c r="R81" s="12"/>
-      <c r="S81" s="12"/>
-      <c r="T81" s="12"/>
-      <c r="U81" s="12"/>
-    </row>
-    <row r="82" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L80" s="25"/>
+      <c r="M80" s="25"/>
+      <c r="N80" s="25"/>
+      <c r="O80" s="25"/>
+      <c r="P80" s="25"/>
+      <c r="Q80" s="25"/>
+      <c r="R80" s="25"/>
+      <c r="S80" s="25"/>
+      <c r="T80" s="27"/>
+      <c r="U80" s="27"/>
+    </row>
+    <row r="81" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="L81" s="25"/>
+      <c r="M81" s="25"/>
+      <c r="N81" s="25"/>
+      <c r="O81" s="25"/>
+      <c r="P81" s="25"/>
+      <c r="Q81" s="25"/>
+      <c r="R81" s="25"/>
+      <c r="S81" s="25"/>
+      <c r="T81" s="25"/>
+      <c r="U81" s="25"/>
+    </row>
+    <row r="82" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="C82">
+        <v>1</v>
+      </c>
       <c r="D82">
         <v>240</v>
       </c>
@@ -5495,46 +5646,49 @@
       <c r="K82" s="2">
         <v>1.8600000000000001E-3</v>
       </c>
-      <c r="L82" s="12">
+      <c r="L82" s="25">
         <v>0.54100000000000004</v>
       </c>
-      <c r="M82" s="12">
+      <c r="M82" s="25">
         <v>0.66900000000000004</v>
       </c>
-      <c r="N82" s="12">
+      <c r="N82" s="25">
         <v>0.51900000000000002</v>
       </c>
-      <c r="O82" s="12">
+      <c r="O82" s="25">
         <v>0.45800000000000002</v>
       </c>
-      <c r="P82" s="12">
+      <c r="P82" s="25">
         <v>0.57699999999999996</v>
       </c>
-      <c r="Q82" s="12">
+      <c r="Q82" s="25">
         <v>0.72099999999999997</v>
       </c>
-      <c r="R82" s="12">
+      <c r="R82" s="25">
         <v>0.57499999999999996</v>
       </c>
-      <c r="S82" s="12">
+      <c r="S82" s="25">
         <v>0.442</v>
       </c>
-      <c r="T82" s="13">
-        <f t="shared" ref="T82:T83" si="14">HARMEAN(L82:O82)</f>
+      <c r="T82" s="28">
+        <f t="shared" ref="T82:T83" si="12">HARMEAN(L82:O82)</f>
         <v>0.53666887107867123</v>
       </c>
-      <c r="U82" s="13">
-        <f t="shared" ref="U82:U83" si="15">HARMEAN(P82:S82)</f>
+      <c r="U82" s="28">
+        <f t="shared" ref="U82:U83" si="13">HARMEAN(P82:S82)</f>
         <v>0.56166848396011737</v>
       </c>
-      <c r="V82" t="s">
+      <c r="V82" s="29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>5</v>
       </c>
+      <c r="C83">
+        <v>1</v>
+      </c>
       <c r="D83">
         <v>240</v>
       </c>
@@ -5559,52 +5713,55 @@
       <c r="K83" s="2">
         <v>1.5900000000000001E-3</v>
       </c>
-      <c r="L83" s="12">
+      <c r="L83" s="25">
         <v>0.53600000000000003</v>
       </c>
-      <c r="M83" s="12">
+      <c r="M83" s="25">
         <v>0.65800000000000003</v>
       </c>
-      <c r="N83" s="12">
+      <c r="N83" s="25">
         <v>0.503</v>
       </c>
-      <c r="O83" s="12">
+      <c r="O83" s="25">
         <v>0.441</v>
       </c>
-      <c r="P83" s="12">
+      <c r="P83" s="25">
         <v>0.58099999999999996</v>
       </c>
-      <c r="Q83" s="12">
+      <c r="Q83" s="25">
         <v>0.73299999999999998</v>
       </c>
-      <c r="R83" s="12">
+      <c r="R83" s="25">
         <v>0.59699999999999998</v>
       </c>
-      <c r="S83" s="12">
+      <c r="S83" s="25">
         <v>0.438</v>
       </c>
-      <c r="T83" s="14">
-        <f t="shared" si="14"/>
+      <c r="T83" s="27">
+        <f t="shared" si="12"/>
         <v>0.52348663711711829</v>
       </c>
-      <c r="U83" s="14">
-        <f t="shared" si="15"/>
+      <c r="U83" s="27">
+        <f t="shared" si="13"/>
         <v>0.56789353356629468</v>
       </c>
     </row>
-    <row r="84" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
-      <c r="O84" s="12"/>
-      <c r="P84" s="12"/>
-      <c r="Q84" s="12"/>
-      <c r="R84" s="12"/>
-      <c r="S84" s="12"/>
-      <c r="T84" s="14"/>
-      <c r="U84" s="14"/>
-    </row>
-    <row r="85" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="L84" s="25"/>
+      <c r="M84" s="25"/>
+      <c r="N84" s="25"/>
+      <c r="O84" s="25"/>
+      <c r="P84" s="25"/>
+      <c r="Q84" s="25"/>
+      <c r="R84" s="25"/>
+      <c r="S84" s="25"/>
+      <c r="T84" s="27"/>
+      <c r="U84" s="27"/>
+    </row>
+    <row r="85" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="C85">
+        <v>1</v>
+      </c>
       <c r="D85">
         <v>240</v>
       </c>
@@ -5614,8 +5771,11 @@
       <c r="F85">
         <v>0.01</v>
       </c>
+      <c r="G85">
+        <v>15</v>
+      </c>
       <c r="H85">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I85">
         <v>300</v>
@@ -5623,30 +5783,49 @@
       <c r="J85" t="s">
         <v>26</v>
       </c>
-      <c r="K85" s="2">
-        <v>2.63E-3</v>
-      </c>
-      <c r="L85" s="12"/>
-      <c r="M85" s="12"/>
-      <c r="N85" s="12"/>
-      <c r="O85" s="12"/>
-      <c r="P85" s="12"/>
-      <c r="Q85" s="12"/>
-      <c r="R85" s="12"/>
-      <c r="S85" s="12"/>
-      <c r="T85" s="13" t="e">
-        <f t="shared" ref="T85:T86" si="16">HARMEAN(L85:O85)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U85" s="13" t="e">
-        <f t="shared" ref="U85:U86" si="17">HARMEAN(P85:S85)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="86" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="L85" s="25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M85" s="25">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="N85" s="25">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="O85" s="25">
+        <v>0.44</v>
+      </c>
+      <c r="P85" s="25">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="Q85" s="25">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="R85" s="25">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="S85" s="25">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T85" s="30">
+        <f t="shared" ref="T85:T86" si="14">HARMEAN(L85:O85)</f>
+        <v>0.54458264504852938</v>
+      </c>
+      <c r="U85" s="30">
+        <f t="shared" ref="U85:U86" si="15">HARMEAN(P85:S85)</f>
+        <v>0.53959294309558425</v>
+      </c>
+      <c r="V85" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="86" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B86">
         <v>6</v>
       </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
       <c r="D86">
         <v>240</v>
       </c>
@@ -5657,10 +5836,10 @@
         <v>0.01</v>
       </c>
       <c r="G86">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H86">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I86">
         <v>300</v>
@@ -5668,50 +5847,107 @@
       <c r="J86" t="s">
         <v>26</v>
       </c>
-      <c r="K86" s="2">
-        <v>1.56E-3</v>
-      </c>
-      <c r="L86" s="12"/>
-      <c r="M86" s="12"/>
-      <c r="N86" s="12"/>
-      <c r="O86" s="12"/>
-      <c r="P86" s="12"/>
-      <c r="Q86" s="12"/>
-      <c r="R86" s="12"/>
-      <c r="S86" s="12"/>
-      <c r="T86" s="14" t="e">
-        <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="U86" s="14" t="e">
-        <f t="shared" si="17"/>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="87" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="L87" s="12"/>
-      <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
-      <c r="O87" s="12"/>
-      <c r="P87" s="12"/>
-      <c r="Q87" s="12"/>
-      <c r="R87" s="12"/>
-      <c r="S87" s="12"/>
-      <c r="T87" s="14"/>
-      <c r="U87" s="14"/>
-    </row>
-    <row r="88" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="L86" s="25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M86" s="25">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="N86" s="25">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="O86" s="25">
+        <v>0.439</v>
+      </c>
+      <c r="P86" s="25">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="Q86" s="25">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="R86" s="25">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="S86" s="25">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="T86" s="27">
+        <f t="shared" si="14"/>
+        <v>0.54419907524651201</v>
+      </c>
+      <c r="U86" s="27">
+        <f t="shared" si="15"/>
+        <v>0.53605119015848213</v>
+      </c>
+      <c r="W86" s="25">
+        <v>0.751</v>
+      </c>
+      <c r="X86" s="25">
+        <v>0.755</v>
+      </c>
+      <c r="Y86" s="25">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="Z86" s="25">
+        <v>0.185</v>
+      </c>
+      <c r="AA86" s="25">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="AB86" s="25">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="AC86" s="25">
+        <v>0.625</v>
+      </c>
+      <c r="AD86" s="25">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="AE86" s="30">
+        <f t="shared" ref="AE86" si="16">HARMEAN(W86:Z86)</f>
+        <v>0.41625672942842756</v>
+      </c>
+      <c r="AF86" s="30">
+        <f t="shared" ref="AF86" si="17">HARMEAN(AA86:AD86)</f>
+        <v>0.40380252565986385</v>
+      </c>
+      <c r="AG86" s="31">
+        <v>0.51</v>
+      </c>
+      <c r="AH86" s="31">
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="87" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="L87" s="25"/>
+      <c r="M87" s="25"/>
+      <c r="N87" s="25"/>
+      <c r="O87" s="25"/>
+      <c r="P87" s="25"/>
+      <c r="Q87" s="25"/>
+      <c r="R87" s="25"/>
+      <c r="S87" s="25"/>
+      <c r="T87" s="27"/>
+      <c r="U87" s="27"/>
+    </row>
+    <row r="88" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="C88">
+        <v>2</v>
+      </c>
       <c r="D88">
         <v>240</v>
       </c>
       <c r="E88">
-        <v>1E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="F88">
         <v>0.01</v>
       </c>
+      <c r="G88">
+        <v>4</v>
+      </c>
       <c r="H88">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I88">
         <v>300</v>
@@ -5720,43 +5956,62 @@
         <v>26</v>
       </c>
       <c r="K88" s="2">
-        <v>2.63E-3</v>
-      </c>
-      <c r="L88" s="12"/>
-      <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
-      <c r="O88" s="12"/>
-      <c r="P88" s="12"/>
-      <c r="Q88" s="12"/>
-      <c r="R88" s="12"/>
-      <c r="S88" s="12"/>
-      <c r="T88" s="13" t="e">
+        <v>4.4099999999999999E-3</v>
+      </c>
+      <c r="L88" s="25">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="M88" s="25">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="N88" s="25">
+        <v>0.497</v>
+      </c>
+      <c r="O88" s="25">
+        <v>0.441</v>
+      </c>
+      <c r="P88" s="25">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="Q88" s="25">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="R88" s="25">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S88" s="25">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="T88" s="27">
         <f t="shared" ref="T88:T89" si="18">HARMEAN(L88:O88)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U88" s="13" t="e">
+        <v>0.5237299496823089</v>
+      </c>
+      <c r="U88" s="27">
         <f t="shared" ref="U88:U89" si="19">HARMEAN(P88:S88)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="89" spans="2:22" x14ac:dyDescent="0.2">
+        <v>0.51937760196054394</v>
+      </c>
+    </row>
+    <row r="89" spans="2:34" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>7</v>
       </c>
+      <c r="C89">
+        <v>2</v>
+      </c>
       <c r="D89">
         <v>240</v>
       </c>
       <c r="E89">
-        <v>1E-3</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="F89">
         <v>0.01</v>
       </c>
       <c r="G89">
+        <v>5</v>
+      </c>
+      <c r="H89">
         <v>10</v>
-      </c>
-      <c r="H89">
-        <v>20</v>
       </c>
       <c r="I89">
         <v>300</v>
@@ -5765,80 +6020,224 @@
         <v>26</v>
       </c>
       <c r="K89" s="2">
-        <v>1.56E-3</v>
-      </c>
-      <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-      <c r="O89" s="12"/>
-      <c r="P89" s="12"/>
-      <c r="Q89" s="12"/>
-      <c r="R89" s="12"/>
-      <c r="S89" s="12"/>
-      <c r="T89" s="14" t="e">
+        <v>3.4399999999999999E-3</v>
+      </c>
+      <c r="L89" s="25">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="M89" s="25">
+        <v>0.67900000000000005</v>
+      </c>
+      <c r="N89" s="25">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="O89" s="25">
+        <v>0.432</v>
+      </c>
+      <c r="P89" s="25">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="Q89" s="25">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="R89" s="25">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="S89" s="25">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="T89" s="27">
         <f t="shared" si="18"/>
+        <v>0.53463630147362762</v>
+      </c>
+      <c r="U89" s="27">
+        <f t="shared" si="19"/>
+        <v>0.5273462685618211</v>
+      </c>
+      <c r="W89" s="1">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="X89" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="Y89" s="1">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="Z89" s="1">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="AA89" s="1">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="AB89" s="1">
+        <v>0.67800000000000005</v>
+      </c>
+      <c r="AC89" s="1">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="AD89" s="1">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AE89" s="7">
+        <f t="shared" ref="AE89" si="20">HARMEAN(W89:Z89)</f>
+        <v>0.38441426085807595</v>
+      </c>
+      <c r="AF89" s="7">
+        <f t="shared" ref="AF89" si="21">HARMEAN(AA89:AD89)</f>
+        <v>0.37342162410993751</v>
+      </c>
+      <c r="AG89" s="26">
+        <v>0.432</v>
+      </c>
+      <c r="AH89" s="26">
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="T90" s="8"/>
+      <c r="U90" s="8"/>
+    </row>
+    <row r="91" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="C91">
+        <v>2</v>
+      </c>
+      <c r="D91">
+        <v>240</v>
+      </c>
+      <c r="E91">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F91">
+        <v>0.01</v>
+      </c>
+      <c r="H91">
+        <v>20</v>
+      </c>
+      <c r="I91">
+        <v>300</v>
+      </c>
+      <c r="J91" t="s">
+        <v>26</v>
+      </c>
+      <c r="L91" s="25"/>
+      <c r="M91" s="25"/>
+      <c r="N91" s="25"/>
+      <c r="O91" s="25"/>
+      <c r="P91" s="25"/>
+      <c r="Q91" s="25"/>
+      <c r="R91" s="25"/>
+      <c r="S91" s="25"/>
+      <c r="T91" s="27" t="e">
+        <f t="shared" ref="T91:T92" si="22">HARMEAN(L91:O91)</f>
         <v>#N/A</v>
       </c>
-      <c r="U89" s="14" t="e">
-        <f t="shared" si="19"/>
+      <c r="U91" s="27" t="e">
+        <f t="shared" ref="U91:U92" si="23">HARMEAN(P91:S91)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="90" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="T90" s="10"/>
-      <c r="U90" s="10"/>
-    </row>
-    <row r="91" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="T91" s="10"/>
-      <c r="U91" s="10"/>
-    </row>
-    <row r="92" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="T92" s="10"/>
-      <c r="U92" s="10"/>
-    </row>
-    <row r="93" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B93" t="s">
+    <row r="92" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>8</v>
+      </c>
+      <c r="C92">
+        <v>2</v>
+      </c>
+      <c r="D92">
+        <v>240</v>
+      </c>
+      <c r="E92">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F92">
+        <v>0.01</v>
+      </c>
+      <c r="G92">
+        <v>10</v>
+      </c>
+      <c r="H92">
+        <v>20</v>
+      </c>
+      <c r="I92">
+        <v>300</v>
+      </c>
+      <c r="J92" t="s">
+        <v>26</v>
+      </c>
+      <c r="L92" s="25"/>
+      <c r="M92" s="25"/>
+      <c r="N92" s="25"/>
+      <c r="O92" s="25"/>
+      <c r="P92" s="25"/>
+      <c r="Q92" s="25"/>
+      <c r="R92" s="25"/>
+      <c r="S92" s="25"/>
+      <c r="T92" s="27" t="e">
+        <f t="shared" si="22"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U92" s="27" t="e">
+        <f t="shared" si="23"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="93" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="T93" s="8"/>
+      <c r="U93" s="8"/>
+    </row>
+    <row r="94" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="T94" s="8"/>
+      <c r="U94" s="8"/>
+    </row>
+    <row r="95" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="T95" s="8"/>
+      <c r="U95" s="8"/>
+    </row>
+    <row r="96" spans="2:34" x14ac:dyDescent="0.2">
+      <c r="B96" t="s">
         <v>23</v>
       </c>
-      <c r="L93" s="1">
+      <c r="L96" s="1">
         <v>0.58399999999999996</v>
       </c>
-      <c r="M93" s="1">
+      <c r="M96" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="N93" s="1">
+      <c r="N96" s="1">
         <v>0.6</v>
       </c>
-      <c r="O93" s="1">
+      <c r="O96" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="P93" s="1">
+      <c r="P96" s="1">
         <v>0.56799999999999995</v>
       </c>
-      <c r="Q93" s="1">
+      <c r="Q96" s="1">
         <v>0.70099999999999996</v>
       </c>
-      <c r="R93" s="1">
+      <c r="R96" s="1">
         <v>0.55800000000000005</v>
       </c>
-      <c r="S93" s="1">
+      <c r="S96" s="1">
         <v>0.432</v>
       </c>
-      <c r="T93" s="9">
-        <f t="shared" ref="T93" si="20">HARMEAN(L93:O93)</f>
+      <c r="T96" s="7">
+        <f t="shared" ref="T96" si="24">HARMEAN(L96:O96)</f>
         <v>0.57826082952638469</v>
       </c>
-      <c r="U93" s="9">
-        <f t="shared" ref="U93" si="21">HARMEAN(P93:S93)</f>
+      <c r="U96" s="7">
+        <f t="shared" ref="U96" si="25">HARMEAN(P96:S96)</f>
         <v>0.54839395595501261</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="AG65:AH65"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C65:G65"/>
     <mergeCell ref="K3:S3"/>
     <mergeCell ref="K65:S65"/>
+    <mergeCell ref="V65:AD65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5846,451 +6245,516 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>1</v>
+        <v>71</v>
+      </c>
+      <c r="C1" s="16">
+        <v>2</v>
+      </c>
+      <c r="D1" s="16">
+        <v>6</v>
+      </c>
+      <c r="E1" s="16">
+        <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16">
+        <v>1</v>
+      </c>
+      <c r="E2" s="16">
+        <v>2</v>
+      </c>
       <c r="I2" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="8">
+        <v>60</v>
+      </c>
+      <c r="J2" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="6">
         <v>1E-3</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="6">
         <v>1E-3</v>
       </c>
-      <c r="M2" s="8">
+      <c r="M2" s="6">
         <v>1E-3</v>
       </c>
-      <c r="N2" s="8">
+      <c r="N2" s="6">
         <v>0.01</v>
       </c>
-      <c r="O2" s="8">
+      <c r="O2" s="6">
         <v>0.01</v>
       </c>
-      <c r="P2" s="8">
+      <c r="P2" s="6">
         <v>0.01</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="Q2" s="6">
         <v>0.01</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R2" s="6">
         <v>0.01</v>
       </c>
-      <c r="S2" s="8">
+      <c r="S2" s="6">
         <v>0.01</v>
       </c>
-      <c r="T2" s="8">
+      <c r="T2" s="6">
         <v>0.01</v>
       </c>
-      <c r="U2" s="8">
+      <c r="U2" s="6">
         <v>0.01</v>
       </c>
-      <c r="V2" s="8">
+      <c r="V2" s="6">
         <v>0.01</v>
       </c>
-      <c r="W2" s="8">
+      <c r="W2" s="6">
         <v>0.01</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>31</v>
-      </c>
+      <c r="A3" s="23"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="16">
-        <v>100</v>
+        <v>240</v>
+      </c>
+      <c r="D3" s="16">
+        <v>240</v>
+      </c>
+      <c r="E3" s="16">
+        <v>240</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="6">
         <v>2</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="6">
         <v>2</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="6">
         <v>2</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="6">
         <v>3</v>
       </c>
-      <c r="N3" s="8">
+      <c r="N3" s="6">
         <v>2</v>
       </c>
-      <c r="O3" s="8">
+      <c r="O3" s="6">
         <v>3</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="6">
         <v>2</v>
       </c>
-      <c r="Q3" s="8">
+      <c r="Q3" s="6">
         <v>2</v>
       </c>
-      <c r="R3" s="8">
+      <c r="R3" s="6">
         <v>2</v>
       </c>
-      <c r="S3" s="8">
+      <c r="S3" s="6">
         <v>4</v>
       </c>
-      <c r="T3" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="U3" s="8">
+      <c r="T3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" s="6">
         <v>2</v>
       </c>
-      <c r="V3" s="8">
+      <c r="V3" s="6">
         <v>2</v>
       </c>
-      <c r="W3" s="8">
+      <c r="W3" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="16">
-        <v>0.01</v>
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D4" s="16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E4" s="16">
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="I4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="6">
         <v>200</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="6">
         <v>200</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="6">
         <v>200</v>
       </c>
-      <c r="M4" s="8">
+      <c r="M4" s="6">
         <v>200</v>
       </c>
-      <c r="N4" s="8">
+      <c r="N4" s="6">
         <v>200</v>
       </c>
-      <c r="O4" s="8">
+      <c r="O4" s="6">
         <v>200</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="6">
         <v>200</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="6">
         <v>200</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4" s="6">
         <v>100</v>
       </c>
-      <c r="S4" s="8">
+      <c r="S4" s="6">
         <v>200</v>
       </c>
-      <c r="T4" s="8">
+      <c r="T4" s="6">
         <v>200</v>
       </c>
-      <c r="U4" s="8">
+      <c r="U4" s="6">
         <v>200</v>
       </c>
-      <c r="V4" s="8">
+      <c r="V4" s="6">
         <v>100</v>
       </c>
-      <c r="W4" s="8">
+      <c r="W4" s="6">
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="16">
         <v>0.01</v>
       </c>
+      <c r="D5" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.01</v>
+      </c>
       <c r="I5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="6">
         <v>1E-3</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="6">
         <v>0.01</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="6">
         <v>0.01</v>
       </c>
-      <c r="M5" s="8">
+      <c r="M5" s="6">
         <v>0.01</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="6">
         <v>0.01</v>
       </c>
-      <c r="O5" s="8">
+      <c r="O5" s="6">
         <v>0.01</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="6">
         <v>0.1</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="6">
         <v>0.1</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="6">
         <v>0.1</v>
       </c>
-      <c r="S5" s="8">
+      <c r="S5" s="6">
         <v>0.1</v>
       </c>
-      <c r="T5" s="8">
+      <c r="T5" s="6">
         <v>0.1</v>
       </c>
-      <c r="U5" s="8">
+      <c r="U5" s="6">
         <v>0.1</v>
       </c>
-      <c r="V5" s="8">
+      <c r="V5" s="6">
         <v>0.1</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="6">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>60</v>
+      <c r="C6" s="16">
+        <v>50</v>
+      </c>
+      <c r="D6" s="16">
+        <v>20</v>
+      </c>
+      <c r="E6" s="16">
+        <v>5</v>
       </c>
       <c r="I6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="6">
         <v>8</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="6">
         <v>9</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <v>8</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="6">
         <v>9</v>
       </c>
-      <c r="N6" s="8">
+      <c r="N6" s="6">
         <v>9</v>
       </c>
-      <c r="O6" s="8">
+      <c r="O6" s="6">
         <v>19</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="6">
         <v>5</v>
       </c>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8">
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6">
         <v>5</v>
       </c>
-      <c r="S6" s="8">
+      <c r="S6" s="6">
         <v>3</v>
       </c>
-      <c r="T6" s="8">
+      <c r="T6" s="6">
         <v>7</v>
       </c>
-      <c r="U6" s="8">
+      <c r="U6" s="6">
         <v>4</v>
       </c>
-      <c r="V6" s="8">
+      <c r="V6" s="6">
         <v>4</v>
       </c>
-      <c r="W6" s="8"/>
+      <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="16">
+        <v>38</v>
+      </c>
+      <c r="D7" s="16">
+        <v>38</v>
+      </c>
+      <c r="E7" s="16">
+        <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="6">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="8">
+      <c r="K7" s="6">
         <v>20</v>
       </c>
-      <c r="K7" s="8">
+      <c r="L7" s="6">
         <v>20</v>
       </c>
-      <c r="L7" s="8">
+      <c r="M7" s="6">
         <v>20</v>
       </c>
-      <c r="M7" s="8">
+      <c r="N7" s="6">
         <v>20</v>
       </c>
-      <c r="N7" s="8">
+      <c r="O7" s="6">
         <v>20</v>
       </c>
-      <c r="O7" s="8">
+      <c r="P7" s="6">
         <v>20</v>
       </c>
-      <c r="P7" s="8">
+      <c r="Q7" s="6">
+        <v>35</v>
+      </c>
+      <c r="R7" s="6">
         <v>20</v>
       </c>
-      <c r="Q7" s="8">
-        <v>35</v>
-      </c>
-      <c r="R7" s="8">
+      <c r="S7" s="6">
         <v>20</v>
       </c>
-      <c r="S7" s="8">
+      <c r="T7" s="6">
         <v>20</v>
       </c>
-      <c r="T7" s="8">
+      <c r="U7" s="6">
         <v>20</v>
       </c>
-      <c r="U7" s="8">
+      <c r="V7" s="6">
         <v>20</v>
       </c>
-      <c r="V7" s="8">
+      <c r="W7" s="6">
         <v>20</v>
       </c>
-      <c r="W7" s="8">
-        <v>20</v>
-      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="16">
         <v>200</v>
       </c>
+      <c r="D8" s="16">
+        <v>300</v>
+      </c>
+      <c r="E8" s="16">
+        <v>300</v>
+      </c>
       <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="6">
         <v>300</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="6">
         <v>300</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="6">
         <v>300</v>
       </c>
-      <c r="M8" s="8">
+      <c r="M8" s="6">
         <v>300</v>
       </c>
-      <c r="N8" s="8">
+      <c r="N8" s="6">
         <v>300</v>
       </c>
-      <c r="O8" s="8">
+      <c r="O8" s="6">
         <v>300</v>
       </c>
-      <c r="P8" s="8">
+      <c r="P8" s="6">
         <v>300</v>
       </c>
-      <c r="Q8" s="8">
+      <c r="Q8" s="6">
         <v>300</v>
       </c>
-      <c r="R8" s="8">
+      <c r="R8" s="6">
         <v>300</v>
       </c>
-      <c r="S8" s="8">
+      <c r="S8" s="6">
         <v>300</v>
       </c>
-      <c r="T8" s="8">
+      <c r="T8" s="6">
         <v>300</v>
       </c>
-      <c r="U8" s="8">
+      <c r="U8" s="6">
         <v>300</v>
       </c>
-      <c r="V8" s="8">
+      <c r="V8" s="6">
         <v>300</v>
       </c>
-      <c r="W8" s="8">
+      <c r="W8" s="6">
         <v>300</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
+      <c r="A9" s="23"/>
       <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>26</v>
       </c>
+      <c r="D9" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="I9" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="8" t="s">
+      <c r="K9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="N9" s="8" t="s">
+      <c r="M9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="Q9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="S9" s="8" t="s">
+      <c r="R9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="T9" s="8" t="s">
+      <c r="T9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="U9" s="8" t="s">
+      <c r="U9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="8" t="s">
+      <c r="V9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="W9" s="8" t="s">
+      <c r="W9" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -6298,347 +6762,258 @@
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="1"/>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
+      <c r="C11" s="16" t="s">
+        <v>57</v>
       </c>
       <c r="J11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="15">
-        <v>0.54900000000000004</v>
-      </c>
-      <c r="D12" s="15">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="E12" s="15">
-        <v>0.53400000000000003</v>
-      </c>
-      <c r="F12" s="15">
-        <v>0.441</v>
-      </c>
-      <c r="G12" s="15">
-        <f t="shared" ref="G12:G13" si="0">HARMEAN(C12:F12)</f>
-        <v>0.53740269136538665</v>
-      </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="26">
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32">
+        <v>7.6100000000000001E-2</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="21">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="21">
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="L12" s="26">
+      <c r="L12" s="21">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="M12" s="26">
+      <c r="M12" s="21">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="N12" s="26">
+      <c r="N12" s="21">
         <v>8.1299999999999997E-2</v>
       </c>
-      <c r="O12" s="26">
+      <c r="O12" s="21">
         <v>8.0699999999999994E-2</v>
       </c>
-      <c r="P12" s="25">
+      <c r="P12" s="20">
         <v>8.1100000000000005E-2</v>
       </c>
-      <c r="Q12" s="26">
+      <c r="Q12" s="21">
         <v>8.2799999999999999E-2</v>
       </c>
-      <c r="R12" s="26">
+      <c r="R12" s="21">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="S12" s="26">
+      <c r="S12" s="21">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="T12" s="25">
+      <c r="T12" s="20">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12" s="20">
         <v>0.10100000000000001</v>
       </c>
-      <c r="V12" s="25">
+      <c r="V12" s="20">
         <v>7.8E-2</v>
       </c>
-      <c r="W12" s="25"/>
+      <c r="W12" s="20"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="15">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.72599999999999998</v>
-      </c>
-      <c r="E13" s="15">
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0.432</v>
-      </c>
-      <c r="G13" s="15">
-        <f t="shared" si="0"/>
-        <v>0.56397720103593907</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="25">
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="20">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K13" s="25">
+      <c r="K13" s="20">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="L13" s="25">
+      <c r="L13" s="20">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="M13" s="25">
+      <c r="M13" s="20">
         <v>6.83E-2</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="20">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="20">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="P13" s="25">
+      <c r="P13" s="20">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="Q13" s="25">
+      <c r="Q13" s="20">
         <v>7.4700000000000003E-2</v>
       </c>
-      <c r="R13" s="25">
+      <c r="R13" s="20">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="S13" s="25">
+      <c r="S13" s="20">
         <v>6.08E-2</v>
       </c>
-      <c r="T13" s="25">
+      <c r="T13" s="20">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="U13" s="25">
+      <c r="U13" s="20">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="V13" s="25">
+      <c r="V13" s="20">
         <v>8.3699999999999997E-2</v>
       </c>
-      <c r="W13" s="25"/>
+      <c r="W13" s="20"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="15">
-        <v>0.752</v>
-      </c>
-      <c r="D14" s="15">
-        <v>0.755</v>
-      </c>
-      <c r="E14" s="15">
-        <v>0.63700000000000001</v>
-      </c>
-      <c r="F14" s="15">
-        <v>0.191</v>
-      </c>
-      <c r="G14" s="19">
-        <f t="shared" ref="G14:G15" si="1">HARMEAN(C14:F14)</f>
-        <v>0.42284409505598886</v>
-      </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="26">
+      <c r="C14" s="32">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0.51</v>
+      </c>
+      <c r="E14" s="32">
+        <v>0.43159999999999998</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="21">
         <v>0.29330000000000001</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="21">
         <v>0.35299999999999998</v>
       </c>
-      <c r="L14" s="26">
+      <c r="L14" s="21">
         <v>0.38300000000000001</v>
       </c>
-      <c r="M14" s="26">
+      <c r="M14" s="21">
         <v>0.35299999999999998</v>
       </c>
-      <c r="N14" s="26">
+      <c r="N14" s="21">
         <v>0.379</v>
       </c>
-      <c r="O14" s="26">
+      <c r="O14" s="21">
         <v>0.38200000000000001</v>
       </c>
-      <c r="P14" s="25">
+      <c r="P14" s="20">
         <v>0.43</v>
       </c>
-      <c r="Q14" s="26">
+      <c r="Q14" s="21">
         <v>0.34699999999999998</v>
       </c>
-      <c r="R14" s="26">
+      <c r="R14" s="21">
         <v>0.42499999999999999</v>
       </c>
-      <c r="S14" s="26">
+      <c r="S14" s="21">
         <v>0.36299999999999999</v>
       </c>
-      <c r="T14" s="25">
+      <c r="T14" s="20">
         <v>0.42099999999999999</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14" s="20">
         <v>0.44800000000000001</v>
       </c>
-      <c r="V14" s="25">
+      <c r="V14" s="20">
         <v>0.45800000000000002</v>
       </c>
-      <c r="W14" s="25"/>
+      <c r="W14" s="20"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="15">
-        <v>0.70399999999999996</v>
-      </c>
-      <c r="D15" s="15">
-        <v>0.70799999999999996</v>
-      </c>
-      <c r="E15" s="15">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="F15" s="15">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="G15" s="15">
-        <f t="shared" si="1"/>
-        <v>0.39675125261755295</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="J15" s="25">
+      <c r="C15" s="32">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="D15" s="32">
+        <v>0.499</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0.41439999999999999</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J15" s="20">
         <v>0.28100000000000003</v>
       </c>
-      <c r="K15" s="25">
+      <c r="K15" s="20">
         <v>0.35599999999999998</v>
       </c>
-      <c r="L15" s="25">
+      <c r="L15" s="20">
         <v>0.371</v>
       </c>
-      <c r="M15" s="25">
+      <c r="M15" s="20">
         <v>0.35599999999999998</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="20">
         <v>0.374</v>
       </c>
-      <c r="O15" s="25">
+      <c r="O15" s="20">
         <v>0.38500000000000001</v>
       </c>
-      <c r="P15" s="25">
+      <c r="P15" s="20">
         <v>0.433</v>
       </c>
-      <c r="Q15" s="25">
+      <c r="Q15" s="20">
         <v>0.34</v>
       </c>
-      <c r="R15" s="25">
+      <c r="R15" s="20">
         <v>0.44800000000000001</v>
       </c>
-      <c r="S15" s="25">
+      <c r="S15" s="20">
         <v>0.34200000000000003</v>
       </c>
-      <c r="T15" s="25">
+      <c r="T15" s="20">
         <v>0.433</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15" s="20">
         <v>0.46</v>
       </c>
-      <c r="V15" s="25">
+      <c r="V15" s="20">
         <v>0.45400000000000001</v>
       </c>
-      <c r="W15" s="25"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="18">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="D17" s="15">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="E17" s="15">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="15">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="D18" s="15">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="E18" s="15">
-        <v>0.59</v>
-      </c>
+      <c r="W15" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A3:A9"/>
+  <mergeCells count="3">
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A2:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6654,10 +7029,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="16" customWidth="1"/>
-    <col min="4" max="13" width="10.83203125" style="15"/>
+    <col min="3" max="3" width="13.83203125" style="11" customWidth="1"/>
+    <col min="4" max="13" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -6666,1257 +7041,1260 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="11">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="21"/>
+      <c r="A3" s="23"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="11">
         <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="11">
         <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="11">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C9" s="17"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="23" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="22" t="s">
+      <c r="C10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22" t="s">
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="J11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="17">
+        <v>41</v>
+      </c>
+      <c r="C12" s="12">
         <v>9.4800000000000006E-3</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="10">
         <v>0.53500000000000003</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="10">
         <v>0.67600000000000005</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="10">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="10">
         <v>0.43</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="10">
         <f>HARMEAN(D12:G12)</f>
         <v>0.53388772000237805</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="10">
         <v>0.55100000000000005</v>
       </c>
-      <c r="J12" s="15">
+      <c r="J12" s="10">
         <v>0.69399999999999995</v>
       </c>
-      <c r="K12" s="15">
+      <c r="K12" s="10">
         <v>0.53800000000000003</v>
       </c>
-      <c r="L12" s="15">
+      <c r="L12" s="10">
         <v>0.41599999999999998</v>
       </c>
-      <c r="M12" s="15">
+      <c r="M12" s="10">
         <f>HARMEAN(I12:L12)</f>
         <v>0.5320290509068597</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" s="17">
+        <v>42</v>
+      </c>
+      <c r="C13" s="12">
         <v>7.43E-3</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="10">
         <v>0.54800000000000004</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="10">
         <v>0.65700000000000003</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="10">
         <v>0.51900000000000002</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="10">
         <v>0.442</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="10">
         <f t="shared" ref="H13:H21" si="0">HARMEAN(D13:G13)</f>
         <v>0.53077758646083895</v>
       </c>
-      <c r="I13" s="15">
+      <c r="I13" s="10">
         <v>0.56499999999999995</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="10">
         <v>0.69199999999999995</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="10">
         <v>0.55900000000000005</v>
       </c>
-      <c r="L13" s="15">
+      <c r="L13" s="10">
         <v>0.42</v>
       </c>
-      <c r="M13" s="15">
+      <c r="M13" s="10">
         <f t="shared" ref="M13:M21" si="1">HARMEAN(I13:L13)</f>
         <v>0.54164877177034054</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="17">
+        <v>43</v>
+      </c>
+      <c r="C14" s="12">
         <v>6.6600000000000001E-3</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="10">
         <v>0.53400000000000003</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="10">
         <v>0.64100000000000001</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="10">
         <v>0.47099999999999997</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="10">
         <v>0.42799999999999999</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="10">
         <f t="shared" si="0"/>
         <v>0.50682230802479034</v>
       </c>
-      <c r="I14" s="15">
+      <c r="I14" s="10">
         <v>0.54100000000000004</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="10">
         <v>0.67300000000000004</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="10">
         <v>0.53200000000000003</v>
       </c>
-      <c r="L14" s="15">
+      <c r="L14" s="10">
         <v>0.42899999999999999</v>
       </c>
-      <c r="M14" s="15">
+      <c r="M14" s="10">
         <f t="shared" si="1"/>
         <v>0.53015139887428453</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="17">
+        <v>44</v>
+      </c>
+      <c r="C15" s="12">
         <v>6.4999999999999997E-3</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="10">
         <v>0.54900000000000004</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="10">
         <v>0.67500000000000004</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="10">
         <v>0.53400000000000003</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="10">
         <v>0.441</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="10">
         <f t="shared" si="0"/>
         <v>0.53740269136538665</v>
       </c>
-      <c r="I15" s="15">
+      <c r="I15" s="10">
         <v>0.57499999999999996</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="10">
         <v>0.72599999999999998</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="10">
         <v>0.60199999999999998</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="10">
         <v>0.432</v>
       </c>
-      <c r="M15" s="15">
+      <c r="M15" s="10">
         <f t="shared" si="1"/>
         <v>0.56397720103593907</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="17">
+        <v>45</v>
+      </c>
+      <c r="C16" s="12">
         <v>5.4299999999999999E-3</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="10">
         <v>0.54700000000000004</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="10">
         <v>0.66700000000000004</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="10">
         <v>0.52900000000000003</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="10">
         <v>0.435</v>
       </c>
-      <c r="H16" s="15">
+      <c r="H16" s="10">
         <f t="shared" si="0"/>
         <v>0.53215452714086109</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="10">
         <v>0.57199999999999995</v>
       </c>
-      <c r="J16" s="15">
+      <c r="J16" s="10">
         <v>0.71</v>
       </c>
-      <c r="K16" s="15">
+      <c r="K16" s="10">
         <v>0.57499999999999996</v>
       </c>
-      <c r="L16" s="15">
+      <c r="L16" s="10">
         <v>0.44</v>
       </c>
-      <c r="M16" s="15">
+      <c r="M16" s="10">
         <f t="shared" si="1"/>
         <v>0.5579921086980546</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="17">
+        <v>46</v>
+      </c>
+      <c r="C17" s="12">
         <v>5.0600000000000003E-3</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="10">
         <v>0.54</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="10">
         <v>0.68300000000000005</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="10">
         <v>0.54500000000000004</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="10">
         <v>0.44900000000000001</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="14">
         <f t="shared" si="0"/>
         <v>0.54215127397444018</v>
       </c>
-      <c r="I17" s="15">
+      <c r="I17" s="10">
         <v>0.58399999999999996</v>
       </c>
-      <c r="J17" s="15">
+      <c r="J17" s="10">
         <v>0.73699999999999999</v>
       </c>
-      <c r="K17" s="15">
+      <c r="K17" s="10">
         <v>0.61799999999999999</v>
       </c>
-      <c r="L17" s="15">
+      <c r="L17" s="10">
         <v>0.42899999999999999</v>
       </c>
-      <c r="M17" s="15">
+      <c r="M17" s="10">
         <f t="shared" si="1"/>
         <v>0.56993808736940832</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="17">
+        <v>47</v>
+      </c>
+      <c r="C18" s="12">
         <v>4.6899999999999997E-3</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="10">
         <v>0.54500000000000004</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="10">
         <v>0.66400000000000003</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="10">
         <v>0.51900000000000002</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="10">
         <v>0.44400000000000001</v>
       </c>
-      <c r="H18" s="15">
+      <c r="H18" s="10">
         <f t="shared" si="0"/>
         <v>0.5319204810765471</v>
       </c>
-      <c r="I18" s="15">
+      <c r="I18" s="10">
         <v>0.57599999999999996</v>
       </c>
-      <c r="J18" s="15">
+      <c r="J18" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="10">
         <v>0.56499999999999995</v>
       </c>
-      <c r="L18" s="15">
+      <c r="L18" s="10">
         <v>0.44500000000000001</v>
       </c>
-      <c r="M18" s="15">
+      <c r="M18" s="10">
         <f t="shared" si="1"/>
         <v>0.55806368101698878</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="17">
+        <v>48</v>
+      </c>
+      <c r="C19" s="12">
         <v>3.7599999999999999E-3</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="10">
         <v>0.54100000000000004</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="10">
         <v>0.67600000000000005</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="10">
         <v>0.53400000000000003</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G19" s="10">
         <v>0.436</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="10">
         <f t="shared" si="0"/>
         <v>0.5337634802270812</v>
       </c>
-      <c r="I19" s="15">
+      <c r="I19" s="10">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J19" s="15">
+      <c r="J19" s="10">
         <v>0.68400000000000005</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="10">
         <v>0.54300000000000004</v>
       </c>
-      <c r="L19" s="15">
+      <c r="L19" s="10">
         <v>0.437</v>
       </c>
-      <c r="M19" s="15">
+      <c r="M19" s="10">
         <f t="shared" si="1"/>
         <v>0.54217786380777488</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="17">
+        <v>49</v>
+      </c>
+      <c r="C20" s="12">
         <v>3.4199999999999999E-3</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="10">
         <v>0.54</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="10">
         <v>0.67200000000000004</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="10">
         <v>0.52900000000000003</v>
       </c>
-      <c r="G20" s="15">
+      <c r="G20" s="10">
         <v>0.441</v>
       </c>
-      <c r="H20" s="15">
+      <c r="H20" s="10">
         <f t="shared" si="0"/>
         <v>0.53348413476369205</v>
       </c>
-      <c r="I20" s="15">
+      <c r="I20" s="10">
         <v>0.58499999999999996</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="10">
         <v>0.71399999999999997</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K20" s="10">
         <v>0.58099999999999996</v>
       </c>
-      <c r="L20" s="15">
+      <c r="L20" s="10">
         <v>0.442</v>
       </c>
-      <c r="M20" s="15">
+      <c r="M20" s="10">
         <f t="shared" si="1"/>
         <v>0.5638905018664454</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="17">
+        <v>50</v>
+      </c>
+      <c r="C21" s="12">
         <v>2.8999999999999998E-3</v>
       </c>
-      <c r="D21" s="15">
+      <c r="D21" s="10">
         <v>0.54</v>
       </c>
-      <c r="E21" s="15">
+      <c r="E21" s="10">
         <v>0.66300000000000003</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="10">
         <v>0.50800000000000001</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="10">
         <v>0.43</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="10">
         <f t="shared" si="0"/>
         <v>0.52258666534092002</v>
       </c>
-      <c r="I21" s="15">
+      <c r="I21" s="10">
         <v>0.57399999999999995</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="10">
         <v>0.70199999999999996</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="10">
         <v>0.54800000000000004</v>
       </c>
-      <c r="L21" s="15">
+      <c r="L21" s="10">
         <v>0.45100000000000001</v>
       </c>
-      <c r="M21" s="15">
+      <c r="M21" s="10">
         <f t="shared" si="1"/>
         <v>0.5548793640169275</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="D22" s="22" t="s">
+      <c r="D22" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22" t="s">
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="1"/>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="L23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="M23" s="15" t="s">
+      <c r="M23" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="15">
+        <v>41</v>
+      </c>
+      <c r="D24" s="10">
         <v>0.69199999999999995</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="10">
         <v>0.69599999999999995</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="10">
         <v>0.55600000000000005</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="10">
         <v>0.182</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H24" s="10">
         <f>HARMEAN(D24:G24)</f>
         <v>0.39312290601678107</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="10">
         <v>0.69299999999999995</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="10">
         <v>0.69599999999999995</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="10">
         <v>0.57399999999999995</v>
       </c>
-      <c r="L24" s="15">
+      <c r="L24" s="10">
         <v>0.17599999999999999</v>
       </c>
-      <c r="M24" s="15">
+      <c r="M24" s="10">
         <f>HARMEAN(I24:L24)</f>
         <v>0.38820774287586218</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="15">
+        <v>42</v>
+      </c>
+      <c r="D25" s="10">
         <v>0.73199999999999998</v>
       </c>
-      <c r="E25" s="15">
+      <c r="E25" s="10">
         <v>0.73599999999999999</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="10">
         <v>0.60899999999999999</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="10">
         <v>0.187</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="10">
         <f t="shared" ref="H25:H33" si="2">HARMEAN(D25:G25)</f>
         <v>0.41175792974529757</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="10">
         <v>0.69299999999999995</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="10">
         <v>0.69599999999999995</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="10">
         <v>0.57099999999999995</v>
       </c>
-      <c r="L25" s="15">
+      <c r="L25" s="10">
         <v>0.17599999999999999</v>
       </c>
-      <c r="M25" s="15">
+      <c r="M25" s="10">
         <f t="shared" ref="M25:M33" si="3">HARMEAN(I25:L25)</f>
         <v>0.38786318988759</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="15">
+        <v>43</v>
+      </c>
+      <c r="D26" s="10">
         <v>0.72499999999999998</v>
       </c>
-      <c r="E26" s="15">
+      <c r="E26" s="10">
         <v>0.72699999999999998</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="10">
         <v>0.59899999999999998</v>
       </c>
-      <c r="G26" s="15">
+      <c r="G26" s="10">
         <v>0.187</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="10">
         <f t="shared" si="2"/>
         <v>0.40933828220850771</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="10">
         <v>0.69499999999999995</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="10">
         <v>0.7</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="10">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L26" s="15">
+      <c r="L26" s="10">
         <v>0.17799999999999999</v>
       </c>
-      <c r="M26" s="15">
+      <c r="M26" s="10">
         <f t="shared" si="3"/>
         <v>0.39063324593071325</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="15">
+        <v>44</v>
+      </c>
+      <c r="D27" s="10">
         <v>0.752</v>
       </c>
-      <c r="E27" s="15">
+      <c r="E27" s="10">
         <v>0.755</v>
       </c>
-      <c r="F27" s="15">
+      <c r="F27" s="10">
         <v>0.63700000000000001</v>
       </c>
-      <c r="G27" s="15">
+      <c r="G27" s="10">
         <v>0.191</v>
       </c>
-      <c r="H27" s="19">
+      <c r="H27" s="14">
         <f t="shared" si="2"/>
         <v>0.42284409505598886</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="10">
         <v>0.70399999999999996</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="10">
         <v>0.70799999999999996</v>
       </c>
-      <c r="K27" s="15">
+      <c r="K27" s="10">
         <v>0.57999999999999996</v>
       </c>
-      <c r="L27" s="15">
+      <c r="L27" s="10">
         <v>0.18099999999999999</v>
       </c>
-      <c r="M27" s="15">
+      <c r="M27" s="10">
         <f t="shared" si="3"/>
         <v>0.39675125261755295</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="15">
+        <v>45</v>
+      </c>
+      <c r="D28" s="10">
         <v>0.74</v>
       </c>
-      <c r="E28" s="15">
+      <c r="E28" s="10">
         <v>0.74299999999999999</v>
       </c>
-      <c r="F28" s="15">
+      <c r="F28" s="10">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G28" s="15">
+      <c r="G28" s="10">
         <v>0.188</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="10">
         <f t="shared" si="2"/>
         <v>0.41483398337066851</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="10">
         <v>0.71</v>
       </c>
-      <c r="K28" s="15">
+      <c r="K28" s="10">
         <v>0.59499999999999997</v>
       </c>
-      <c r="L28" s="15">
+      <c r="L28" s="10">
         <v>0.17799999999999999</v>
       </c>
-      <c r="M28" s="15">
+      <c r="M28" s="10">
         <f t="shared" si="3"/>
         <v>0.39519726024260893</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="15">
+        <v>46</v>
+      </c>
+      <c r="D29" s="10">
         <v>0.73099999999999998</v>
       </c>
-      <c r="E29" s="15">
+      <c r="E29" s="10">
         <v>0.73399999999999999</v>
       </c>
-      <c r="F29" s="15">
+      <c r="F29" s="10">
         <v>0.60199999999999998</v>
       </c>
-      <c r="G29" s="15">
+      <c r="G29" s="10">
         <v>0.188</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="10">
         <f t="shared" si="2"/>
         <v>0.41191822014802931</v>
       </c>
-      <c r="I29" s="15">
+      <c r="I29" s="10">
         <v>0.68</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="10">
         <v>0.68400000000000005</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="10">
         <v>0.54800000000000004</v>
       </c>
-      <c r="L29" s="15">
+      <c r="L29" s="10">
         <v>0.17699999999999999</v>
       </c>
-      <c r="M29" s="15">
+      <c r="M29" s="10">
         <f t="shared" si="3"/>
         <v>0.38435256242030275</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="15">
+        <v>47</v>
+      </c>
+      <c r="D30" s="10">
         <v>0.745</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="10">
         <v>0.747</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="10">
         <v>0.624</v>
       </c>
-      <c r="G30" s="15">
+      <c r="G30" s="10">
         <v>0.189</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H30" s="10">
         <f t="shared" si="2"/>
         <v>0.4177746678198106</v>
       </c>
-      <c r="I30" s="15">
+      <c r="I30" s="10">
         <v>0.70299999999999996</v>
       </c>
-      <c r="J30" s="15">
+      <c r="J30" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="K30" s="15">
+      <c r="K30" s="10">
         <v>0.57399999999999995</v>
       </c>
-      <c r="L30" s="15">
+      <c r="L30" s="10">
         <v>0.17899999999999999</v>
       </c>
-      <c r="M30" s="15">
+      <c r="M30" s="10">
         <f t="shared" si="3"/>
         <v>0.3934817884043173</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="15">
+        <v>48</v>
+      </c>
+      <c r="D31" s="10">
         <v>0.751</v>
       </c>
-      <c r="E31" s="15">
+      <c r="E31" s="10">
         <v>0.754</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="10">
         <v>0.63800000000000001</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G31" s="10">
         <v>0.187</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H31" s="10">
         <f t="shared" si="2"/>
         <v>0.41785015883037702</v>
       </c>
-      <c r="I31" s="15">
+      <c r="I31" s="10">
         <v>0.68700000000000006</v>
       </c>
-      <c r="J31" s="15">
+      <c r="J31" s="10">
         <v>0.69099999999999995</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="10">
         <v>0.55800000000000005</v>
       </c>
-      <c r="L31" s="15">
+      <c r="L31" s="10">
         <v>0.17399999999999999</v>
       </c>
-      <c r="M31" s="15">
+      <c r="M31" s="10">
         <f t="shared" si="3"/>
         <v>0.38306752621447526</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="15">
+        <v>49</v>
+      </c>
+      <c r="D32" s="10">
         <v>0.74299999999999999</v>
       </c>
-      <c r="E32" s="15">
+      <c r="E32" s="10">
         <v>0.747</v>
       </c>
-      <c r="F32" s="15">
+      <c r="F32" s="10">
         <v>0.626</v>
       </c>
-      <c r="G32" s="15">
+      <c r="G32" s="10">
         <v>0.185</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="10">
         <f t="shared" si="2"/>
         <v>0.4129060985363579</v>
       </c>
-      <c r="I32" s="15">
+      <c r="I32" s="10">
         <v>0.69599999999999995</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="10">
         <v>0.7</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="10">
         <v>0.57599999999999996</v>
       </c>
-      <c r="L32" s="15">
+      <c r="L32" s="10">
         <v>0.17599999999999999</v>
       </c>
-      <c r="M32" s="15">
+      <c r="M32" s="10">
         <f t="shared" si="3"/>
         <v>0.38898085955102052</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="15">
+        <v>50</v>
+      </c>
+      <c r="D33" s="10">
         <v>0.70699999999999996</v>
       </c>
-      <c r="E33" s="15">
+      <c r="E33" s="10">
         <v>0.71099999999999997</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="10">
         <v>0.58499999999999996</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="10">
         <v>0.18099999999999999</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="10">
         <f t="shared" si="2"/>
         <v>0.3978056837292761</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="10">
         <v>0.66900000000000004</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="10">
         <v>0.67300000000000004</v>
       </c>
-      <c r="K33" s="15">
+      <c r="K33" s="10">
         <v>0.54500000000000004</v>
       </c>
-      <c r="L33" s="15">
+      <c r="L33" s="10">
         <v>0.17100000000000001</v>
       </c>
-      <c r="M33" s="15">
+      <c r="M33" s="10">
         <f t="shared" si="3"/>
         <v>0.37511248637692057</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21" t="s">
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H35" s="15" t="s">
-        <v>59</v>
+      <c r="C35" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="13">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="E36" s="10">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="H36" s="10">
+        <v>0.79700000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="23"/>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="13">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="H37" s="10">
+        <v>0.60899999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="23"/>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="13">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.439</v>
+      </c>
+      <c r="E38" s="10">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="F38" s="10">
+        <v>0.155</v>
+      </c>
+      <c r="G38" s="10">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0.56100000000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="23"/>
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="13">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="F39" s="10">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="H39" s="10">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="23"/>
+      <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="18">
+      <c r="C40" s="13">
+        <v>0.151</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="F40" s="10">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0.36</v>
+      </c>
+      <c r="H40" s="10">
+        <v>0.621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="23"/>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="13">
+        <v>0.17199999999999999</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.434</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0.624</v>
+      </c>
+      <c r="F41" s="10">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="G41" s="10">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0.63300000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="23"/>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="13">
+        <v>0.183</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.35399999999999998</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0.68400000000000005</v>
+      </c>
+      <c r="F42" s="10">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G42" s="10">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="H42" s="10">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="23"/>
+      <c r="B43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="13">
+        <v>0.17</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="F43" s="10">
+        <v>0.155</v>
+      </c>
+      <c r="G43" s="10">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="H43" s="10">
+        <v>0.64600000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="23"/>
+      <c r="B44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="13">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.376</v>
+      </c>
+      <c r="E44" s="10">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="F44" s="10">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="G44" s="10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H44" s="10">
+        <v>0.60199999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="23"/>
+      <c r="B45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="13">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="E45" s="10">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="F45" s="10">
         <v>0.16900000000000001</v>
       </c>
-      <c r="D36" s="15">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="E36" s="15">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="F36" s="15">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="G36" s="15">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="H36" s="15">
-        <v>0.79700000000000004</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
-      <c r="B37" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="18">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="D37" s="15">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="E37" s="15">
-        <v>0.65700000000000003</v>
-      </c>
-      <c r="F37" s="15">
-        <v>0.14899999999999999</v>
-      </c>
-      <c r="G37" s="15">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="H37" s="15">
-        <v>0.60899999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C38" s="18">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="D38" s="15">
-        <v>0.439</v>
-      </c>
-      <c r="E38" s="15">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="F38" s="15">
-        <v>0.155</v>
-      </c>
-      <c r="G38" s="15">
-        <v>0.48399999999999999</v>
-      </c>
-      <c r="H38" s="15">
-        <v>0.56100000000000005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
-      <c r="B39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="18">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="D39" s="15">
-        <v>0.47099999999999997</v>
-      </c>
-      <c r="E39" s="15">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="F39" s="15">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="G39" s="15">
-        <v>0.39800000000000002</v>
-      </c>
-      <c r="H39" s="15">
-        <v>0.59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="18">
-        <v>0.151</v>
-      </c>
-      <c r="D40" s="15">
-        <v>0.38100000000000001</v>
-      </c>
-      <c r="E40" s="15">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="F40" s="15">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="G40" s="15">
-        <v>0.36</v>
-      </c>
-      <c r="H40" s="15">
-        <v>0.621</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
-      <c r="B41" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="18">
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="D41" s="15">
-        <v>0.434</v>
-      </c>
-      <c r="E41" s="15">
-        <v>0.624</v>
-      </c>
-      <c r="F41" s="15">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="G41" s="15">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="H41" s="15">
-        <v>0.63300000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="18">
-        <v>0.183</v>
-      </c>
-      <c r="D42" s="15">
-        <v>0.35399999999999998</v>
-      </c>
-      <c r="E42" s="15">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="F42" s="15">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="G42" s="15">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="H42" s="15">
-        <v>0.65400000000000003</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="21"/>
-      <c r="B43" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="18">
-        <v>0.17</v>
-      </c>
-      <c r="D43" s="15">
-        <v>0.39700000000000002</v>
-      </c>
-      <c r="E43" s="15">
-        <v>0.64</v>
-      </c>
-      <c r="F43" s="15">
-        <v>0.155</v>
-      </c>
-      <c r="G43" s="15">
-        <v>0.34399999999999997</v>
-      </c>
-      <c r="H43" s="15">
-        <v>0.64600000000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="18">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="D44" s="15">
-        <v>0.376</v>
-      </c>
-      <c r="E44" s="15">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="F44" s="15">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="G44" s="15">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H44" s="15">
-        <v>0.60199999999999998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="18">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="D45" s="15">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="E45" s="15">
-        <v>0.67200000000000004</v>
-      </c>
-      <c r="F45" s="15">
-        <v>0.16900000000000001</v>
-      </c>
-      <c r="G45" s="15">
+      <c r="G45" s="10">
         <v>0.32800000000000001</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H45" s="10">
         <v>0.68100000000000005</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A34:A45"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="I10:M10"/>
@@ -7924,9 +8302,6 @@
     <mergeCell ref="A22:A33"/>
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="I22:M22"/>
-    <mergeCell ref="A34:A45"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
more trials added, minor fix
fixed mean pooling logic in LSTM
</commit_message>
<xml_diff>
--- a/ModelPerformances.xlsx
+++ b/ModelPerformances.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nslonge/Documents/mit/year4/6806/final_proj_gh/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenhu/Desktop/whole1205/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="4220" windowWidth="21560" windowHeight="18280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2760" yWindow="1860" windowWidth="26260" windowHeight="18280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Task 1 Question Retrieval" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="73">
   <si>
     <t>CNN</t>
   </si>
@@ -246,6 +246,9 @@
   <si>
     <t>LSTM model#</t>
   </si>
+  <si>
+    <t>bidir</t>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +313,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +344,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -360,7 +369,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -416,7 +425,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -424,6 +432,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -435,6 +446,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -648,11 +660,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1916907568"/>
-        <c:axId val="-1862410688"/>
+        <c:axId val="1720742368"/>
+        <c:axId val="1720744416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1916907568"/>
+        <c:axId val="1720742368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,7 +706,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1862410688"/>
+        <c:crossAx val="1720744416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -702,7 +714,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1862410688"/>
+        <c:axId val="1720744416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916907568"/>
+        <c:crossAx val="1720742368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1025,11 +1037,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1862390544"/>
-        <c:axId val="-1917053376"/>
+        <c:axId val="1720768656"/>
+        <c:axId val="1720774704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1862390544"/>
+        <c:axId val="1720768656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1083,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1917053376"/>
+        <c:crossAx val="1720774704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1079,7 +1091,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1917053376"/>
+        <c:axId val="1720774704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,6 +1111,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1129,7 +1142,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1862390544"/>
+        <c:crossAx val="1720768656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2649,10 +2662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH96"/>
+  <dimension ref="A1:AH114"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="W57" workbookViewId="0">
-      <selection activeCell="AG73" sqref="AG73:AH73"/>
+    <sheetView tabSelected="1" topLeftCell="P76" workbookViewId="0">
+      <selection activeCell="AH93" sqref="AH93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5027,11 +5040,11 @@
       <c r="S67" s="1">
         <v>0.433</v>
       </c>
-      <c r="T67" s="6">
+      <c r="T67" s="7">
         <f>HARMEAN(L67:O67)</f>
         <v>0.5341466465864888</v>
       </c>
-      <c r="U67" s="6">
+      <c r="U67" s="7">
         <f t="shared" ref="U67:U68" si="2">HARMEAN(P67:S67)</f>
         <v>0.55869760966365589</v>
       </c>
@@ -5434,11 +5447,11 @@
       <c r="S75" s="1">
         <v>0.438</v>
       </c>
-      <c r="T75" s="6">
+      <c r="T75" s="7">
         <f t="shared" ref="T75:T76" si="8">HARMEAN(L75:O75)</f>
         <v>0.52869598003963159</v>
       </c>
-      <c r="U75" s="6">
+      <c r="U75" s="7">
         <f t="shared" ref="U75:U76" si="9">HARMEAN(P75:S75)</f>
         <v>0.54836378195331514</v>
       </c>
@@ -5606,7 +5619,7 @@
       <c r="T80" s="24"/>
       <c r="U80" s="24"/>
     </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L81" s="22"/>
       <c r="M81" s="22"/>
       <c r="N81" s="22"/>
@@ -5618,7 +5631,7 @@
       <c r="T81" s="22"/>
       <c r="U81" s="22"/>
     </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C82">
         <v>1</v>
       </c>
@@ -5670,19 +5683,19 @@
       <c r="S82" s="22">
         <v>0.442</v>
       </c>
-      <c r="T82" s="25">
+      <c r="T82" s="24">
         <f t="shared" ref="T82:T83" si="12">HARMEAN(L82:O82)</f>
         <v>0.53666887107867123</v>
       </c>
-      <c r="U82" s="25">
+      <c r="U82" s="24">
         <f t="shared" ref="U82:U83" si="13">HARMEAN(P82:S82)</f>
         <v>0.56166848396011737</v>
       </c>
-      <c r="V82" s="26" t="s">
+      <c r="V82" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>5</v>
       </c>
@@ -5746,7 +5759,7 @@
         <v>0.56789353356629468</v>
       </c>
     </row>
-    <row r="84" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L84" s="22"/>
       <c r="M84" s="22"/>
       <c r="N84" s="22"/>
@@ -5758,7 +5771,7 @@
       <c r="T84" s="24"/>
       <c r="U84" s="24"/>
     </row>
-    <row r="85" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C85">
         <v>1</v>
       </c>
@@ -5807,19 +5820,19 @@
       <c r="S85" s="22">
         <v>0.42399999999999999</v>
       </c>
-      <c r="T85" s="27">
+      <c r="T85" s="24">
         <f t="shared" ref="T85:T86" si="14">HARMEAN(L85:O85)</f>
         <v>0.54458264504852938</v>
       </c>
-      <c r="U85" s="27">
+      <c r="U85" s="24">
         <f t="shared" ref="U85:U86" si="15">HARMEAN(P85:S85)</f>
         <v>0.53959294309558425</v>
       </c>
-      <c r="V85" s="26" t="s">
+      <c r="V85" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B86">
         <v>6</v>
       </c>
@@ -5903,22 +5916,22 @@
       <c r="AD86" s="22">
         <v>0.17899999999999999</v>
       </c>
-      <c r="AE86" s="27">
+      <c r="AE86" s="26">
         <f t="shared" ref="AE86" si="16">HARMEAN(W86:Z86)</f>
         <v>0.41625672942842756</v>
       </c>
-      <c r="AF86" s="27">
+      <c r="AF86" s="26">
         <f t="shared" ref="AF86" si="17">HARMEAN(AA86:AD86)</f>
         <v>0.40380252565986385</v>
       </c>
-      <c r="AG86" s="28">
+      <c r="AG86" s="27">
         <v>0.51</v>
       </c>
-      <c r="AH86" s="28">
+      <c r="AH86" s="27">
         <v>0.499</v>
       </c>
     </row>
-    <row r="87" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L87" s="22"/>
       <c r="M87" s="22"/>
       <c r="N87" s="22"/>
@@ -5930,7 +5943,7 @@
       <c r="T87" s="24"/>
       <c r="U87" s="24"/>
     </row>
-    <row r="88" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C88">
         <v>2</v>
       </c>
@@ -5991,7 +6004,7 @@
         <v>0.51937760196054394</v>
       </c>
     </row>
-    <row r="89" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>7</v>
       </c>
@@ -6093,23 +6106,29 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="90" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="T90" s="7"/>
       <c r="U90" s="7"/>
     </row>
-    <row r="91" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>72</v>
+      </c>
       <c r="C91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>240</v>
       </c>
       <c r="E91">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F91">
         <v>0.01</v>
       </c>
+      <c r="G91">
+        <v>8</v>
+      </c>
       <c r="H91">
         <v>20</v>
       </c>
@@ -6119,35 +6138,57 @@
       <c r="J91" t="s">
         <v>26</v>
       </c>
-      <c r="L91" s="22"/>
-      <c r="M91" s="22"/>
-      <c r="N91" s="22"/>
-      <c r="O91" s="22"/>
-      <c r="P91" s="22"/>
-      <c r="Q91" s="22"/>
-      <c r="R91" s="22"/>
-      <c r="S91" s="22"/>
-      <c r="T91" s="24" t="e">
+      <c r="K91" s="2">
+        <v>1.15E-3</v>
+      </c>
+      <c r="L91" s="22">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="M91" s="22">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="N91" s="22">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="O91" s="22">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="P91" s="22">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="Q91" s="22">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="R91" s="22">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S91" s="22">
+        <v>0.439</v>
+      </c>
+      <c r="T91" s="24">
         <f t="shared" ref="T91:T92" si="22">HARMEAN(L91:O91)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U91" s="24" t="e">
+        <v>0.56430390558359023</v>
+      </c>
+      <c r="U91" s="24">
         <f t="shared" ref="U91:U92" si="23">HARMEAN(P91:S91)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="2:34" x14ac:dyDescent="0.2">
+        <v>0.5431625594807501</v>
+      </c>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>72</v>
+      </c>
       <c r="B92">
         <v>8</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>240</v>
       </c>
       <c r="E92">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F92">
         <v>0.01</v>
@@ -6164,69 +6205,992 @@
       <c r="J92" t="s">
         <v>26</v>
       </c>
-      <c r="L92" s="22"/>
-      <c r="M92" s="22"/>
-      <c r="N92" s="22"/>
-      <c r="O92" s="22"/>
-      <c r="P92" s="22"/>
-      <c r="Q92" s="22"/>
-      <c r="R92" s="22"/>
-      <c r="S92" s="22"/>
-      <c r="T92" s="24" t="e">
+      <c r="K92" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="L92" s="22">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="M92" s="22">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="N92" s="22">
+        <v>0.624</v>
+      </c>
+      <c r="O92" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="P92" s="22">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="Q92" s="22">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="R92" s="22">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="S92" s="22">
+        <v>0.44</v>
+      </c>
+      <c r="T92" s="34">
         <f t="shared" si="22"/>
+        <v>0.57773044238217408</v>
+      </c>
+      <c r="U92" s="34">
+        <f t="shared" si="23"/>
+        <v>0.54739550893922295</v>
+      </c>
+      <c r="W92" s="1">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="X92" s="1">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="Y92" s="1">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="Z92" s="1">
+        <v>0.189</v>
+      </c>
+      <c r="AA92" s="1">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="AB92" s="1">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AC92" s="1">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="AD92" s="1">
+        <v>0.185</v>
+      </c>
+      <c r="AE92" s="6">
+        <f t="shared" ref="AE92" si="24">HARMEAN(W92:Z92)</f>
+        <v>0.4257571213174961</v>
+      </c>
+      <c r="AF92" s="6">
+        <f t="shared" ref="AF92" si="25">HARMEAN(AA92:AD92)</f>
+        <v>0.42153062298529126</v>
+      </c>
+      <c r="AG92" s="23">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="AH92" s="23">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L93" s="22"/>
+      <c r="M93" s="22"/>
+      <c r="N93" s="22"/>
+      <c r="O93" s="22"/>
+      <c r="P93" s="22"/>
+      <c r="Q93" s="22"/>
+      <c r="R93" s="22"/>
+      <c r="S93" s="22"/>
+      <c r="T93" s="24"/>
+      <c r="U93" s="24"/>
+    </row>
+    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>72</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>240</v>
+      </c>
+      <c r="E94">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F94">
+        <v>0.01</v>
+      </c>
+      <c r="G94">
+        <v>9</v>
+      </c>
+      <c r="H94">
+        <v>20</v>
+      </c>
+      <c r="I94">
+        <v>300</v>
+      </c>
+      <c r="J94" t="s">
+        <v>26</v>
+      </c>
+      <c r="K94" s="2">
+        <v>1.48E-3</v>
+      </c>
+      <c r="L94" s="22">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="M94" s="22">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="N94" s="22">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="O94" s="22">
+        <v>0.443</v>
+      </c>
+      <c r="P94" s="22">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="Q94" s="22">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="R94" s="22">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="S94" s="22">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T94" s="24">
+        <f t="shared" ref="T94:T95" si="26">HARMEAN(L94:O94)</f>
+        <v>0.55753469811401624</v>
+      </c>
+      <c r="U94" s="24">
+        <f t="shared" ref="U94:U95" si="27">HARMEAN(P94:S94)</f>
+        <v>0.55737598191173199</v>
+      </c>
+      <c r="W94" s="1">
+        <v>0.754</v>
+      </c>
+      <c r="X94" s="1">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="Y94" s="1">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="Z94" s="1">
+        <v>0.186</v>
+      </c>
+      <c r="AA94" s="1">
+        <v>0.746</v>
+      </c>
+      <c r="AB94" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="AC94" s="1">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AD94" s="1">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="AE94" s="6">
+        <f t="shared" ref="AE94" si="28">HARMEAN(W94:Z94)</f>
+        <v>0.41888417502506126</v>
+      </c>
+      <c r="AF94" s="6">
+        <f t="shared" ref="AF94" si="29">HARMEAN(AA94:AD94)</f>
+        <v>0.40746607508208299</v>
+      </c>
+      <c r="AG94" s="23">
+        <v>0.497</v>
+      </c>
+      <c r="AH94" s="23">
+        <v>0.50900000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>72</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>240</v>
+      </c>
+      <c r="E95">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F95">
+        <v>0.01</v>
+      </c>
+      <c r="G95">
+        <v>10</v>
+      </c>
+      <c r="H95">
+        <v>20</v>
+      </c>
+      <c r="I95">
+        <v>300</v>
+      </c>
+      <c r="J95" t="s">
+        <v>26</v>
+      </c>
+      <c r="K95" s="2">
+        <v>1.17E-3</v>
+      </c>
+      <c r="L95" s="22">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="M95" s="22">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="N95" s="22">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="O95" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="P95" s="22">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="Q95" s="22">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="R95" s="22">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="S95" s="22">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T95" s="24">
+        <f t="shared" si="26"/>
+        <v>0.561119591277767</v>
+      </c>
+      <c r="U95" s="24">
+        <f t="shared" si="27"/>
+        <v>0.55152226399181714</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T96" s="7"/>
+      <c r="U96" s="7"/>
+    </row>
+    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>72</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>240</v>
+      </c>
+      <c r="E97">
+        <v>1E-3</v>
+      </c>
+      <c r="F97">
+        <v>0.01</v>
+      </c>
+      <c r="G97">
+        <v>8</v>
+      </c>
+      <c r="H97">
+        <v>20</v>
+      </c>
+      <c r="I97">
+        <v>300</v>
+      </c>
+      <c r="J97" t="s">
+        <v>27</v>
+      </c>
+      <c r="K97" s="2">
+        <v>1.56E-3</v>
+      </c>
+      <c r="L97" s="22">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="M97" s="22">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N97" s="22">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="O97" s="22">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="P97" s="22">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="Q97" s="22">
+        <v>0.68</v>
+      </c>
+      <c r="R97" s="22">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S97" s="22">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="T97" s="24">
+        <f t="shared" ref="T97:T98" si="30">HARMEAN(L97:O97)</f>
+        <v>0.56947548393464664</v>
+      </c>
+      <c r="U97" s="24">
+        <f t="shared" ref="U97:U98" si="31">HARMEAN(P97:S97)</f>
+        <v>0.53028156876269039</v>
+      </c>
+    </row>
+    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>240</v>
+      </c>
+      <c r="E98">
+        <v>1E-3</v>
+      </c>
+      <c r="F98">
+        <v>0.01</v>
+      </c>
+      <c r="G98">
+        <v>10</v>
+      </c>
+      <c r="H98">
+        <v>20</v>
+      </c>
+      <c r="I98">
+        <v>300</v>
+      </c>
+      <c r="J98" t="s">
+        <v>27</v>
+      </c>
+      <c r="K98" s="2">
+        <v>1.07E-3</v>
+      </c>
+      <c r="L98" s="22">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M98" s="22">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="N98" s="22">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="O98" s="22">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="P98" s="22">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="Q98" s="22">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="R98" s="22">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="S98" s="22">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="T98" s="24">
+        <f t="shared" si="30"/>
+        <v>0.56611714570412963</v>
+      </c>
+      <c r="U98" s="24">
+        <f t="shared" si="31"/>
+        <v>0.54491010137918205</v>
+      </c>
+      <c r="W98" s="1">
+        <v>0.74400000000000011</v>
+      </c>
+      <c r="X98" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="Y98" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="Z98" s="1">
+        <v>0.187</v>
+      </c>
+      <c r="AA98" s="1">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="AB98" s="1">
+        <v>0.74400000000000011</v>
+      </c>
+      <c r="AC98" s="1">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AD98" s="1">
+        <v>0.17800000000000002</v>
+      </c>
+      <c r="AE98" s="1">
+        <f t="shared" ref="AE98" si="32">HARMEAN(W98:Z98)</f>
+        <v>0.41608743594148978</v>
+      </c>
+      <c r="AF98" s="1">
+        <f t="shared" ref="AF98" si="33">HARMEAN(AA98:AD98)</f>
+        <v>0.40549912587160197</v>
+      </c>
+      <c r="AG98" s="23">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="AH98" s="23">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>240</v>
+      </c>
+      <c r="E99">
+        <v>1E-3</v>
+      </c>
+      <c r="F99">
+        <v>0.01</v>
+      </c>
+      <c r="G99">
+        <v>15</v>
+      </c>
+      <c r="H99">
+        <v>20</v>
+      </c>
+      <c r="I99">
+        <v>300</v>
+      </c>
+      <c r="J99" t="s">
+        <v>27</v>
+      </c>
+      <c r="K99" s="2">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="L99" s="22">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="M99" s="22">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="N99" s="22">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="O99" s="22">
+        <v>0.442</v>
+      </c>
+      <c r="P99" s="22">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="Q99" s="22">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="R99" s="22">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S99" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="T99" s="24">
+        <f t="shared" ref="T99" si="34">HARMEAN(L99:O99)</f>
+        <v>0.55568844615019009</v>
+      </c>
+      <c r="U99" s="24">
+        <f t="shared" ref="U99" si="35">HARMEAN(P99:S99)</f>
+        <v>0.53255096258067558</v>
+      </c>
+    </row>
+    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T100" s="7"/>
+      <c r="U100" s="7"/>
+    </row>
+    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>72</v>
+      </c>
+      <c r="B101">
+        <v>11</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>240</v>
+      </c>
+      <c r="E101">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F101">
+        <v>0.01</v>
+      </c>
+      <c r="G101">
+        <v>15</v>
+      </c>
+      <c r="H101">
+        <v>20</v>
+      </c>
+      <c r="I101">
+        <v>200</v>
+      </c>
+      <c r="J101" t="s">
+        <v>26</v>
+      </c>
+      <c r="L101" s="22"/>
+      <c r="M101" s="22"/>
+      <c r="N101" s="22"/>
+      <c r="O101" s="22"/>
+      <c r="P101" s="22"/>
+      <c r="Q101" s="22"/>
+      <c r="R101" s="22"/>
+      <c r="S101" s="22"/>
+      <c r="T101" s="24" t="e">
+        <f t="shared" ref="T101:T102" si="36">HARMEAN(L101:O101)</f>
         <v>#N/A</v>
       </c>
-      <c r="U92" s="24" t="e">
-        <f t="shared" si="23"/>
+      <c r="U101" s="24" t="e">
+        <f t="shared" ref="U101:U102" si="37">HARMEAN(P101:S101)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="93" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="T93" s="7"/>
-      <c r="U93" s="7"/>
-    </row>
-    <row r="94" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="T94" s="7"/>
-      <c r="U94" s="7"/>
-    </row>
-    <row r="95" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="T95" s="7"/>
-      <c r="U95" s="7"/>
-    </row>
-    <row r="96" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
+      <c r="V101" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>72</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>240</v>
+      </c>
+      <c r="E102">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F102">
+        <v>0.01</v>
+      </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
+      <c r="H102">
+        <v>20</v>
+      </c>
+      <c r="I102">
+        <v>200</v>
+      </c>
+      <c r="J102" t="s">
+        <v>26</v>
+      </c>
+      <c r="L102" s="22"/>
+      <c r="M102" s="22"/>
+      <c r="N102" s="22"/>
+      <c r="O102" s="22"/>
+      <c r="P102" s="22"/>
+      <c r="Q102" s="22"/>
+      <c r="R102" s="22"/>
+      <c r="S102" s="22"/>
+      <c r="T102" s="24" t="e">
+        <f t="shared" si="36"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U102" s="24" t="e">
+        <f t="shared" si="37"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W102" s="22"/>
+      <c r="X102" s="22"/>
+      <c r="Y102" s="22"/>
+      <c r="Z102" s="22"/>
+      <c r="AA102" s="22"/>
+      <c r="AB102" s="22"/>
+      <c r="AC102" s="22"/>
+      <c r="AD102" s="22"/>
+      <c r="AE102" s="26"/>
+      <c r="AF102" s="26"/>
+      <c r="AG102" s="27"/>
+      <c r="AH102" s="27"/>
+    </row>
+    <row r="103" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L103" s="22"/>
+      <c r="M103" s="22"/>
+      <c r="N103" s="22"/>
+      <c r="O103" s="22"/>
+      <c r="P103" s="22"/>
+      <c r="Q103" s="22"/>
+      <c r="R103" s="22"/>
+      <c r="S103" s="22"/>
+      <c r="T103" s="24"/>
+      <c r="U103" s="24"/>
+    </row>
+    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>72</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>240</v>
+      </c>
+      <c r="E104">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F104">
+        <v>0.01</v>
+      </c>
+      <c r="G104">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>20</v>
+      </c>
+      <c r="I104">
+        <v>200</v>
+      </c>
+      <c r="J104" t="s">
+        <v>26</v>
+      </c>
+      <c r="L104" s="22"/>
+      <c r="M104" s="22"/>
+      <c r="N104" s="22"/>
+      <c r="O104" s="22"/>
+      <c r="P104" s="22"/>
+      <c r="Q104" s="22"/>
+      <c r="R104" s="22"/>
+      <c r="S104" s="22"/>
+      <c r="T104" s="24" t="e">
+        <f t="shared" ref="T104:T105" si="38">HARMEAN(L104:O104)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U104" s="24" t="e">
+        <f t="shared" ref="U104:U105" si="39">HARMEAN(P104:S104)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>240</v>
+      </c>
+      <c r="E105">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F105">
+        <v>0.01</v>
+      </c>
+      <c r="G105">
+        <v>5</v>
+      </c>
+      <c r="H105">
+        <v>20</v>
+      </c>
+      <c r="I105">
+        <v>200</v>
+      </c>
+      <c r="J105" t="s">
+        <v>26</v>
+      </c>
+      <c r="L105" s="22"/>
+      <c r="M105" s="22"/>
+      <c r="N105" s="22"/>
+      <c r="O105" s="22"/>
+      <c r="P105" s="22"/>
+      <c r="Q105" s="22"/>
+      <c r="R105" s="22"/>
+      <c r="S105" s="22"/>
+      <c r="T105" s="24" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U105" s="24" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+      <c r="Z105" s="1"/>
+      <c r="AA105" s="1"/>
+      <c r="AB105" s="1"/>
+      <c r="AC105" s="1"/>
+      <c r="AD105" s="1"/>
+      <c r="AE105" s="6"/>
+      <c r="AF105" s="6"/>
+      <c r="AG105" s="23"/>
+      <c r="AH105" s="23"/>
+    </row>
+    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T106" s="7"/>
+      <c r="U106" s="7"/>
+    </row>
+    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>72</v>
+      </c>
+      <c r="B107">
+        <v>13</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>240</v>
+      </c>
+      <c r="E107">
+        <v>1E-3</v>
+      </c>
+      <c r="F107">
+        <v>0.01</v>
+      </c>
+      <c r="G107">
+        <v>8</v>
+      </c>
+      <c r="H107">
+        <v>20</v>
+      </c>
+      <c r="I107">
+        <v>200</v>
+      </c>
+      <c r="J107" t="s">
+        <v>27</v>
+      </c>
+      <c r="L107" s="22"/>
+      <c r="M107" s="22"/>
+      <c r="N107" s="22"/>
+      <c r="O107" s="22"/>
+      <c r="P107" s="22"/>
+      <c r="Q107" s="22"/>
+      <c r="R107" s="22"/>
+      <c r="S107" s="22"/>
+      <c r="T107" s="24" t="e">
+        <f t="shared" ref="T107:T108" si="40">HARMEAN(L107:O107)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U107" s="24" t="e">
+        <f t="shared" ref="U107:U108" si="41">HARMEAN(P107:S107)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>72</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>240</v>
+      </c>
+      <c r="E108">
+        <v>1E-3</v>
+      </c>
+      <c r="F108">
+        <v>0.01</v>
+      </c>
+      <c r="G108">
+        <v>10</v>
+      </c>
+      <c r="H108">
+        <v>20</v>
+      </c>
+      <c r="I108">
+        <v>200</v>
+      </c>
+      <c r="J108" t="s">
+        <v>27</v>
+      </c>
+      <c r="L108" s="22"/>
+      <c r="M108" s="22"/>
+      <c r="N108" s="22"/>
+      <c r="O108" s="22"/>
+      <c r="P108" s="22"/>
+      <c r="Q108" s="22"/>
+      <c r="R108" s="22"/>
+      <c r="S108" s="22"/>
+      <c r="T108" s="34" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U108" s="34" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W108" s="22"/>
+      <c r="X108" s="22"/>
+      <c r="Y108" s="22"/>
+      <c r="Z108" s="22"/>
+      <c r="AA108" s="22"/>
+      <c r="AB108" s="22"/>
+      <c r="AC108" s="22"/>
+      <c r="AD108" s="22"/>
+      <c r="AE108" s="26"/>
+      <c r="AF108" s="26"/>
+      <c r="AG108" s="27"/>
+      <c r="AH108" s="27"/>
+    </row>
+    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L109" s="22"/>
+      <c r="M109" s="22"/>
+      <c r="N109" s="22"/>
+      <c r="O109" s="22"/>
+      <c r="P109" s="22"/>
+      <c r="Q109" s="22"/>
+      <c r="R109" s="22"/>
+      <c r="S109" s="22"/>
+      <c r="T109" s="24"/>
+      <c r="U109" s="24"/>
+    </row>
+    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>72</v>
+      </c>
+      <c r="B110">
+        <v>14</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>240</v>
+      </c>
+      <c r="E110">
+        <v>1E-3</v>
+      </c>
+      <c r="F110">
+        <v>0.01</v>
+      </c>
+      <c r="H110">
+        <v>20</v>
+      </c>
+      <c r="I110">
+        <v>200</v>
+      </c>
+      <c r="J110" t="s">
+        <v>27</v>
+      </c>
+      <c r="L110" s="22"/>
+      <c r="M110" s="22"/>
+      <c r="N110" s="22"/>
+      <c r="O110" s="22"/>
+      <c r="P110" s="22"/>
+      <c r="Q110" s="22"/>
+      <c r="R110" s="22"/>
+      <c r="S110" s="22"/>
+      <c r="T110" s="24" t="e">
+        <f t="shared" ref="T110:T111" si="42">HARMEAN(L110:O110)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U110" s="24" t="e">
+        <f t="shared" ref="U110:U111" si="43">HARMEAN(P110:S110)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>72</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>240</v>
+      </c>
+      <c r="E111">
+        <v>1E-3</v>
+      </c>
+      <c r="F111">
+        <v>0.01</v>
+      </c>
+      <c r="G111">
+        <v>10</v>
+      </c>
+      <c r="H111">
+        <v>20</v>
+      </c>
+      <c r="I111">
+        <v>200</v>
+      </c>
+      <c r="J111" t="s">
+        <v>27</v>
+      </c>
+      <c r="L111" s="22"/>
+      <c r="M111" s="22"/>
+      <c r="N111" s="22"/>
+      <c r="O111" s="22"/>
+      <c r="P111" s="22"/>
+      <c r="Q111" s="22"/>
+      <c r="R111" s="22"/>
+      <c r="S111" s="22"/>
+      <c r="T111" s="24" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U111" s="24" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W111" s="1"/>
+      <c r="X111" s="1"/>
+      <c r="Y111" s="1"/>
+      <c r="Z111" s="1"/>
+      <c r="AA111" s="1"/>
+      <c r="AB111" s="1"/>
+      <c r="AC111" s="1"/>
+      <c r="AD111" s="1"/>
+      <c r="AE111" s="6"/>
+      <c r="AF111" s="6"/>
+      <c r="AG111" s="23"/>
+      <c r="AH111" s="23"/>
+    </row>
+    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T112" s="7"/>
+      <c r="U112" s="7"/>
+    </row>
+    <row r="113" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T113" s="7"/>
+      <c r="U113" s="7"/>
+    </row>
+    <row r="114" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
         <v>23</v>
       </c>
-      <c r="L96" s="1">
+      <c r="L114" s="1">
         <v>0.58399999999999996</v>
       </c>
-      <c r="M96" s="1">
+      <c r="M114" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="N96" s="1">
+      <c r="N114" s="1">
         <v>0.6</v>
       </c>
-      <c r="O96" s="1">
+      <c r="O114" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="P96" s="1">
+      <c r="P114" s="1">
         <v>0.56799999999999995</v>
       </c>
-      <c r="Q96" s="1">
+      <c r="Q114" s="1">
         <v>0.70099999999999996</v>
       </c>
-      <c r="R96" s="1">
+      <c r="R114" s="1">
         <v>0.55800000000000005</v>
       </c>
-      <c r="S96" s="1">
+      <c r="S114" s="1">
         <v>0.432</v>
       </c>
-      <c r="T96" s="6">
-        <f t="shared" ref="T96" si="24">HARMEAN(L96:O96)</f>
+      <c r="T114" s="6">
+        <f t="shared" ref="T114" si="44">HARMEAN(L114:O114)</f>
         <v>0.57826082952638469</v>
       </c>
-      <c r="U96" s="6">
-        <f t="shared" ref="U96" si="25">HARMEAN(P96:S96)</f>
+      <c r="U114" s="6">
+        <f t="shared" ref="U114" si="45">HARMEAN(P114:S114)</f>
         <v>0.54839395595501261</v>
       </c>
     </row>
@@ -6245,20 +7209,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10.83203125" style="15"/>
+    <col min="3" max="6" width="10.83203125" style="15"/>
+    <col min="7" max="12" width="10.83203125" style="30"/>
+    <col min="13" max="14" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>71</v>
       </c>
@@ -6271,11 +7237,24 @@
       <c r="E1" s="15">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="F1" s="15">
+        <v>10</v>
+      </c>
+      <c r="G1">
+        <v>9</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>31</v>
       </c>
@@ -6291,38 +7270,33 @@
       <c r="E2" s="15">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="O2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="21">
+      <c r="P2" s="21">
         <v>1E-3</v>
       </c>
-      <c r="K2" s="21">
+      <c r="Q2" s="21">
         <v>1E-3</v>
       </c>
-      <c r="L2" s="21">
+      <c r="R2" s="21">
         <v>1E-3</v>
       </c>
-      <c r="M2" s="21">
+      <c r="S2" s="21">
         <v>1E-3</v>
-      </c>
-      <c r="N2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="O2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="P2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="Q2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="R2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="S2" s="21">
-        <v>0.01</v>
       </c>
       <c r="T2" s="21">
         <v>0.01</v>
@@ -6345,8 +7319,26 @@
       <c r="Z2" s="21">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AB2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AC2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AD2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AE2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AF2" s="21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" s="32"/>
       <c r="B3" t="s">
         <v>15</v>
@@ -6360,25 +7352,20 @@
       <c r="E3" s="15">
         <v>240</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="21">
-        <v>2</v>
-      </c>
-      <c r="K3" s="21">
-        <v>2</v>
-      </c>
-      <c r="L3" s="21">
-        <v>2</v>
-      </c>
-      <c r="M3" s="21">
-        <v>3</v>
-      </c>
-      <c r="N3" s="21">
-        <v>2</v>
-      </c>
-      <c r="O3" s="21">
+      <c r="F3">
+        <v>240</v>
+      </c>
+      <c r="G3">
+        <v>240</v>
+      </c>
+      <c r="H3">
+        <v>240</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="O3" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="21">
@@ -6391,13 +7378,13 @@
         <v>2</v>
       </c>
       <c r="S3" s="21">
-        <v>4</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>63</v>
+        <v>3</v>
+      </c>
+      <c r="T3" s="21">
+        <v>2</v>
       </c>
       <c r="U3" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V3" s="21">
         <v>2</v>
@@ -6409,13 +7396,31 @@
         <v>2</v>
       </c>
       <c r="Y3" s="21">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA3" s="21">
         <v>2</v>
       </c>
-      <c r="Z3" s="21">
+      <c r="AB3" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AC3" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="21">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="21">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" s="32"/>
       <c r="B4" t="s">
         <v>7</v>
@@ -6429,26 +7434,21 @@
       <c r="E4" s="15">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="F4">
+        <v>1E-3</v>
+      </c>
+      <c r="G4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H4">
+        <v>1E-3</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="O4" t="s">
         <v>5</v>
-      </c>
-      <c r="J4" s="21">
-        <v>200</v>
-      </c>
-      <c r="K4" s="21">
-        <v>200</v>
-      </c>
-      <c r="L4" s="21">
-        <v>200</v>
-      </c>
-      <c r="M4" s="21">
-        <v>200</v>
-      </c>
-      <c r="N4" s="21">
-        <v>200</v>
-      </c>
-      <c r="O4" s="21">
-        <v>200</v>
       </c>
       <c r="P4" s="21">
         <v>200</v>
@@ -6457,7 +7457,7 @@
         <v>200</v>
       </c>
       <c r="R4" s="21">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S4" s="21">
         <v>200</v>
@@ -6469,22 +7469,40 @@
         <v>200</v>
       </c>
       <c r="V4" s="21">
+        <v>200</v>
+      </c>
+      <c r="W4" s="21">
+        <v>200</v>
+      </c>
+      <c r="X4" s="21">
         <v>100</v>
       </c>
-      <c r="W4" s="21">
+      <c r="Y4" s="21">
+        <v>200</v>
+      </c>
+      <c r="Z4" s="21">
+        <v>200</v>
+      </c>
+      <c r="AA4" s="21">
+        <v>200</v>
+      </c>
+      <c r="AB4" s="21">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="21">
         <v>400</v>
       </c>
-      <c r="X4" s="21">
+      <c r="AD4" s="21">
         <v>400</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="AE4" s="21">
         <v>300</v>
       </c>
-      <c r="Z4" s="21">
+      <c r="AF4" s="21">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" s="32"/>
       <c r="B5" t="s">
         <v>8</v>
@@ -6498,44 +7516,39 @@
       <c r="E5" s="15">
         <v>0.01</v>
       </c>
-      <c r="I5" t="s">
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <v>0.01</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="O5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21">
+      <c r="P5" s="21">
         <v>1E-3</v>
       </c>
-      <c r="K5" s="21">
+      <c r="Q5" s="21">
         <v>0.01</v>
       </c>
-      <c r="L5" s="21">
+      <c r="R5" s="21">
         <v>0.01</v>
       </c>
-      <c r="M5" s="21">
+      <c r="S5" s="21">
         <v>0.01</v>
       </c>
-      <c r="N5" s="21">
+      <c r="T5" s="21">
         <v>0.01</v>
       </c>
-      <c r="O5" s="21">
+      <c r="U5" s="21">
         <v>0.01</v>
-      </c>
-      <c r="P5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="R5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="S5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="T5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="U5" s="21">
-        <v>0.1</v>
       </c>
       <c r="V5" s="21">
         <v>0.1</v>
@@ -6552,8 +7565,26 @@
       <c r="Z5" s="21">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AB5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AC5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AD5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AE5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AF5" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" s="32"/>
       <c r="B6" t="s">
         <v>6</v>
@@ -6567,56 +7598,69 @@
       <c r="E6" s="15">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="O6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="21">
+      <c r="P6" s="21">
         <v>8</v>
       </c>
-      <c r="K6" s="21">
+      <c r="Q6" s="21">
         <v>9</v>
       </c>
-      <c r="L6" s="21">
+      <c r="R6" s="21">
         <v>8</v>
       </c>
-      <c r="M6" s="21">
+      <c r="S6" s="21">
         <v>9</v>
       </c>
-      <c r="N6" s="21">
+      <c r="T6" s="21">
         <v>9</v>
       </c>
-      <c r="O6" s="21">
+      <c r="U6" s="21">
         <v>19</v>
       </c>
-      <c r="P6" s="21">
+      <c r="V6" s="21">
         <v>5</v>
       </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21">
+      <c r="W6" s="21"/>
+      <c r="X6" s="21">
         <v>5</v>
       </c>
-      <c r="S6" s="21">
+      <c r="Y6" s="21">
         <v>3</v>
       </c>
-      <c r="T6" s="21">
+      <c r="Z6" s="21">
         <v>7</v>
       </c>
-      <c r="U6" s="21">
+      <c r="AA6" s="21">
         <v>4</v>
       </c>
-      <c r="V6" s="21">
+      <c r="AB6" s="21">
         <v>4</v>
       </c>
-      <c r="W6" s="21">
+      <c r="AC6" s="21">
         <v>7</v>
       </c>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21">
+      <c r="AD6" s="21"/>
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" s="32"/>
       <c r="B7" t="s">
         <v>25</v>
@@ -6630,32 +7674,27 @@
       <c r="E7" s="15">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="O7" t="s">
         <v>56</v>
-      </c>
-      <c r="J7" s="21">
-        <v>20</v>
-      </c>
-      <c r="K7" s="21">
-        <v>20</v>
-      </c>
-      <c r="L7" s="21">
-        <v>20</v>
-      </c>
-      <c r="M7" s="21">
-        <v>20</v>
-      </c>
-      <c r="N7" s="21">
-        <v>20</v>
-      </c>
-      <c r="O7" s="21">
-        <v>20</v>
       </c>
       <c r="P7" s="21">
         <v>20</v>
       </c>
       <c r="Q7" s="21">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R7" s="21">
         <v>20</v>
@@ -6673,19 +7712,37 @@
         <v>20</v>
       </c>
       <c r="W7" s="21">
+        <v>35</v>
+      </c>
+      <c r="X7" s="21">
         <v>20</v>
       </c>
-      <c r="X7" s="21">
-        <v>35</v>
-      </c>
       <c r="Y7" s="21">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="Z7" s="21">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA7" s="21">
+        <v>20</v>
+      </c>
+      <c r="AB7" s="21">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="21">
+        <v>20</v>
+      </c>
+      <c r="AD7" s="21">
+        <v>35</v>
+      </c>
+      <c r="AE7" s="21">
+        <v>35</v>
+      </c>
+      <c r="AF7" s="21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" s="32"/>
       <c r="B8" t="s">
         <v>28</v>
@@ -6699,26 +7756,21 @@
       <c r="E8" s="15">
         <v>300</v>
       </c>
-      <c r="I8" t="s">
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <v>300</v>
+      </c>
+      <c r="H8">
+        <v>300</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="O8" t="s">
         <v>28</v>
-      </c>
-      <c r="J8" s="21">
-        <v>300</v>
-      </c>
-      <c r="K8" s="21">
-        <v>300</v>
-      </c>
-      <c r="L8" s="21">
-        <v>300</v>
-      </c>
-      <c r="M8" s="21">
-        <v>300</v>
-      </c>
-      <c r="N8" s="21">
-        <v>300</v>
-      </c>
-      <c r="O8" s="21">
-        <v>300</v>
       </c>
       <c r="P8" s="21">
         <v>300</v>
@@ -6753,8 +7805,26 @@
       <c r="Z8" s="21">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="AA8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AB8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AC8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AD8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AE8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AF8" s="21">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" s="32"/>
       <c r="B9" t="s">
         <v>24</v>
@@ -6768,26 +7838,21 @@
       <c r="E9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I9" t="s">
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="O9" t="s">
         <v>24</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="21" t="s">
-        <v>27</v>
       </c>
       <c r="P9" s="21" t="s">
         <v>27</v>
@@ -6796,34 +7861,52 @@
         <v>27</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="T9" s="21" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="X9" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="21" t="s">
+      <c r="AB9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="W9" s="21" t="s">
+      <c r="AC9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="X9" s="21" t="s">
+      <c r="AD9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="Y9" s="21" t="s">
+      <c r="AE9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="Z9" s="21" t="s">
+      <c r="AF9" s="21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>32</v>
       </c>
@@ -6831,279 +7914,327 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A11" s="32"/>
       <c r="B11" s="1"/>
       <c r="C11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J11" t="s">
+      <c r="P11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A12" s="32"/>
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28">
         <v>7.6100000000000001E-2</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17" t="s">
+      <c r="F12" s="28">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0.1053</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0.1042</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="20">
+      <c r="P12" s="20">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="K12" s="20">
+      <c r="Q12" s="20">
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="L12" s="20">
+      <c r="R12" s="20">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="M12" s="20">
+      <c r="S12" s="20">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="N12" s="20">
+      <c r="T12" s="20">
         <v>8.1299999999999997E-2</v>
       </c>
-      <c r="O12" s="20">
+      <c r="U12" s="20">
         <v>8.0699999999999994E-2</v>
       </c>
-      <c r="P12" s="19">
+      <c r="V12" s="19">
         <v>8.1100000000000005E-2</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="W12" s="20">
         <v>8.2799999999999999E-2</v>
       </c>
-      <c r="R12" s="20">
+      <c r="X12" s="20">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="S12" s="20">
+      <c r="Y12" s="20">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="T12" s="19">
+      <c r="Z12" s="19">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="U12" s="19">
+      <c r="AA12" s="19">
         <v>0.10100000000000001</v>
       </c>
-      <c r="V12" s="19">
+      <c r="AB12" s="19">
         <v>7.8E-2</v>
       </c>
-      <c r="W12" s="19">
+      <c r="AC12" s="19">
         <v>9.01E-2</v>
       </c>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19">
+      <c r="AD12" s="19"/>
+      <c r="AE12" s="19"/>
+      <c r="AF12" s="19">
         <v>9.1499999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A13" s="32"/>
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="18" t="s">
+      <c r="F13" s="28">
+        <v>9.11E-2</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="H13" s="28">
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="19">
+      <c r="P13" s="19">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K13" s="19">
+      <c r="Q13" s="19">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="L13" s="19">
+      <c r="R13" s="19">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="M13" s="19">
+      <c r="S13" s="19">
         <v>6.83E-2</v>
       </c>
-      <c r="N13" s="19">
+      <c r="T13" s="19">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="O13" s="19">
+      <c r="U13" s="19">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="P13" s="19">
+      <c r="V13" s="19">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="W13" s="19">
         <v>7.4700000000000003E-2</v>
       </c>
-      <c r="R13" s="19">
+      <c r="X13" s="19">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="S13" s="19">
+      <c r="Y13" s="19">
         <v>6.08E-2</v>
       </c>
-      <c r="T13" s="19">
+      <c r="Z13" s="19">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="U13" s="19">
+      <c r="AA13" s="19">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="V13" s="19">
+      <c r="AB13" s="19">
         <v>8.3699999999999997E-2</v>
       </c>
-      <c r="W13" s="19">
+      <c r="AC13" s="19">
         <v>0.08</v>
       </c>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19">
+      <c r="AD13" s="19"/>
+      <c r="AE13" s="19"/>
+      <c r="AF13" s="19">
         <v>8.7900000000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>0.26700000000000002</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>0.51</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="28">
         <v>0.43159999999999998</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="17" t="s">
+      <c r="F14" s="28">
+        <v>0.45860000000000001</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0.49680000000000002</v>
+      </c>
+      <c r="H14" s="28">
+        <v>0.55630000000000002</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="20">
+      <c r="P14" s="20">
         <v>0.29330000000000001</v>
       </c>
-      <c r="K14" s="20">
+      <c r="Q14" s="20">
         <v>0.35299999999999998</v>
       </c>
-      <c r="L14" s="20">
+      <c r="R14" s="20">
         <v>0.38300000000000001</v>
       </c>
-      <c r="M14" s="20">
+      <c r="S14" s="20">
         <v>0.35299999999999998</v>
       </c>
-      <c r="N14" s="20">
+      <c r="T14" s="20">
         <v>0.379</v>
       </c>
-      <c r="O14" s="20">
+      <c r="U14" s="20">
         <v>0.38200000000000001</v>
       </c>
-      <c r="P14" s="19">
+      <c r="V14" s="19">
         <v>0.43</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="W14" s="20">
         <v>0.34699999999999998</v>
       </c>
-      <c r="R14" s="20">
+      <c r="X14" s="20">
         <v>0.42499999999999999</v>
       </c>
-      <c r="S14" s="20">
+      <c r="Y14" s="20">
         <v>0.36299999999999999</v>
       </c>
-      <c r="T14" s="19">
+      <c r="Z14" s="19">
         <v>0.42099999999999999</v>
       </c>
-      <c r="U14" s="19">
+      <c r="AA14" s="19">
         <v>0.44800000000000001</v>
       </c>
-      <c r="V14" s="19">
+      <c r="AB14" s="19">
         <v>0.45800000000000002</v>
       </c>
-      <c r="W14" s="19">
+      <c r="AC14" s="19">
         <v>0.46500000000000002</v>
       </c>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19">
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19">
         <v>0.46899999999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A15" s="32"/>
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>0.29799999999999999</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>0.499</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <v>0.41439999999999999</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="18" t="s">
+      <c r="F15" s="28">
+        <v>0.47860000000000003</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0.50919999999999999</v>
+      </c>
+      <c r="H15" s="28">
+        <v>0.55130000000000001</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="19">
+      <c r="P15" s="19">
         <v>0.28100000000000003</v>
       </c>
-      <c r="K15" s="19">
+      <c r="Q15" s="19">
         <v>0.35599999999999998</v>
       </c>
-      <c r="L15" s="19">
+      <c r="R15" s="19">
         <v>0.371</v>
       </c>
-      <c r="M15" s="19">
+      <c r="S15" s="19">
         <v>0.35599999999999998</v>
       </c>
-      <c r="N15" s="19">
+      <c r="T15" s="19">
         <v>0.374</v>
       </c>
-      <c r="O15" s="19">
+      <c r="U15" s="19">
         <v>0.38500000000000001</v>
       </c>
-      <c r="P15" s="19">
+      <c r="V15" s="19">
         <v>0.433</v>
       </c>
-      <c r="Q15" s="19">
+      <c r="W15" s="19">
         <v>0.34</v>
       </c>
-      <c r="R15" s="19">
+      <c r="X15" s="19">
         <v>0.44800000000000001</v>
       </c>
-      <c r="S15" s="19">
+      <c r="Y15" s="19">
         <v>0.34200000000000003</v>
       </c>
-      <c r="T15" s="19">
+      <c r="Z15" s="19">
         <v>0.433</v>
       </c>
-      <c r="U15" s="19">
+      <c r="AA15" s="19">
         <v>0.46</v>
       </c>
-      <c r="V15" s="19">
+      <c r="AB15" s="19">
         <v>0.45400000000000001</v>
       </c>
-      <c r="W15" s="19">
+      <c r="AC15" s="19">
         <v>0.46700000000000003</v>
       </c>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19">
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19">
         <v>0.45700000000000002</v>
       </c>
     </row>
@@ -7121,7 +8252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
@@ -8390,16 +9521,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A34:A45"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="D10:H10"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="A10:A21"/>
     <mergeCell ref="A22:A33"/>
     <mergeCell ref="D22:H22"/>
     <mergeCell ref="I22:M22"/>
-    <mergeCell ref="A34:A45"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="D10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added more performance data
</commit_message>
<xml_diff>
--- a/ModelPerformances.xlsx
+++ b/ModelPerformances.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="4220" windowWidth="21560" windowHeight="18280" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2760" yWindow="1720" windowWidth="26260" windowHeight="18280" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task 1 Question Retrieval" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="75">
   <si>
     <t>CNN</t>
   </si>
@@ -246,6 +246,15 @@
   <si>
     <t>LSTM model#</t>
   </si>
+  <si>
+    <t>bidir</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>2,3,4</t>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +350,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -360,7 +375,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -416,7 +431,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -426,6 +440,13 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -648,11 +669,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1916907568"/>
-        <c:axId val="-1862410688"/>
+        <c:axId val="-1407093744"/>
+        <c:axId val="-1407091264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1916907568"/>
+        <c:axId val="-1407093744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,7 +715,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1862410688"/>
+        <c:crossAx val="-1407091264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -702,7 +723,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1862410688"/>
+        <c:axId val="-1407091264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -752,7 +773,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1916907568"/>
+        <c:crossAx val="-1407093744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1025,11 +1046,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1862390544"/>
-        <c:axId val="-1917053376"/>
+        <c:axId val="-1407066288"/>
+        <c:axId val="-1407063536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1862390544"/>
+        <c:axId val="-1407066288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1071,7 +1092,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1917053376"/>
+        <c:crossAx val="-1407063536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1079,7 +1100,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1917053376"/>
+        <c:axId val="-1407063536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1099,6 +1120,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1129,7 +1151,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1862390544"/>
+        <c:crossAx val="-1407066288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2649,10 +2671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH96"/>
+  <dimension ref="A1:AH114"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="W57" workbookViewId="0">
-      <selection activeCell="AG73" sqref="AG73:AH73"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="AH93" sqref="AH93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2676,27 +2698,27 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="3"/>
       <c r="I3" s="5"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="31" t="s">
+      <c r="K3" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -4832,44 +4854,44 @@
       </c>
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="C65" s="31" t="s">
+      <c r="C65" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="31"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="31"/>
-      <c r="G65" s="31"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="33"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="33"/>
       <c r="H65" s="14"/>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
-      <c r="K65" s="31" t="s">
+      <c r="K65" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="L65" s="31"/>
-      <c r="M65" s="31"/>
-      <c r="N65" s="31"/>
-      <c r="O65" s="31"/>
-      <c r="P65" s="31"/>
-      <c r="Q65" s="31"/>
-      <c r="R65" s="31"/>
-      <c r="S65" s="31"/>
-      <c r="V65" s="31" t="s">
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+      <c r="N65" s="33"/>
+      <c r="O65" s="33"/>
+      <c r="P65" s="33"/>
+      <c r="Q65" s="33"/>
+      <c r="R65" s="33"/>
+      <c r="S65" s="33"/>
+      <c r="V65" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="W65" s="31"/>
-      <c r="X65" s="31"/>
-      <c r="Y65" s="31"/>
-      <c r="Z65" s="31"/>
-      <c r="AA65" s="31"/>
-      <c r="AB65" s="31"/>
-      <c r="AC65" s="31"/>
-      <c r="AD65" s="31"/>
+      <c r="W65" s="33"/>
+      <c r="X65" s="33"/>
+      <c r="Y65" s="33"/>
+      <c r="Z65" s="33"/>
+      <c r="AA65" s="33"/>
+      <c r="AB65" s="33"/>
+      <c r="AC65" s="33"/>
+      <c r="AD65" s="33"/>
       <c r="AE65" s="1"/>
       <c r="AF65" s="1"/>
-      <c r="AG65" s="31" t="s">
+      <c r="AG65" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="AH65" s="31"/>
+      <c r="AH65" s="33"/>
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -5027,11 +5049,11 @@
       <c r="S67" s="1">
         <v>0.433</v>
       </c>
-      <c r="T67" s="6">
+      <c r="T67" s="7">
         <f>HARMEAN(L67:O67)</f>
         <v>0.5341466465864888</v>
       </c>
-      <c r="U67" s="6">
+      <c r="U67" s="7">
         <f t="shared" ref="U67:U68" si="2">HARMEAN(P67:S67)</f>
         <v>0.55869760966365589</v>
       </c>
@@ -5434,11 +5456,11 @@
       <c r="S75" s="1">
         <v>0.438</v>
       </c>
-      <c r="T75" s="6">
+      <c r="T75" s="7">
         <f t="shared" ref="T75:T76" si="8">HARMEAN(L75:O75)</f>
         <v>0.52869598003963159</v>
       </c>
-      <c r="U75" s="6">
+      <c r="U75" s="7">
         <f t="shared" ref="U75:U76" si="9">HARMEAN(P75:S75)</f>
         <v>0.54836378195331514</v>
       </c>
@@ -5606,7 +5628,7 @@
       <c r="T80" s="24"/>
       <c r="U80" s="24"/>
     </row>
-    <row r="81" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L81" s="22"/>
       <c r="M81" s="22"/>
       <c r="N81" s="22"/>
@@ -5618,7 +5640,7 @@
       <c r="T81" s="22"/>
       <c r="U81" s="22"/>
     </row>
-    <row r="82" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C82">
         <v>1</v>
       </c>
@@ -5670,19 +5692,19 @@
       <c r="S82" s="22">
         <v>0.442</v>
       </c>
-      <c r="T82" s="25">
+      <c r="T82" s="24">
         <f t="shared" ref="T82:T83" si="12">HARMEAN(L82:O82)</f>
         <v>0.53666887107867123</v>
       </c>
-      <c r="U82" s="25">
+      <c r="U82" s="24">
         <f t="shared" ref="U82:U83" si="13">HARMEAN(P82:S82)</f>
         <v>0.56166848396011737</v>
       </c>
-      <c r="V82" s="26" t="s">
+      <c r="V82" s="25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B83">
         <v>5</v>
       </c>
@@ -5746,7 +5768,7 @@
         <v>0.56789353356629468</v>
       </c>
     </row>
-    <row r="84" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L84" s="22"/>
       <c r="M84" s="22"/>
       <c r="N84" s="22"/>
@@ -5758,7 +5780,7 @@
       <c r="T84" s="24"/>
       <c r="U84" s="24"/>
     </row>
-    <row r="85" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C85">
         <v>1</v>
       </c>
@@ -5807,19 +5829,19 @@
       <c r="S85" s="22">
         <v>0.42399999999999999</v>
       </c>
-      <c r="T85" s="27">
+      <c r="T85" s="24">
         <f t="shared" ref="T85:T86" si="14">HARMEAN(L85:O85)</f>
         <v>0.54458264504852938</v>
       </c>
-      <c r="U85" s="27">
+      <c r="U85" s="24">
         <f t="shared" ref="U85:U86" si="15">HARMEAN(P85:S85)</f>
         <v>0.53959294309558425</v>
       </c>
-      <c r="V85" s="26" t="s">
+      <c r="V85" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="86" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B86">
         <v>6</v>
       </c>
@@ -5903,22 +5925,22 @@
       <c r="AD86" s="22">
         <v>0.17899999999999999</v>
       </c>
-      <c r="AE86" s="27">
+      <c r="AE86" s="26">
         <f t="shared" ref="AE86" si="16">HARMEAN(W86:Z86)</f>
         <v>0.41625672942842756</v>
       </c>
-      <c r="AF86" s="27">
+      <c r="AF86" s="26">
         <f t="shared" ref="AF86" si="17">HARMEAN(AA86:AD86)</f>
         <v>0.40380252565986385</v>
       </c>
-      <c r="AG86" s="28">
+      <c r="AG86" s="27">
         <v>0.51</v>
       </c>
-      <c r="AH86" s="28">
+      <c r="AH86" s="27">
         <v>0.499</v>
       </c>
     </row>
-    <row r="87" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
       <c r="L87" s="22"/>
       <c r="M87" s="22"/>
       <c r="N87" s="22"/>
@@ -5930,7 +5952,7 @@
       <c r="T87" s="24"/>
       <c r="U87" s="24"/>
     </row>
-    <row r="88" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
       <c r="C88">
         <v>2</v>
       </c>
@@ -5991,7 +6013,7 @@
         <v>0.51937760196054394</v>
       </c>
     </row>
-    <row r="89" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
       <c r="B89">
         <v>7</v>
       </c>
@@ -6093,23 +6115,29 @@
         <v>0.41399999999999998</v>
       </c>
     </row>
-    <row r="90" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
       <c r="T90" s="7"/>
       <c r="U90" s="7"/>
     </row>
-    <row r="91" spans="2:34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>72</v>
+      </c>
       <c r="C91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D91">
         <v>240</v>
       </c>
       <c r="E91">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F91">
         <v>0.01</v>
       </c>
+      <c r="G91">
+        <v>8</v>
+      </c>
       <c r="H91">
         <v>20</v>
       </c>
@@ -6119,35 +6147,57 @@
       <c r="J91" t="s">
         <v>26</v>
       </c>
-      <c r="L91" s="22"/>
-      <c r="M91" s="22"/>
-      <c r="N91" s="22"/>
-      <c r="O91" s="22"/>
-      <c r="P91" s="22"/>
-      <c r="Q91" s="22"/>
-      <c r="R91" s="22"/>
-      <c r="S91" s="22"/>
-      <c r="T91" s="24" t="e">
+      <c r="K91" s="2">
+        <v>1.15E-3</v>
+      </c>
+      <c r="L91" s="22">
+        <v>0.57299999999999995</v>
+      </c>
+      <c r="M91" s="22">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="N91" s="22">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="O91" s="22">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="P91" s="22">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="Q91" s="22">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="R91" s="22">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S91" s="22">
+        <v>0.439</v>
+      </c>
+      <c r="T91" s="24">
         <f t="shared" ref="T91:T92" si="22">HARMEAN(L91:O91)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U91" s="24" t="e">
+        <v>0.56430390558359023</v>
+      </c>
+      <c r="U91" s="24">
         <f t="shared" ref="U91:U92" si="23">HARMEAN(P91:S91)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="92" spans="2:34" x14ac:dyDescent="0.2">
+        <v>0.5431625594807501</v>
+      </c>
+    </row>
+    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>72</v>
+      </c>
       <c r="B92">
         <v>8</v>
       </c>
       <c r="C92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D92">
         <v>240</v>
       </c>
       <c r="E92">
-        <v>2.9999999999999997E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="F92">
         <v>0.01</v>
@@ -6164,69 +6214,992 @@
       <c r="J92" t="s">
         <v>26</v>
       </c>
-      <c r="L92" s="22"/>
-      <c r="M92" s="22"/>
-      <c r="N92" s="22"/>
-      <c r="O92" s="22"/>
-      <c r="P92" s="22"/>
-      <c r="Q92" s="22"/>
-      <c r="R92" s="22"/>
-      <c r="S92" s="22"/>
-      <c r="T92" s="24" t="e">
+      <c r="K92" s="2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="L92" s="22">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="M92" s="22">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="N92" s="22">
+        <v>0.624</v>
+      </c>
+      <c r="O92" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="P92" s="22">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="Q92" s="22">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="R92" s="22">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="S92" s="22">
+        <v>0.44</v>
+      </c>
+      <c r="T92" s="32">
         <f t="shared" si="22"/>
+        <v>0.57773044238217408</v>
+      </c>
+      <c r="U92" s="32">
+        <f t="shared" si="23"/>
+        <v>0.54739550893922295</v>
+      </c>
+      <c r="W92" s="1">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="X92" s="1">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="Y92" s="1">
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="Z92" s="1">
+        <v>0.189</v>
+      </c>
+      <c r="AA92" s="1">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="AB92" s="1">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="AC92" s="1">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="AD92" s="1">
+        <v>0.185</v>
+      </c>
+      <c r="AE92" s="6">
+        <f t="shared" ref="AE92" si="24">HARMEAN(W92:Z92)</f>
+        <v>0.4257571213174961</v>
+      </c>
+      <c r="AF92" s="6">
+        <f t="shared" ref="AF92" si="25">HARMEAN(AA92:AD92)</f>
+        <v>0.42153062298529126</v>
+      </c>
+      <c r="AG92" s="23">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="AH92" s="23">
+        <v>0.55100000000000005</v>
+      </c>
+    </row>
+    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L93" s="22"/>
+      <c r="M93" s="22"/>
+      <c r="N93" s="22"/>
+      <c r="O93" s="22"/>
+      <c r="P93" s="22"/>
+      <c r="Q93" s="22"/>
+      <c r="R93" s="22"/>
+      <c r="S93" s="22"/>
+      <c r="T93" s="24"/>
+      <c r="U93" s="24"/>
+    </row>
+    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>72</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>240</v>
+      </c>
+      <c r="E94">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F94">
+        <v>0.01</v>
+      </c>
+      <c r="G94">
+        <v>9</v>
+      </c>
+      <c r="H94">
+        <v>20</v>
+      </c>
+      <c r="I94">
+        <v>300</v>
+      </c>
+      <c r="J94" t="s">
+        <v>26</v>
+      </c>
+      <c r="K94" s="2">
+        <v>1.48E-3</v>
+      </c>
+      <c r="L94" s="22">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="M94" s="22">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="N94" s="22">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="O94" s="22">
+        <v>0.443</v>
+      </c>
+      <c r="P94" s="22">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="Q94" s="22">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="R94" s="22">
+        <v>0.59699999999999998</v>
+      </c>
+      <c r="S94" s="22">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T94" s="24">
+        <f t="shared" ref="T94:T95" si="26">HARMEAN(L94:O94)</f>
+        <v>0.55753469811401624</v>
+      </c>
+      <c r="U94" s="24">
+        <f t="shared" ref="U94:U95" si="27">HARMEAN(P94:S94)</f>
+        <v>0.55737598191173199</v>
+      </c>
+      <c r="W94" s="1">
+        <v>0.754</v>
+      </c>
+      <c r="X94" s="1">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="Y94" s="1">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="Z94" s="1">
+        <v>0.186</v>
+      </c>
+      <c r="AA94" s="1">
+        <v>0.746</v>
+      </c>
+      <c r="AB94" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="AC94" s="1">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AD94" s="1">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="AE94" s="6">
+        <f t="shared" ref="AE94" si="28">HARMEAN(W94:Z94)</f>
+        <v>0.41888417502506126</v>
+      </c>
+      <c r="AF94" s="6">
+        <f t="shared" ref="AF94" si="29">HARMEAN(AA94:AD94)</f>
+        <v>0.40746607508208299</v>
+      </c>
+      <c r="AG94" s="23">
+        <v>0.497</v>
+      </c>
+      <c r="AH94" s="23">
+        <v>0.50900000000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>72</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>240</v>
+      </c>
+      <c r="E95">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F95">
+        <v>0.01</v>
+      </c>
+      <c r="G95">
+        <v>10</v>
+      </c>
+      <c r="H95">
+        <v>20</v>
+      </c>
+      <c r="I95">
+        <v>300</v>
+      </c>
+      <c r="J95" t="s">
+        <v>26</v>
+      </c>
+      <c r="K95" s="2">
+        <v>1.17E-3</v>
+      </c>
+      <c r="L95" s="22">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="M95" s="22">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="N95" s="22">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="O95" s="22">
+        <v>0.45</v>
+      </c>
+      <c r="P95" s="22">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="Q95" s="22">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="R95" s="22">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="S95" s="22">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="T95" s="24">
+        <f t="shared" si="26"/>
+        <v>0.561119591277767</v>
+      </c>
+      <c r="U95" s="24">
+        <f t="shared" si="27"/>
+        <v>0.55152226399181714</v>
+      </c>
+    </row>
+    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T96" s="7"/>
+      <c r="U96" s="7"/>
+    </row>
+    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>72</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>240</v>
+      </c>
+      <c r="E97">
+        <v>1E-3</v>
+      </c>
+      <c r="F97">
+        <v>0.01</v>
+      </c>
+      <c r="G97">
+        <v>8</v>
+      </c>
+      <c r="H97">
+        <v>20</v>
+      </c>
+      <c r="I97">
+        <v>300</v>
+      </c>
+      <c r="J97" t="s">
+        <v>27</v>
+      </c>
+      <c r="K97" s="2">
+        <v>1.56E-3</v>
+      </c>
+      <c r="L97" s="22">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="M97" s="22">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="N97" s="22">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="O97" s="22">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="P97" s="22">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="Q97" s="22">
+        <v>0.68</v>
+      </c>
+      <c r="R97" s="22">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S97" s="22">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="T97" s="24">
+        <f t="shared" ref="T97:T98" si="30">HARMEAN(L97:O97)</f>
+        <v>0.56947548393464664</v>
+      </c>
+      <c r="U97" s="24">
+        <f t="shared" ref="U97:U98" si="31">HARMEAN(P97:S97)</f>
+        <v>0.53028156876269039</v>
+      </c>
+    </row>
+    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>240</v>
+      </c>
+      <c r="E98">
+        <v>1E-3</v>
+      </c>
+      <c r="F98">
+        <v>0.01</v>
+      </c>
+      <c r="G98">
+        <v>10</v>
+      </c>
+      <c r="H98">
+        <v>20</v>
+      </c>
+      <c r="I98">
+        <v>300</v>
+      </c>
+      <c r="J98" t="s">
+        <v>27</v>
+      </c>
+      <c r="K98" s="2">
+        <v>1.07E-3</v>
+      </c>
+      <c r="L98" s="22">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="M98" s="22">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="N98" s="22">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="O98" s="22">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="P98" s="22">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="Q98" s="22">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="R98" s="22">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="S98" s="22">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="T98" s="24">
+        <f t="shared" si="30"/>
+        <v>0.56611714570412963</v>
+      </c>
+      <c r="U98" s="24">
+        <f t="shared" si="31"/>
+        <v>0.54491010137918205</v>
+      </c>
+      <c r="W98" s="1">
+        <v>0.74400000000000011</v>
+      </c>
+      <c r="X98" s="1">
+        <v>0.748</v>
+      </c>
+      <c r="Y98" s="1">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="Z98" s="1">
+        <v>0.187</v>
+      </c>
+      <c r="AA98" s="1">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="AB98" s="1">
+        <v>0.74400000000000011</v>
+      </c>
+      <c r="AC98" s="1">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="AD98" s="1">
+        <v>0.17800000000000002</v>
+      </c>
+      <c r="AE98" s="1">
+        <f t="shared" ref="AE98" si="32">HARMEAN(W98:Z98)</f>
+        <v>0.41608743594148978</v>
+      </c>
+      <c r="AF98" s="1">
+        <f t="shared" ref="AF98" si="33">HARMEAN(AA98:AD98)</f>
+        <v>0.40549912587160197</v>
+      </c>
+      <c r="AG98" s="23">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="AH98" s="23">
+        <v>0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>72</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>240</v>
+      </c>
+      <c r="E99">
+        <v>1E-3</v>
+      </c>
+      <c r="F99">
+        <v>0.01</v>
+      </c>
+      <c r="G99">
+        <v>15</v>
+      </c>
+      <c r="H99">
+        <v>20</v>
+      </c>
+      <c r="I99">
+        <v>300</v>
+      </c>
+      <c r="J99" t="s">
+        <v>27</v>
+      </c>
+      <c r="K99" s="2">
+        <v>3.6000000000000002E-4</v>
+      </c>
+      <c r="L99" s="22">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="M99" s="22">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="N99" s="22">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="O99" s="22">
+        <v>0.442</v>
+      </c>
+      <c r="P99" s="22">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="Q99" s="22">
+        <v>0.68200000000000005</v>
+      </c>
+      <c r="R99" s="22">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="S99" s="22">
+        <v>0.42</v>
+      </c>
+      <c r="T99" s="24">
+        <f t="shared" ref="T99" si="34">HARMEAN(L99:O99)</f>
+        <v>0.55568844615019009</v>
+      </c>
+      <c r="U99" s="24">
+        <f t="shared" ref="U99" si="35">HARMEAN(P99:S99)</f>
+        <v>0.53255096258067558</v>
+      </c>
+    </row>
+    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T100" s="7"/>
+      <c r="U100" s="7"/>
+    </row>
+    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>72</v>
+      </c>
+      <c r="B101">
+        <v>11</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>240</v>
+      </c>
+      <c r="E101">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F101">
+        <v>0.01</v>
+      </c>
+      <c r="G101">
+        <v>15</v>
+      </c>
+      <c r="H101">
+        <v>20</v>
+      </c>
+      <c r="I101">
+        <v>200</v>
+      </c>
+      <c r="J101" t="s">
+        <v>26</v>
+      </c>
+      <c r="L101" s="22"/>
+      <c r="M101" s="22"/>
+      <c r="N101" s="22"/>
+      <c r="O101" s="22"/>
+      <c r="P101" s="22"/>
+      <c r="Q101" s="22"/>
+      <c r="R101" s="22"/>
+      <c r="S101" s="22"/>
+      <c r="T101" s="24" t="e">
+        <f t="shared" ref="T101:T102" si="36">HARMEAN(L101:O101)</f>
         <v>#N/A</v>
       </c>
-      <c r="U92" s="24" t="e">
-        <f t="shared" si="23"/>
+      <c r="U101" s="24" t="e">
+        <f t="shared" ref="U101:U102" si="37">HARMEAN(P101:S101)</f>
         <v>#N/A</v>
       </c>
-    </row>
-    <row r="93" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="T93" s="7"/>
-      <c r="U93" s="7"/>
-    </row>
-    <row r="94" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="T94" s="7"/>
-      <c r="U94" s="7"/>
-    </row>
-    <row r="95" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="T95" s="7"/>
-      <c r="U95" s="7"/>
-    </row>
-    <row r="96" spans="2:34" x14ac:dyDescent="0.2">
-      <c r="B96" t="s">
+      <c r="V101" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>72</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>240</v>
+      </c>
+      <c r="E102">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F102">
+        <v>0.01</v>
+      </c>
+      <c r="G102">
+        <v>20</v>
+      </c>
+      <c r="H102">
+        <v>20</v>
+      </c>
+      <c r="I102">
+        <v>200</v>
+      </c>
+      <c r="J102" t="s">
+        <v>26</v>
+      </c>
+      <c r="L102" s="22"/>
+      <c r="M102" s="22"/>
+      <c r="N102" s="22"/>
+      <c r="O102" s="22"/>
+      <c r="P102" s="22"/>
+      <c r="Q102" s="22"/>
+      <c r="R102" s="22"/>
+      <c r="S102" s="22"/>
+      <c r="T102" s="24" t="e">
+        <f t="shared" si="36"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U102" s="24" t="e">
+        <f t="shared" si="37"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W102" s="22"/>
+      <c r="X102" s="22"/>
+      <c r="Y102" s="22"/>
+      <c r="Z102" s="22"/>
+      <c r="AA102" s="22"/>
+      <c r="AB102" s="22"/>
+      <c r="AC102" s="22"/>
+      <c r="AD102" s="22"/>
+      <c r="AE102" s="26"/>
+      <c r="AF102" s="26"/>
+      <c r="AG102" s="27"/>
+      <c r="AH102" s="27"/>
+    </row>
+    <row r="103" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L103" s="22"/>
+      <c r="M103" s="22"/>
+      <c r="N103" s="22"/>
+      <c r="O103" s="22"/>
+      <c r="P103" s="22"/>
+      <c r="Q103" s="22"/>
+      <c r="R103" s="22"/>
+      <c r="S103" s="22"/>
+      <c r="T103" s="24"/>
+      <c r="U103" s="24"/>
+    </row>
+    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>72</v>
+      </c>
+      <c r="B104">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>1</v>
+      </c>
+      <c r="D104">
+        <v>240</v>
+      </c>
+      <c r="E104">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F104">
+        <v>0.01</v>
+      </c>
+      <c r="G104">
+        <v>4</v>
+      </c>
+      <c r="H104">
+        <v>20</v>
+      </c>
+      <c r="I104">
+        <v>200</v>
+      </c>
+      <c r="J104" t="s">
+        <v>26</v>
+      </c>
+      <c r="L104" s="22"/>
+      <c r="M104" s="22"/>
+      <c r="N104" s="22"/>
+      <c r="O104" s="22"/>
+      <c r="P104" s="22"/>
+      <c r="Q104" s="22"/>
+      <c r="R104" s="22"/>
+      <c r="S104" s="22"/>
+      <c r="T104" s="24" t="e">
+        <f t="shared" ref="T104:T105" si="38">HARMEAN(L104:O104)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U104" s="24" t="e">
+        <f t="shared" ref="U104:U105" si="39">HARMEAN(P104:S104)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>72</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>240</v>
+      </c>
+      <c r="E105">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F105">
+        <v>0.01</v>
+      </c>
+      <c r="G105">
+        <v>5</v>
+      </c>
+      <c r="H105">
+        <v>20</v>
+      </c>
+      <c r="I105">
+        <v>200</v>
+      </c>
+      <c r="J105" t="s">
+        <v>26</v>
+      </c>
+      <c r="L105" s="22"/>
+      <c r="M105" s="22"/>
+      <c r="N105" s="22"/>
+      <c r="O105" s="22"/>
+      <c r="P105" s="22"/>
+      <c r="Q105" s="22"/>
+      <c r="R105" s="22"/>
+      <c r="S105" s="22"/>
+      <c r="T105" s="24" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U105" s="24" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
+      <c r="Y105" s="1"/>
+      <c r="Z105" s="1"/>
+      <c r="AA105" s="1"/>
+      <c r="AB105" s="1"/>
+      <c r="AC105" s="1"/>
+      <c r="AD105" s="1"/>
+      <c r="AE105" s="6"/>
+      <c r="AF105" s="6"/>
+      <c r="AG105" s="23"/>
+      <c r="AH105" s="23"/>
+    </row>
+    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T106" s="7"/>
+      <c r="U106" s="7"/>
+    </row>
+    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>72</v>
+      </c>
+      <c r="B107">
+        <v>13</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <v>240</v>
+      </c>
+      <c r="E107">
+        <v>1E-3</v>
+      </c>
+      <c r="F107">
+        <v>0.01</v>
+      </c>
+      <c r="G107">
+        <v>8</v>
+      </c>
+      <c r="H107">
+        <v>20</v>
+      </c>
+      <c r="I107">
+        <v>200</v>
+      </c>
+      <c r="J107" t="s">
+        <v>27</v>
+      </c>
+      <c r="L107" s="22"/>
+      <c r="M107" s="22"/>
+      <c r="N107" s="22"/>
+      <c r="O107" s="22"/>
+      <c r="P107" s="22"/>
+      <c r="Q107" s="22"/>
+      <c r="R107" s="22"/>
+      <c r="S107" s="22"/>
+      <c r="T107" s="24" t="e">
+        <f t="shared" ref="T107:T108" si="40">HARMEAN(L107:O107)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U107" s="24" t="e">
+        <f t="shared" ref="U107:U108" si="41">HARMEAN(P107:S107)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>72</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>240</v>
+      </c>
+      <c r="E108">
+        <v>1E-3</v>
+      </c>
+      <c r="F108">
+        <v>0.01</v>
+      </c>
+      <c r="G108">
+        <v>10</v>
+      </c>
+      <c r="H108">
+        <v>20</v>
+      </c>
+      <c r="I108">
+        <v>200</v>
+      </c>
+      <c r="J108" t="s">
+        <v>27</v>
+      </c>
+      <c r="L108" s="22"/>
+      <c r="M108" s="22"/>
+      <c r="N108" s="22"/>
+      <c r="O108" s="22"/>
+      <c r="P108" s="22"/>
+      <c r="Q108" s="22"/>
+      <c r="R108" s="22"/>
+      <c r="S108" s="22"/>
+      <c r="T108" s="32" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U108" s="32" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W108" s="22"/>
+      <c r="X108" s="22"/>
+      <c r="Y108" s="22"/>
+      <c r="Z108" s="22"/>
+      <c r="AA108" s="22"/>
+      <c r="AB108" s="22"/>
+      <c r="AC108" s="22"/>
+      <c r="AD108" s="22"/>
+      <c r="AE108" s="26"/>
+      <c r="AF108" s="26"/>
+      <c r="AG108" s="27"/>
+      <c r="AH108" s="27"/>
+    </row>
+    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="L109" s="22"/>
+      <c r="M109" s="22"/>
+      <c r="N109" s="22"/>
+      <c r="O109" s="22"/>
+      <c r="P109" s="22"/>
+      <c r="Q109" s="22"/>
+      <c r="R109" s="22"/>
+      <c r="S109" s="22"/>
+      <c r="T109" s="24"/>
+      <c r="U109" s="24"/>
+    </row>
+    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>72</v>
+      </c>
+      <c r="B110">
+        <v>14</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>240</v>
+      </c>
+      <c r="E110">
+        <v>1E-3</v>
+      </c>
+      <c r="F110">
+        <v>0.01</v>
+      </c>
+      <c r="H110">
+        <v>20</v>
+      </c>
+      <c r="I110">
+        <v>200</v>
+      </c>
+      <c r="J110" t="s">
+        <v>27</v>
+      </c>
+      <c r="L110" s="22"/>
+      <c r="M110" s="22"/>
+      <c r="N110" s="22"/>
+      <c r="O110" s="22"/>
+      <c r="P110" s="22"/>
+      <c r="Q110" s="22"/>
+      <c r="R110" s="22"/>
+      <c r="S110" s="22"/>
+      <c r="T110" s="24" t="e">
+        <f t="shared" ref="T110:T111" si="42">HARMEAN(L110:O110)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U110" s="24" t="e">
+        <f t="shared" ref="U110:U111" si="43">HARMEAN(P110:S110)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="111" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>72</v>
+      </c>
+      <c r="C111">
+        <v>1</v>
+      </c>
+      <c r="D111">
+        <v>240</v>
+      </c>
+      <c r="E111">
+        <v>1E-3</v>
+      </c>
+      <c r="F111">
+        <v>0.01</v>
+      </c>
+      <c r="G111">
+        <v>10</v>
+      </c>
+      <c r="H111">
+        <v>20</v>
+      </c>
+      <c r="I111">
+        <v>200</v>
+      </c>
+      <c r="J111" t="s">
+        <v>27</v>
+      </c>
+      <c r="L111" s="22"/>
+      <c r="M111" s="22"/>
+      <c r="N111" s="22"/>
+      <c r="O111" s="22"/>
+      <c r="P111" s="22"/>
+      <c r="Q111" s="22"/>
+      <c r="R111" s="22"/>
+      <c r="S111" s="22"/>
+      <c r="T111" s="24" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="U111" s="24" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="W111" s="1"/>
+      <c r="X111" s="1"/>
+      <c r="Y111" s="1"/>
+      <c r="Z111" s="1"/>
+      <c r="AA111" s="1"/>
+      <c r="AB111" s="1"/>
+      <c r="AC111" s="1"/>
+      <c r="AD111" s="1"/>
+      <c r="AE111" s="6"/>
+      <c r="AF111" s="6"/>
+      <c r="AG111" s="23"/>
+      <c r="AH111" s="23"/>
+    </row>
+    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="T112" s="7"/>
+      <c r="U112" s="7"/>
+    </row>
+    <row r="113" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="T113" s="7"/>
+      <c r="U113" s="7"/>
+    </row>
+    <row r="114" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B114" t="s">
         <v>23</v>
       </c>
-      <c r="L96" s="1">
+      <c r="L114" s="1">
         <v>0.58399999999999996</v>
       </c>
-      <c r="M96" s="1">
+      <c r="M114" s="1">
         <v>0.72299999999999998</v>
       </c>
-      <c r="N96" s="1">
+      <c r="N114" s="1">
         <v>0.6</v>
       </c>
-      <c r="O96" s="1">
+      <c r="O114" s="1">
         <v>0.46400000000000002</v>
       </c>
-      <c r="P96" s="1">
+      <c r="P114" s="1">
         <v>0.56799999999999995</v>
       </c>
-      <c r="Q96" s="1">
+      <c r="Q114" s="1">
         <v>0.70099999999999996</v>
       </c>
-      <c r="R96" s="1">
+      <c r="R114" s="1">
         <v>0.55800000000000005</v>
       </c>
-      <c r="S96" s="1">
+      <c r="S114" s="1">
         <v>0.432</v>
       </c>
-      <c r="T96" s="6">
-        <f t="shared" ref="T96" si="24">HARMEAN(L96:O96)</f>
+      <c r="T114" s="6">
+        <f t="shared" ref="T114" si="44">HARMEAN(L114:O114)</f>
         <v>0.57826082952638469</v>
       </c>
-      <c r="U96" s="6">
-        <f t="shared" ref="U96" si="25">HARMEAN(P96:S96)</f>
+      <c r="U114" s="6">
+        <f t="shared" ref="U114" si="45">HARMEAN(P114:S114)</f>
         <v>0.54839395595501261</v>
       </c>
     </row>
@@ -6245,20 +7218,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="10.83203125" style="15"/>
+    <col min="3" max="6" width="10.83203125" style="15"/>
+    <col min="7" max="12" width="10.83203125" style="30"/>
+    <col min="13" max="14" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>71</v>
       </c>
@@ -6271,12 +7246,25 @@
       <c r="E1" s="15">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="F1" s="15">
+        <v>10</v>
+      </c>
+      <c r="G1">
+        <v>9</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
@@ -6291,38 +7279,33 @@
       <c r="E2" s="15">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="O2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="21">
+      <c r="P2" s="21">
         <v>1E-3</v>
       </c>
-      <c r="K2" s="21">
+      <c r="Q2" s="21">
         <v>1E-3</v>
       </c>
-      <c r="L2" s="21">
+      <c r="R2" s="21">
         <v>1E-3</v>
       </c>
-      <c r="M2" s="21">
+      <c r="S2" s="21">
         <v>1E-3</v>
-      </c>
-      <c r="N2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="O2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="P2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="Q2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="R2" s="21">
-        <v>0.01</v>
-      </c>
-      <c r="S2" s="21">
-        <v>0.01</v>
       </c>
       <c r="T2" s="21">
         <v>0.01</v>
@@ -6345,9 +7328,39 @@
       <c r="Z2" s="21">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+      <c r="AA2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AB2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AC2" s="21">
+        <v>0.01</v>
+      </c>
+      <c r="AD2" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="AE2" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="AF2" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="AG2" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="AH2" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="AI2" s="31">
+        <v>0.01</v>
+      </c>
+      <c r="AJ2" s="31">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -6360,25 +7373,20 @@
       <c r="E3" s="15">
         <v>240</v>
       </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="21">
-        <v>2</v>
-      </c>
-      <c r="K3" s="21">
-        <v>2</v>
-      </c>
-      <c r="L3" s="21">
-        <v>2</v>
-      </c>
-      <c r="M3" s="21">
-        <v>3</v>
-      </c>
-      <c r="N3" s="21">
-        <v>2</v>
-      </c>
-      <c r="O3" s="21">
+      <c r="F3">
+        <v>240</v>
+      </c>
+      <c r="G3">
+        <v>240</v>
+      </c>
+      <c r="H3">
+        <v>240</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="O3" t="s">
         <v>3</v>
       </c>
       <c r="P3" s="21">
@@ -6391,13 +7399,13 @@
         <v>2</v>
       </c>
       <c r="S3" s="21">
-        <v>4</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>63</v>
+        <v>3</v>
+      </c>
+      <c r="T3" s="21">
+        <v>2</v>
       </c>
       <c r="U3" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V3" s="21">
         <v>2</v>
@@ -6409,14 +7417,44 @@
         <v>2</v>
       </c>
       <c r="Y3" s="21">
+        <v>4</v>
+      </c>
+      <c r="Z3" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA3" s="21">
         <v>2</v>
       </c>
-      <c r="Z3" s="21">
+      <c r="AB3" s="21">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
+      <c r="AC3" s="21">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="31">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="31">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG3" s="31">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="31">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ3" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -6429,26 +7467,21 @@
       <c r="E4" s="15">
         <v>2.9999999999999997E-4</v>
       </c>
-      <c r="I4" t="s">
+      <c r="F4">
+        <v>1E-3</v>
+      </c>
+      <c r="G4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H4">
+        <v>1E-3</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="O4" t="s">
         <v>5</v>
-      </c>
-      <c r="J4" s="21">
-        <v>200</v>
-      </c>
-      <c r="K4" s="21">
-        <v>200</v>
-      </c>
-      <c r="L4" s="21">
-        <v>200</v>
-      </c>
-      <c r="M4" s="21">
-        <v>200</v>
-      </c>
-      <c r="N4" s="21">
-        <v>200</v>
-      </c>
-      <c r="O4" s="21">
-        <v>200</v>
       </c>
       <c r="P4" s="21">
         <v>200</v>
@@ -6457,7 +7490,7 @@
         <v>200</v>
       </c>
       <c r="R4" s="21">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="S4" s="21">
         <v>200</v>
@@ -6469,23 +7502,53 @@
         <v>200</v>
       </c>
       <c r="V4" s="21">
+        <v>200</v>
+      </c>
+      <c r="W4" s="21">
+        <v>200</v>
+      </c>
+      <c r="X4" s="21">
         <v>100</v>
       </c>
-      <c r="W4" s="21">
+      <c r="Y4" s="21">
+        <v>200</v>
+      </c>
+      <c r="Z4" s="21">
+        <v>200</v>
+      </c>
+      <c r="AA4" s="21">
+        <v>200</v>
+      </c>
+      <c r="AB4" s="21">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="21">
         <v>400</v>
       </c>
-      <c r="X4" s="21">
+      <c r="AD4" s="31">
         <v>400</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="AE4" s="31">
         <v>300</v>
       </c>
-      <c r="Z4" s="21">
+      <c r="AF4" s="31">
+        <v>300</v>
+      </c>
+      <c r="AG4" s="31">
+        <v>300</v>
+      </c>
+      <c r="AH4" s="31">
         <v>600</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
+      <c r="AI4" s="31">
+        <v>300</v>
+      </c>
+      <c r="AJ4" s="31">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -6498,44 +7561,39 @@
       <c r="E5" s="15">
         <v>0.01</v>
       </c>
-      <c r="I5" t="s">
+      <c r="F5">
+        <v>0.01</v>
+      </c>
+      <c r="G5">
+        <v>0.01</v>
+      </c>
+      <c r="H5">
+        <v>0.01</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="O5" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="21">
+      <c r="P5" s="21">
         <v>1E-3</v>
       </c>
-      <c r="K5" s="21">
+      <c r="Q5" s="21">
         <v>0.01</v>
       </c>
-      <c r="L5" s="21">
+      <c r="R5" s="21">
         <v>0.01</v>
       </c>
-      <c r="M5" s="21">
+      <c r="S5" s="21">
         <v>0.01</v>
       </c>
-      <c r="N5" s="21">
+      <c r="T5" s="21">
         <v>0.01</v>
       </c>
-      <c r="O5" s="21">
+      <c r="U5" s="21">
         <v>0.01</v>
-      </c>
-      <c r="P5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="R5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="S5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="T5" s="21">
-        <v>0.1</v>
-      </c>
-      <c r="U5" s="21">
-        <v>0.1</v>
       </c>
       <c r="V5" s="21">
         <v>0.1</v>
@@ -6552,9 +7610,39 @@
       <c r="Z5" s="21">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
+      <c r="AA5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AB5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AC5" s="21">
+        <v>0.1</v>
+      </c>
+      <c r="AD5" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="AE5" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="AF5" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="AG5" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="AH5" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="AI5" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="AJ5" s="31">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -6567,57 +7655,82 @@
       <c r="E6" s="15">
         <v>5</v>
       </c>
-      <c r="I6" t="s">
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="O6" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="21">
+      <c r="P6" s="21">
         <v>8</v>
       </c>
-      <c r="K6" s="21">
+      <c r="Q6" s="21">
         <v>9</v>
       </c>
-      <c r="L6" s="21">
+      <c r="R6" s="21">
         <v>8</v>
       </c>
-      <c r="M6" s="21">
+      <c r="S6" s="21">
         <v>9</v>
       </c>
-      <c r="N6" s="21">
+      <c r="T6" s="21">
         <v>9</v>
       </c>
-      <c r="O6" s="21">
+      <c r="U6" s="21">
         <v>19</v>
       </c>
-      <c r="P6" s="21">
+      <c r="V6" s="21">
         <v>5</v>
       </c>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21">
+      <c r="W6" s="21"/>
+      <c r="X6" s="21">
         <v>5</v>
       </c>
-      <c r="S6" s="21">
+      <c r="Y6" s="21">
         <v>3</v>
       </c>
-      <c r="T6" s="21">
+      <c r="Z6" s="21">
         <v>7</v>
       </c>
-      <c r="U6" s="21">
+      <c r="AA6" s="21">
         <v>4</v>
       </c>
-      <c r="V6" s="21">
+      <c r="AB6" s="21">
         <v>4</v>
       </c>
-      <c r="W6" s="21">
+      <c r="AC6" s="21">
         <v>7</v>
       </c>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21">
+      <c r="AD6" s="31">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="31">
+        <v>4</v>
+      </c>
+      <c r="AF6" s="31">
+        <v>4</v>
+      </c>
+      <c r="AG6" s="31"/>
+      <c r="AH6" s="31">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
+      <c r="AI6" s="31">
+        <v>2</v>
+      </c>
+      <c r="AJ6" s="31"/>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -6630,32 +7743,27 @@
       <c r="E7" s="15">
         <v>10</v>
       </c>
-      <c r="I7" t="s">
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="O7" t="s">
         <v>56</v>
-      </c>
-      <c r="J7" s="21">
-        <v>20</v>
-      </c>
-      <c r="K7" s="21">
-        <v>20</v>
-      </c>
-      <c r="L7" s="21">
-        <v>20</v>
-      </c>
-      <c r="M7" s="21">
-        <v>20</v>
-      </c>
-      <c r="N7" s="21">
-        <v>20</v>
-      </c>
-      <c r="O7" s="21">
-        <v>20</v>
       </c>
       <c r="P7" s="21">
         <v>20</v>
       </c>
       <c r="Q7" s="21">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="R7" s="21">
         <v>20</v>
@@ -6673,20 +7781,50 @@
         <v>20</v>
       </c>
       <c r="W7" s="21">
+        <v>35</v>
+      </c>
+      <c r="X7" s="21">
         <v>20</v>
       </c>
-      <c r="X7" s="21">
-        <v>35</v>
-      </c>
       <c r="Y7" s="21">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="Z7" s="21">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
+      <c r="AA7" s="21">
+        <v>20</v>
+      </c>
+      <c r="AB7" s="21">
+        <v>20</v>
+      </c>
+      <c r="AC7" s="21">
+        <v>20</v>
+      </c>
+      <c r="AD7" s="31">
+        <v>35</v>
+      </c>
+      <c r="AE7" s="31">
+        <v>20</v>
+      </c>
+      <c r="AF7" s="31">
+        <v>20</v>
+      </c>
+      <c r="AG7" s="31">
+        <v>35</v>
+      </c>
+      <c r="AH7" s="31">
+        <v>20</v>
+      </c>
+      <c r="AI7" s="31">
+        <v>20</v>
+      </c>
+      <c r="AJ7" s="31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>28</v>
       </c>
@@ -6699,26 +7837,21 @@
       <c r="E8" s="15">
         <v>300</v>
       </c>
-      <c r="I8" t="s">
+      <c r="F8">
+        <v>300</v>
+      </c>
+      <c r="G8">
+        <v>300</v>
+      </c>
+      <c r="H8">
+        <v>300</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="O8" t="s">
         <v>28</v>
-      </c>
-      <c r="J8" s="21">
-        <v>300</v>
-      </c>
-      <c r="K8" s="21">
-        <v>300</v>
-      </c>
-      <c r="L8" s="21">
-        <v>300</v>
-      </c>
-      <c r="M8" s="21">
-        <v>300</v>
-      </c>
-      <c r="N8" s="21">
-        <v>300</v>
-      </c>
-      <c r="O8" s="21">
-        <v>300</v>
       </c>
       <c r="P8" s="21">
         <v>300</v>
@@ -6753,9 +7886,39 @@
       <c r="Z8" s="21">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
+      <c r="AA8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AB8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AC8" s="21">
+        <v>300</v>
+      </c>
+      <c r="AD8" s="31">
+        <v>300</v>
+      </c>
+      <c r="AE8" s="31">
+        <v>300</v>
+      </c>
+      <c r="AF8" s="31">
+        <v>300</v>
+      </c>
+      <c r="AG8" s="31">
+        <v>300</v>
+      </c>
+      <c r="AH8" s="31">
+        <v>300</v>
+      </c>
+      <c r="AI8" s="31">
+        <v>300</v>
+      </c>
+      <c r="AJ8" s="31">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
       <c r="B9" t="s">
         <v>24</v>
       </c>
@@ -6768,26 +7931,21 @@
       <c r="E9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="I9" t="s">
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="O9" t="s">
         <v>24</v>
-      </c>
-      <c r="J9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="M9" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="N9" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="O9" s="21" t="s">
-        <v>27</v>
       </c>
       <c r="P9" s="21" t="s">
         <v>27</v>
@@ -6796,314 +7954,444 @@
         <v>27</v>
       </c>
       <c r="R9" s="21" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="S9" s="21" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="T9" s="21" t="s">
         <v>27</v>
       </c>
       <c r="U9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="W9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="X9" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="V9" s="21" t="s">
+      <c r="AB9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="W9" s="21" t="s">
+      <c r="AC9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="X9" s="21" t="s">
+      <c r="AD9" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="Y9" s="21" t="s">
+      <c r="AE9" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="Z9" s="21" t="s">
+      <c r="AF9" s="31" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="AG9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="AH9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="AI9" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ9" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
       <c r="B11" s="1"/>
       <c r="C11" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="J11" t="s">
+      <c r="P11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28">
         <v>7.6100000000000001E-2</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17" t="s">
+      <c r="F12" s="28">
+        <v>9.0300000000000005E-2</v>
+      </c>
+      <c r="G12" s="28">
+        <v>0.1053</v>
+      </c>
+      <c r="H12" s="28">
+        <v>0.1042</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="20">
+      <c r="P12" s="20">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="K12" s="20">
+      <c r="Q12" s="20">
         <v>8.6800000000000002E-2</v>
       </c>
-      <c r="L12" s="20">
+      <c r="R12" s="20">
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="M12" s="20">
+      <c r="S12" s="20">
         <v>8.6699999999999999E-2</v>
       </c>
-      <c r="N12" s="20">
+      <c r="T12" s="20">
         <v>8.1299999999999997E-2</v>
       </c>
-      <c r="O12" s="20">
+      <c r="U12" s="20">
         <v>8.0699999999999994E-2</v>
       </c>
-      <c r="P12" s="19">
+      <c r="V12" s="19">
         <v>8.1100000000000005E-2</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="W12" s="20">
         <v>8.2799999999999999E-2</v>
       </c>
-      <c r="R12" s="20">
+      <c r="X12" s="20">
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="S12" s="20">
+      <c r="Y12" s="20">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="T12" s="19">
+      <c r="Z12" s="19">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="U12" s="19">
+      <c r="AA12" s="19">
         <v>0.10100000000000001</v>
       </c>
-      <c r="V12" s="19">
+      <c r="AB12" s="19">
         <v>7.8E-2</v>
       </c>
-      <c r="W12" s="19">
+      <c r="AC12" s="19">
         <v>9.01E-2</v>
       </c>
-      <c r="X12" s="19"/>
-      <c r="Y12" s="19"/>
-      <c r="Z12" s="19">
+      <c r="AD12" s="19">
+        <v>9.35E-2</v>
+      </c>
+      <c r="AE12" s="19">
+        <v>0.106</v>
+      </c>
+      <c r="AF12" s="19">
+        <v>9.5399999999999999E-2</v>
+      </c>
+      <c r="AG12" s="19">
+        <v>9.7900000000000001E-2</v>
+      </c>
+      <c r="AH12" s="19">
         <v>9.1499999999999998E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
+      <c r="AI12" s="19">
+        <v>9.1200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A13" s="34"/>
       <c r="B13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28">
         <v>8.7599999999999997E-2</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="18" t="s">
+      <c r="F13" s="28">
+        <v>9.11E-2</v>
+      </c>
+      <c r="G13" s="28">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="H13" s="28">
+        <v>9.9599999999999994E-2</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J13" s="19">
+      <c r="P13" s="19">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="K13" s="19">
+      <c r="Q13" s="19">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="L13" s="19">
+      <c r="R13" s="19">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="M13" s="19">
+      <c r="S13" s="19">
         <v>6.83E-2</v>
       </c>
-      <c r="N13" s="19">
+      <c r="T13" s="19">
         <v>7.1199999999999999E-2</v>
       </c>
-      <c r="O13" s="19">
+      <c r="U13" s="19">
         <v>7.4200000000000002E-2</v>
       </c>
-      <c r="P13" s="19">
+      <c r="V13" s="19">
         <v>7.5300000000000006E-2</v>
       </c>
-      <c r="Q13" s="19">
+      <c r="W13" s="19">
         <v>7.4700000000000003E-2</v>
       </c>
-      <c r="R13" s="19">
+      <c r="X13" s="19">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="S13" s="19">
+      <c r="Y13" s="19">
         <v>6.08E-2</v>
       </c>
-      <c r="T13" s="19">
+      <c r="Z13" s="19">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="U13" s="19">
+      <c r="AA13" s="19">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="V13" s="19">
+      <c r="AB13" s="19">
         <v>8.3699999999999997E-2</v>
       </c>
-      <c r="W13" s="19">
+      <c r="AC13" s="19">
         <v>0.08</v>
       </c>
-      <c r="X13" s="19"/>
-      <c r="Y13" s="19"/>
-      <c r="Z13" s="19">
+      <c r="AD13" s="19">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="AE13" s="19">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AF13" s="19">
+        <v>6.8400000000000002E-2</v>
+      </c>
+      <c r="AG13" s="19">
+        <v>8.14E-2</v>
+      </c>
+      <c r="AH13" s="19">
         <v>8.7900000000000006E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
+      <c r="AI13" s="19">
+        <v>7.5600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A14" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C14" s="28">
         <v>0.26700000000000002</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="28">
         <v>0.51</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E14" s="28">
         <v>0.43159999999999998</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="17" t="s">
+      <c r="F14" s="28">
+        <v>0.45860000000000001</v>
+      </c>
+      <c r="G14" s="28">
+        <v>0.49680000000000002</v>
+      </c>
+      <c r="H14" s="28">
+        <v>0.55630000000000002</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="20">
+      <c r="P14" s="20">
         <v>0.29330000000000001</v>
       </c>
-      <c r="K14" s="20">
+      <c r="Q14" s="20">
         <v>0.35299999999999998</v>
       </c>
-      <c r="L14" s="20">
+      <c r="R14" s="20">
         <v>0.38300000000000001</v>
       </c>
-      <c r="M14" s="20">
+      <c r="S14" s="20">
         <v>0.35299999999999998</v>
       </c>
-      <c r="N14" s="20">
+      <c r="T14" s="20">
         <v>0.379</v>
       </c>
-      <c r="O14" s="20">
+      <c r="U14" s="20">
         <v>0.38200000000000001</v>
       </c>
-      <c r="P14" s="19">
+      <c r="V14" s="19">
         <v>0.43</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="W14" s="20">
         <v>0.34699999999999998</v>
       </c>
-      <c r="R14" s="20">
+      <c r="X14" s="20">
         <v>0.42499999999999999</v>
       </c>
-      <c r="S14" s="20">
+      <c r="Y14" s="20">
         <v>0.36299999999999999</v>
       </c>
-      <c r="T14" s="19">
+      <c r="Z14" s="19">
         <v>0.42099999999999999</v>
       </c>
-      <c r="U14" s="19">
+      <c r="AA14" s="19">
         <v>0.44800000000000001</v>
       </c>
-      <c r="V14" s="19">
+      <c r="AB14" s="19">
         <v>0.45800000000000002</v>
       </c>
-      <c r="W14" s="19">
+      <c r="AC14" s="19">
         <v>0.46500000000000002</v>
       </c>
-      <c r="X14" s="19"/>
-      <c r="Y14" s="19"/>
-      <c r="Z14" s="19">
+      <c r="AD14" s="19">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="AE14" s="19">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="AF14" s="19">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="AG14" s="19">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="AH14" s="19">
         <v>0.46899999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="AI14" s="19">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A15" s="34"/>
       <c r="B15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="28">
         <v>0.29799999999999999</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="28">
         <v>0.499</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E15" s="28">
         <v>0.41439999999999999</v>
       </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="18" t="s">
+      <c r="F15" s="28">
+        <v>0.47860000000000003</v>
+      </c>
+      <c r="G15" s="28">
+        <v>0.50919999999999999</v>
+      </c>
+      <c r="H15" s="28">
+        <v>0.55130000000000001</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="J15" s="19">
+      <c r="P15" s="19">
         <v>0.28100000000000003</v>
       </c>
-      <c r="K15" s="19">
+      <c r="Q15" s="19">
         <v>0.35599999999999998</v>
       </c>
-      <c r="L15" s="19">
+      <c r="R15" s="19">
         <v>0.371</v>
       </c>
-      <c r="M15" s="19">
+      <c r="S15" s="19">
         <v>0.35599999999999998</v>
       </c>
-      <c r="N15" s="19">
+      <c r="T15" s="19">
         <v>0.374</v>
       </c>
-      <c r="O15" s="19">
+      <c r="U15" s="19">
         <v>0.38500000000000001</v>
       </c>
-      <c r="P15" s="19">
+      <c r="V15" s="19">
         <v>0.433</v>
       </c>
-      <c r="Q15" s="19">
+      <c r="W15" s="19">
         <v>0.34</v>
       </c>
-      <c r="R15" s="19">
+      <c r="X15" s="19">
         <v>0.44800000000000001</v>
       </c>
-      <c r="S15" s="19">
+      <c r="Y15" s="19">
         <v>0.34200000000000003</v>
       </c>
-      <c r="T15" s="19">
+      <c r="Z15" s="19">
         <v>0.433</v>
       </c>
-      <c r="U15" s="19">
+      <c r="AA15" s="19">
         <v>0.46</v>
       </c>
-      <c r="V15" s="19">
+      <c r="AB15" s="19">
         <v>0.45400000000000001</v>
       </c>
-      <c r="W15" s="19">
+      <c r="AC15" s="19">
         <v>0.46700000000000003</v>
       </c>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19">
+      <c r="AD15" s="19">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="AE15" s="19">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="AF15" s="19">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="AG15" s="19">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="AH15" s="19">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="AI15" s="19">
         <v>0.45700000000000002</v>
       </c>
     </row>
@@ -7121,7 +8409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
@@ -7139,7 +8427,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
@@ -7150,7 +8438,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
+      <c r="A3" s="34"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -7159,7 +8447,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
+      <c r="A4" s="34"/>
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -7168,7 +8456,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
+      <c r="A5" s="34"/>
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -7177,7 +8465,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
+      <c r="A6" s="34"/>
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -7186,7 +8474,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
+      <c r="A7" s="34"/>
       <c r="B7" t="s">
         <v>28</v>
       </c>
@@ -7195,7 +8483,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
+      <c r="A8" s="34"/>
       <c r="B8" t="s">
         <v>24</v>
       </c>
@@ -7207,30 +8495,30 @@
       <c r="C9" s="11"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="34" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33" t="s">
+      <c r="E10" s="35"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="35"/>
+      <c r="M10" s="35"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="1"/>
       <c r="C11" s="11" t="s">
         <v>52</v>
@@ -7267,7 +8555,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
@@ -7308,7 +8596,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
@@ -7349,7 +8637,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="1" t="s">
         <v>43</v>
       </c>
@@ -7390,7 +8678,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="1" t="s">
         <v>44</v>
       </c>
@@ -7431,7 +8719,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
@@ -7472,7 +8760,7 @@
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>46</v>
       </c>
@@ -7513,7 +8801,7 @@
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
+      <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
@@ -7554,7 +8842,7 @@
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="32"/>
+      <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
@@ -7595,7 +8883,7 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>49</v>
       </c>
@@ -7636,7 +8924,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
+      <c r="A21" s="34"/>
       <c r="B21" s="1" t="s">
         <v>50</v>
       </c>
@@ -7677,27 +8965,27 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="34" t="s">
         <v>33</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33" t="s">
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="1"/>
       <c r="D23" s="9" t="s">
         <v>35</v>
@@ -7731,7 +9019,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="32"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
@@ -7769,7 +9057,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="32"/>
+      <c r="A25" s="34"/>
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
@@ -7807,7 +9095,7 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
+      <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>43</v>
       </c>
@@ -7845,7 +9133,7 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
+      <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>44</v>
       </c>
@@ -7883,7 +9171,7 @@
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="32"/>
+      <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>45</v>
       </c>
@@ -7921,7 +9209,7 @@
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
+      <c r="A29" s="34"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
@@ -7959,7 +9247,7 @@
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="32"/>
+      <c r="A30" s="34"/>
       <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
@@ -7997,7 +9285,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="32"/>
+      <c r="A31" s="34"/>
       <c r="B31" s="1" t="s">
         <v>48</v>
       </c>
@@ -8035,7 +9323,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="32"/>
+      <c r="A32" s="34"/>
       <c r="B32" s="1" t="s">
         <v>49</v>
       </c>
@@ -8073,7 +9361,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="32"/>
+      <c r="A33" s="34"/>
       <c r="B33" s="1" t="s">
         <v>50</v>
       </c>
@@ -8111,23 +9399,23 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="32" t="s">
+      <c r="C34" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="32"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="32" t="s">
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="32"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="1"/>
       <c r="C35" s="10" t="s">
         <v>53</v>
@@ -8149,7 +9437,7 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="32"/>
+      <c r="A36" s="34"/>
       <c r="B36" s="1" t="s">
         <v>41</v>
       </c>
@@ -8173,7 +9461,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="32"/>
+      <c r="A37" s="34"/>
       <c r="B37" s="1" t="s">
         <v>42</v>
       </c>
@@ -8197,7 +9485,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A38" s="32"/>
+      <c r="A38" s="34"/>
       <c r="B38" s="1" t="s">
         <v>43</v>
       </c>
@@ -8221,7 +9509,7 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A39" s="32"/>
+      <c r="A39" s="34"/>
       <c r="B39" s="1" t="s">
         <v>44</v>
       </c>
@@ -8245,7 +9533,7 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A40" s="32"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
@@ -8269,7 +9557,7 @@
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A41" s="32"/>
+      <c r="A41" s="34"/>
       <c r="B41" s="1" t="s">
         <v>46</v>
       </c>
@@ -8293,7 +9581,7 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A42" s="32"/>
+      <c r="A42" s="34"/>
       <c r="B42" s="1" t="s">
         <v>47</v>
       </c>
@@ -8317,7 +9605,7 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43" s="32"/>
+      <c r="A43" s="34"/>
       <c r="B43" s="1" t="s">
         <v>48</v>
       </c>
@@ -8341,7 +9629,7 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44" s="32"/>
+      <c r="A44" s="34"/>
       <c r="B44" s="1" t="s">
         <v>49</v>
       </c>
@@ -8365,7 +9653,7 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45" s="32"/>
+      <c r="A45" s="34"/>
       <c r="B45" s="1" t="s">
         <v>50</v>
       </c>

</xml_diff>